<commit_message>
Update latest output (run 5)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,42 +475,22 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46037.16666666666</v>
+        <v>46037</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>46037.66666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>45.36</v>
+        <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>1043.48709075</v>
+        <v>1632.584050499999</v>
       </c>
       <c r="F2" t="n">
-        <v>23.00456549272488</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>46037.83333333334</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>46038</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E3" t="n">
-        <v>709.8202994999998</v>
-      </c>
-      <c r="F3" t="n">
-        <v>46.94578700396824</v>
+        <v>26.99378390376983</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,7 +541,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46037.02083333334</v>
+        <v>46037</v>
       </c>
       <c r="B2" t="n">
         <v>78</v>
@@ -576,16 +556,16 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46037.04166666666</v>
+        <v>46037.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>78</v>
+        <v>76.66624</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -597,20 +577,20 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46037.0625</v>
+        <v>46037.04166666666</v>
       </c>
       <c r="B4" t="n">
         <v>78</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
@@ -618,20 +598,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46037.08333333334</v>
+        <v>46037.0625</v>
       </c>
       <c r="B5" t="n">
-        <v>78</v>
+        <v>82.35556</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
@@ -639,20 +619,20 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46037.10416666666</v>
+        <v>46037.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>74.34273</v>
+        <v>78</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
@@ -660,16 +640,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46037.125</v>
+        <v>46037.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>73.35939</v>
+        <v>76.64994</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -681,16 +661,16 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46037.14583333334</v>
+        <v>46037.125</v>
       </c>
       <c r="B8" t="n">
-        <v>65.84793999999999</v>
+        <v>73.59164</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -702,16 +682,16 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46037.16666666666</v>
+        <v>46037.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>64.78918</v>
+        <v>72.6703</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -729,10 +709,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46037.1875</v>
+        <v>46037.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>60.83516</v>
+        <v>64.37671</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -750,10 +730,10 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46037.20833333334</v>
+        <v>46037.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>64.23663999999999</v>
+        <v>61.34927</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -771,10 +751,10 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46037.22916666666</v>
+        <v>46037.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>84.7901</v>
+        <v>63.83266</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -792,10 +772,10 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46037.25</v>
+        <v>46037.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>80.28617</v>
+        <v>84.7901</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -813,10 +793,10 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46037.27083333334</v>
+        <v>46037.25</v>
       </c>
       <c r="B14" t="n">
-        <v>78.74827000000001</v>
+        <v>80.06771000000001</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -834,10 +814,10 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46037.29166666666</v>
+        <v>46037.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>56.98</v>
+        <v>78.25467999999999</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -855,10 +835,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46037.3125</v>
+        <v>46037.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>51.38425</v>
+        <v>52.16133</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -876,10 +856,10 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46037.33333333334</v>
+        <v>46037.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>49.76664</v>
+        <v>51.07513</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -897,10 +877,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46037.35416666666</v>
+        <v>46037.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>36.06</v>
+        <v>49.7656</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -918,10 +898,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46037.375</v>
+        <v>46037.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>42.1703</v>
+        <v>36.06</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -939,10 +919,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46037.39583333334</v>
+        <v>46037.375</v>
       </c>
       <c r="B20" t="n">
-        <v>8.037800000000001</v>
+        <v>41.92585</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -960,10 +940,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46037.41666666666</v>
+        <v>46037.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>0.51</v>
+        <v>10.52921</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -981,10 +961,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46037.4375</v>
+        <v>46037.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>26.37936</v>
+        <v>11.75013</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1002,10 +982,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46037.45833333334</v>
+        <v>46037.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>5.29955</v>
+        <v>36.06</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1023,7 +1003,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46037.47916666666</v>
+        <v>46037.45833333334</v>
       </c>
       <c r="B24" t="n">
         <v>0.51</v>
@@ -1044,10 +1024,10 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46037.5</v>
+        <v>46037.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>36.06</v>
+        <v>2.83675</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1065,10 +1045,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46037.52083333334</v>
+        <v>46037.5</v>
       </c>
       <c r="B26" t="n">
-        <v>36.0601</v>
+        <v>36.06</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1086,10 +1066,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>46037.54166666666</v>
+        <v>46037.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>26.82405</v>
+        <v>36.0601</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1107,10 +1087,10 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>46037.5625</v>
+        <v>46037.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>36.0601</v>
+        <v>0.51</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1128,10 +1108,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>46037.58333333334</v>
+        <v>46037.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>52.10755</v>
+        <v>36.0601</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1149,10 +1129,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>46037.60416666666</v>
+        <v>46037.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>56.98</v>
+        <v>52.11471</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1170,10 +1150,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>46037.625</v>
+        <v>46037.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>58.38795</v>
+        <v>56.98</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1191,10 +1171,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>46037.64583333334</v>
+        <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>56.98</v>
+        <v>58.40146</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1212,10 +1192,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>46037.66666666666</v>
+        <v>46037.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>44.16666</v>
+        <v>56.98</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1227,16 +1207,16 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>46037.6875</v>
+        <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>53.07603</v>
+        <v>47.42517</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1254,10 +1234,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>46037.70833333334</v>
+        <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>59.47781</v>
+        <v>53.07603</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1275,10 +1255,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>46037.72916666666</v>
+        <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>28.43649</v>
+        <v>57.6972</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1296,10 +1276,10 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>46037.75</v>
+        <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>62.71437</v>
+        <v>21.07294</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1317,10 +1297,10 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>46037.77083333334</v>
+        <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>80.02</v>
+        <v>61.49051</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1338,10 +1318,10 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>46037.79166666666</v>
+        <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>101.76767</v>
+        <v>70.66426</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1359,10 +1339,10 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>46037.8125</v>
+        <v>46037.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>139.06772</v>
+        <v>101.77225</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1380,10 +1360,10 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>46037.83333333334</v>
+        <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>158.99</v>
+        <v>132.06252</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1395,16 +1375,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>46037.85416666666</v>
+        <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>120.01</v>
+        <v>158.99</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1416,16 +1396,16 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>46037.875</v>
+        <v>46037.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>85.95</v>
+        <v>120.01</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1437,16 +1417,16 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>46037.89583333334</v>
+        <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>78.00005</v>
+        <v>85.95</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1458,16 +1438,16 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>46037.91666666666</v>
+        <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>78.00005</v>
+        <v>77.14255</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1479,16 +1459,16 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>46037.9375</v>
+        <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.09</v>
+        <v>78.00005</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1500,16 +1480,16 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46037.95833333334</v>
+        <v>46037.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>71.98072000000001</v>
+        <v>64.99985</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1521,28 +1501,49 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
+        <v>46037.95833333334</v>
+      </c>
+      <c r="B48" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>46037</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
         <v>46037.97916666666</v>
       </c>
-      <c r="B48" t="n">
-        <v>78</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>forecast</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="n">
-        <v>46037</v>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>ON</t>
+      <c r="B49" t="n">
+        <v>72.27782999999999</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>46037</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update latest output (run 7)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>1674.97327725</v>
+        <v>1718.68822125</v>
       </c>
       <c r="F2" t="n">
-        <v>27.69466397569445</v>
+        <v>28.41746397569445</v>
       </c>
     </row>
   </sheetData>
@@ -649,7 +649,7 @@
         <v>46037.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>67.98876</v>
+        <v>78</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -670,7 +670,7 @@
         <v>46037.125</v>
       </c>
       <c r="B8" t="n">
-        <v>68.04342</v>
+        <v>78</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -691,11 +691,11 @@
         <v>46037.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>67.2062</v>
+        <v>67.27928</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
@@ -712,11 +712,11 @@
         <v>46037.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>66.36573</v>
+        <v>65.84793999999999</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
@@ -733,7 +733,7 @@
         <v>46037.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>61.70593</v>
+        <v>61.54031</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         <v>46037.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>63.8185</v>
+        <v>62.8085</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
         <v>46037.25</v>
       </c>
       <c r="B14" t="n">
-        <v>80.06771000000001</v>
+        <v>80.02</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         <v>46037.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>78.71372</v>
+        <v>78.33004</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>46037.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>56.98</v>
+        <v>52.33926</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>46037.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>51.37223</v>
+        <v>51.39572</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46037.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>50.05842</v>
+        <v>50.07721</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46037.375</v>
       </c>
       <c r="B20" t="n">
-        <v>41.92894</v>
+        <v>42.1835</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46037.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>19.05581</v>
+        <v>19.39377</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46037.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>0.51</v>
+        <v>25.87642</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>46037.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>34.01</v>
+        <v>36.06</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46037.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>27.65305</v>
+        <v>22.07</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46037.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>12.09885</v>
+        <v>23.65517</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46037.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>52.11742</v>
+        <v>52.11771</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46037.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>59.44001</v>
+        <v>59.75743</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>62.04007</v>
+        <v>59.25835</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>47.4258</v>
+        <v>47.57833</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>53.14823</v>
+        <v>61.7683</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>61.98752</v>
+        <v>62.02801</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>24.39195</v>
+        <v>28.59972</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>33.74417</v>
+        <v>57.09237</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>80.02</v>
+        <v>73.69302</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46037.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>158.99</v>
+        <v>135.68796</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>198.74561</v>
+        <v>165.37731</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>158.99</v>
+        <v>167.77584</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46037.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>66.44042</v>
+        <v>63.56007</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>59.81397</v>
+        <v>59.821</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 8)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>1718.68822125</v>
+        <v>1610.531286</v>
       </c>
       <c r="F2" t="n">
-        <v>28.41746397569445</v>
+        <v>26.62915486111111</v>
       </c>
     </row>
   </sheetData>
@@ -691,7 +691,7 @@
         <v>46037.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>67.27928</v>
+        <v>73.78127000000001</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
         <v>46037.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>65.84793999999999</v>
+        <v>73.1985</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -733,11 +733,11 @@
         <v>46037.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>61.54031</v>
+        <v>56.98</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
@@ -754,11 +754,11 @@
         <v>46037.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>62.8085</v>
+        <v>62.2571</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
@@ -775,7 +775,7 @@
         <v>46037.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>84.7901</v>
+        <v>80.93711999999999</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
         <v>46037.25</v>
       </c>
       <c r="B14" t="n">
-        <v>80.02</v>
+        <v>79.88200999999999</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         <v>46037.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>78.33004</v>
+        <v>63.65493</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>46037.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>52.33926</v>
+        <v>50.14936</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>46037.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>51.39572</v>
+        <v>49.96245</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46037.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>50.07721</v>
+        <v>44.39991</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46037.375</v>
       </c>
       <c r="B20" t="n">
-        <v>42.1835</v>
+        <v>36.06</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46037.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>19.39377</v>
+        <v>0.009379999999999999</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46037.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>25.87642</v>
+        <v>-0.3133</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>46037.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>36.06</v>
+        <v>36.07</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46037.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>22.07</v>
+        <v>0.51</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46037.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>22.07</v>
+        <v>34.01</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46037.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>23.65517</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46037.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>52.11771</v>
+        <v>53.10611</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46037.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>59.75743</v>
+        <v>56.98</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>59.25835</v>
+        <v>58.81093</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46037.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>56.98</v>
+        <v>52.47475</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>47.57833</v>
+        <v>56.33086</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>61.7683</v>
+        <v>61.21598</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>62.02801</v>
+        <v>64.01355</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>28.59972</v>
+        <v>37.60586</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>57.09237</v>
+        <v>57.00873</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>73.69302</v>
+        <v>80.02</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46037.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>135.68796</v>
+        <v>120.01</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>165.37731</v>
+        <v>158.99</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>167.77584</v>
+        <v>159.6199</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46037.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>120.01</v>
+        <v>111.89625</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>75.21648</v>
+        <v>85.95</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>65.0001</v>
+        <v>78.00005</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>65</v>
+        <v>105.79</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46037.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>65</v>
+        <v>64.99985</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46037.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>63.56007</v>
+        <v>57.73363</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>59.821</v>
+        <v>59.4713</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 9)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>1610.531286</v>
+        <v>1534.7215845</v>
       </c>
       <c r="F2" t="n">
-        <v>26.62915486111111</v>
+        <v>25.37568757440476</v>
       </c>
     </row>
   </sheetData>
@@ -733,7 +733,7 @@
         <v>46037.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>56.98</v>
+        <v>65.15832</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         <v>46037.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>62.2571</v>
+        <v>81.07834</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -775,11 +775,11 @@
         <v>46037.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>80.93711999999999</v>
+        <v>79.35364</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
@@ -796,11 +796,11 @@
         <v>46037.25</v>
       </c>
       <c r="B14" t="n">
-        <v>79.88200999999999</v>
+        <v>80.02</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
@@ -817,7 +817,7 @@
         <v>46037.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>63.65493</v>
+        <v>63.99078</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>46037.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>50.14936</v>
+        <v>36.07</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>46037.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>49.96245</v>
+        <v>36.07</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46037.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>44.39991</v>
+        <v>36.06</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46037.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>36.06</v>
+        <v>26.42341</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46037.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>0.009379999999999999</v>
+        <v>0.51</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46037.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.3133</v>
+        <v>0.51</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>46037.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>36.07</v>
+        <v>5.21834</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46037.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>34.01</v>
+        <v>0.51</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46037.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46037.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>53.10611</v>
+        <v>53.42659</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>58.81093</v>
+        <v>58.80779</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46037.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>52.47475</v>
+        <v>56.98</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>56.33086</v>
+        <v>56.69206</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>61.21598</v>
+        <v>61.2163</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>64.01355</v>
+        <v>66.20182</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>37.60586</v>
+        <v>32.55525</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>57.00873</v>
+        <v>52.09869</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>80.02</v>
+        <v>73.69302</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>158.99</v>
+        <v>120.01</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>159.6199</v>
+        <v>158.99</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46037.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>111.89625</v>
+        <v>120.01</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>85.95</v>
+        <v>105.79</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>78.00005</v>
+        <v>105.79</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>105.79</v>
+        <v>120.01</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46037.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>64.99985</v>
+        <v>69.11084</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46037.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.73363</v>
+        <v>58.17358</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>59.4713</v>
+        <v>60.55376</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 13)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>1414.76449725</v>
+        <v>1686.649185</v>
       </c>
       <c r="F2" t="n">
-        <v>23.3922701264881</v>
+        <v>27.88771800595238</v>
       </c>
     </row>
   </sheetData>
@@ -943,11 +943,11 @@
         <v>46037.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>0.08382000000000001</v>
+        <v>48.97284</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
@@ -964,11 +964,11 @@
         <v>46037.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>0.02167</v>
+        <v>36.06</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
@@ -985,7 +985,7 @@
         <v>46037.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>22.07</v>
+        <v>36.06</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46037.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.0001</v>
+        <v>34.01</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46037.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-2.52488</v>
+        <v>36.06</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46037.5</v>
       </c>
       <c r="B26" t="n">
-        <v>0.51</v>
+        <v>36.06</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46037.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-4.66156</v>
+        <v>11.92153</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46037.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-5.50985</v>
+        <v>0.51</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46037.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>0.51</v>
+        <v>49.7961</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>36.0601</v>
+        <v>36.01246</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46037.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>36.0601</v>
+        <v>36.01246</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>40.61245</v>
+        <v>40.69742</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>44.01368</v>
+        <v>41.04596</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>47.46912</v>
+        <v>54.74532</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>19.05091</v>
+        <v>25.11183</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>49.58561</v>
+        <v>55.11546</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>70.46706</v>
+        <v>72.95139</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>120.01</v>
+        <v>158.99</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>140.37518</v>
+        <v>158.99</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>105.79004</v>
+        <v>105.79</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>105.79</v>
+        <v>85.95</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>85.95</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46037.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>65.31265</v>
+        <v>64.99985</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46037.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>67.74731</v>
+        <v>70.27191000000001</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>74.51801</v>
+        <v>60.18313</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 14)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>1686.649185</v>
+        <v>1739.1522525</v>
       </c>
       <c r="F2" t="n">
-        <v>27.88771800595238</v>
+        <v>28.75582428075397</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +943,7 @@
         <v>46037.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>48.97284</v>
+        <v>8.18614</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46037.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>36.06</v>
+        <v>10.3824</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -989,7 +989,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
@@ -1006,11 +1006,11 @@
         <v>46037.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>34.01</v>
+        <v>0.51</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
@@ -1048,11 +1048,11 @@
         <v>46037.5</v>
       </c>
       <c r="B26" t="n">
-        <v>36.06</v>
+        <v>55.43646</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
@@ -1069,7 +1069,7 @@
         <v>46037.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>0.51</v>
+        <v>51.22117</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46037.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>11.92153</v>
+        <v>36.06009</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46037.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>0.51</v>
+        <v>36.0601</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46037.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>49.7961</v>
+        <v>44.79373</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46037.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>36.0601</v>
+        <v>56.98</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>36.01246</v>
+        <v>39.93588</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46037.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>36.01246</v>
+        <v>40.20882</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>40.69742</v>
+        <v>43.87656</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>41.04596</v>
+        <v>44.10049</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>54.74532</v>
+        <v>49.23158</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>25.11183</v>
+        <v>23.49459</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>55.11546</v>
+        <v>66.7022</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>72.95139</v>
+        <v>63.34815</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46037.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>120.01</v>
+        <v>106.89055</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>158.99</v>
+        <v>120.01</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>158.99</v>
+        <v>125.00189</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46037.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>120.01</v>
+        <v>101.25</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>105.79</v>
+        <v>85.08304</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>85.95</v>
+        <v>80.02</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>71.40000000000001</v>
+        <v>69.09674</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46037.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>64.99985</v>
+        <v>57.09</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46037.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>70.27191000000001</v>
+        <v>57.09</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>60.18313</v>
+        <v>57.09</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 15)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,19 +478,79 @@
         <v>46037</v>
       </c>
       <c r="B2" s="2" t="n">
+        <v>46037.20833333334</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="E2" t="n">
+        <v>737.8842217499999</v>
+      </c>
+      <c r="F2" t="n">
+        <v>39.04149321428572</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>46037.29166666666</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>46037.66666666666</v>
       </c>
-      <c r="C2" t="n">
-        <v>16</v>
-      </c>
-      <c r="D2" t="n">
-        <v>60.48</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1739.1522525</v>
-      </c>
-      <c r="F2" t="n">
-        <v>28.75582428075397</v>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>34.02</v>
+      </c>
+      <c r="E3" t="n">
+        <v>583.4340525</v>
+      </c>
+      <c r="F3" t="n">
+        <v>17.14973699294533</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>46037.91666666666</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>46038.125</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>532.4608867500001</v>
+      </c>
+      <c r="F4" t="n">
+        <v>28.1725336904762</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>46038.29166666666</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>46038.66666666666</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>34.02</v>
+      </c>
+      <c r="E5" t="n">
+        <v>483.8738970000001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>14.22321860670194</v>
       </c>
     </row>
   </sheetData>
@@ -504,7 +564,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,7 +826,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -787,7 +847,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -808,7 +868,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -829,7 +889,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1087,7 @@
         <v>46037.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>36.06</v>
+        <v>0.51</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1108,7 @@
         <v>46037.5</v>
       </c>
       <c r="B26" t="n">
-        <v>55.43646</v>
+        <v>34.01</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,11 +1129,11 @@
         <v>46037.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>51.22117</v>
+        <v>36.0601</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
@@ -1090,11 +1150,11 @@
         <v>46037.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>36.06009</v>
+        <v>0.51</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D28" s="3" t="n">
@@ -1111,11 +1171,11 @@
         <v>46037.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>36.0601</v>
+        <v>39.0601</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
@@ -1132,11 +1192,11 @@
         <v>46037.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>44.79373</v>
+        <v>52.32496</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D30" s="3" t="n">
@@ -1153,7 +1213,7 @@
         <v>46037.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>56.98</v>
+        <v>57.08</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1234,7 @@
         <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>39.93588</v>
+        <v>36.07</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1255,7 @@
         <v>46037.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>40.20882</v>
+        <v>56.98</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1276,7 @@
         <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>43.87656</v>
+        <v>44.01769</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1297,7 @@
         <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>44.10049</v>
+        <v>49.15376</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1318,7 @@
         <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>49.23158</v>
+        <v>54.3948</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1339,7 @@
         <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>23.49459</v>
+        <v>18.54764</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1360,7 @@
         <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>66.7022</v>
+        <v>55.11462</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1381,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>63.34815</v>
+        <v>70.47145</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1402,7 @@
         <v>46037.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>106.89055</v>
+        <v>120.01</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1384,7 +1444,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>125.00189</v>
+        <v>120.01</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1426,7 +1486,7 @@
         <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>85.08304</v>
+        <v>85.95</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1507,7 @@
         <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>80.02</v>
+        <v>83.95355000000001</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1528,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>69.09674</v>
+        <v>69.09249</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1480,7 +1540,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1561,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1582,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1591,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>57.09</v>
+        <v>57.41519</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1542,6 +1602,1014 @@
         <v>46037</v>
       </c>
       <c r="E49" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>46038</v>
+      </c>
+      <c r="B50" t="n">
+        <v>57.06008</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>46038.02083333334</v>
+      </c>
+      <c r="B51" t="n">
+        <v>57.06003</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>46038.04166666666</v>
+      </c>
+      <c r="B52" t="n">
+        <v>56.98</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>46038.0625</v>
+      </c>
+      <c r="B53" t="n">
+        <v>49.66065</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>46038.08333333334</v>
+      </c>
+      <c r="B54" t="n">
+        <v>48.59529</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>46038.10416666666</v>
+      </c>
+      <c r="B55" t="n">
+        <v>36.07</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>46038.125</v>
+      </c>
+      <c r="B56" t="n">
+        <v>36.07</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>46038.14583333334</v>
+      </c>
+      <c r="B57" t="n">
+        <v>42.26032</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>46038.16666666666</v>
+      </c>
+      <c r="B58" t="n">
+        <v>55.39499</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>46038.1875</v>
+      </c>
+      <c r="B59" t="n">
+        <v>57.05991</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>46038.20833333334</v>
+      </c>
+      <c r="B60" t="n">
+        <v>57.06003</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>46038.22916666666</v>
+      </c>
+      <c r="B61" t="n">
+        <v>60.57749</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>46038.25</v>
+      </c>
+      <c r="B62" t="n">
+        <v>57.07828</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>46038.27083333334</v>
+      </c>
+      <c r="B63" t="n">
+        <v>56.98</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>46038.29166666666</v>
+      </c>
+      <c r="B64" t="n">
+        <v>36.05972</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>46038.3125</v>
+      </c>
+      <c r="B65" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>46038.33333333334</v>
+      </c>
+      <c r="B66" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>46038.35416666666</v>
+      </c>
+      <c r="B67" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>46038.375</v>
+      </c>
+      <c r="B68" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>46038.39583333334</v>
+      </c>
+      <c r="B69" t="n">
+        <v>22.62945</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>46038.41666666666</v>
+      </c>
+      <c r="B70" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>46038.4375</v>
+      </c>
+      <c r="B71" t="n">
+        <v>36.07</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>46038.45833333334</v>
+      </c>
+      <c r="B72" t="n">
+        <v>36.05949</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>46038.47916666666</v>
+      </c>
+      <c r="B73" t="n">
+        <v>36.05989</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D73" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>46038.5</v>
+      </c>
+      <c r="B74" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>46038.52083333334</v>
+      </c>
+      <c r="B75" t="n">
+        <v>36.0601</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>46038.54166666666</v>
+      </c>
+      <c r="B76" t="n">
+        <v>36.0601</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D76" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>46038.5625</v>
+      </c>
+      <c r="B77" t="n">
+        <v>22.07</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>46038.58333333334</v>
+      </c>
+      <c r="B78" t="n">
+        <v>-7.01</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D78" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>46038.60416666666</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-2.47963</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D79" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>46038.625</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.57069</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>46038.64583333334</v>
+      </c>
+      <c r="B81" t="n">
+        <v>27.77111</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>46038.66666666666</v>
+      </c>
+      <c r="B82" t="n">
+        <v>27.7711</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D82" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>46038.6875</v>
+      </c>
+      <c r="B83" t="n">
+        <v>21.4936</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>46038.70833333334</v>
+      </c>
+      <c r="B84" t="n">
+        <v>43.24919</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>46038.72916666666</v>
+      </c>
+      <c r="B85" t="n">
+        <v>37.83416</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>46038.75</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.48373</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>46038.77083333334</v>
+      </c>
+      <c r="B87" t="n">
+        <v>53.90481</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D87" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>46038.79166666666</v>
+      </c>
+      <c r="B88" t="n">
+        <v>299.98</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>46038.8125</v>
+      </c>
+      <c r="B89" t="n">
+        <v>299.98</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>46038.83333333334</v>
+      </c>
+      <c r="B90" t="n">
+        <v>67.39879999999999</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D90" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>46038.85416666666</v>
+      </c>
+      <c r="B91" t="n">
+        <v>49.23153</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>46038.875</v>
+      </c>
+      <c r="B92" t="n">
+        <v>40.98924</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>46038.89583333334</v>
+      </c>
+      <c r="B93" t="n">
+        <v>40.5543</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>46038.91666666666</v>
+      </c>
+      <c r="B94" t="n">
+        <v>40.56485</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>46038.9375</v>
+      </c>
+      <c r="B95" t="n">
+        <v>48.38127</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>46038.95833333334</v>
+      </c>
+      <c r="B96" t="n">
+        <v>47.88557</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D96" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>46038.97916666666</v>
+      </c>
+      <c r="B97" t="n">
+        <v>40.46757</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E97" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>

</xml_diff>

<commit_message>
Update latest output (run 17)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -507,10 +507,10 @@
         <v>34.02</v>
       </c>
       <c r="E3" t="n">
-        <v>563.1449849999999</v>
+        <v>583.6327769999999</v>
       </c>
       <c r="F3" t="n">
-        <v>16.55335052910053</v>
+        <v>17.15557839506173</v>
       </c>
     </row>
     <row r="4">
@@ -518,39 +518,39 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46038.10416666666</v>
+        <v>46038.125</v>
       </c>
       <c r="C4" t="n">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>17.01</v>
+        <v>18.9</v>
       </c>
       <c r="E4" t="n">
-        <v>513.38060475</v>
+        <v>543.31524975</v>
       </c>
       <c r="F4" t="n">
-        <v>30.18110551146385</v>
+        <v>28.74683861111112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46038.27083333334</v>
+        <v>46038.29166666666</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>46038.66666666666</v>
       </c>
       <c r="C5" t="n">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>35.91</v>
+        <v>34.02</v>
       </c>
       <c r="E5" t="n">
-        <v>601.14417675</v>
+        <v>583.0842810000001</v>
       </c>
       <c r="F5" t="n">
-        <v>16.74030010442774</v>
+        <v>17.13945564373898</v>
       </c>
     </row>
   </sheetData>
@@ -1213,7 +1213,7 @@
         <v>46037.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>39.7501</v>
+        <v>52.15699</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1234,7 +1234,7 @@
         <v>46037.625</v>
       </c>
       <c r="B32" t="n">
-        <v>36.0601</v>
+        <v>58.73807</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1255,7 +1255,7 @@
         <v>46037.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>57.04293</v>
+        <v>42.97119</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1276,11 +1276,11 @@
         <v>46037.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>43.94456</v>
+        <v>43.22303</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D34" s="3" t="n">
@@ -1297,7 +1297,7 @@
         <v>46037.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>46.29749</v>
+        <v>43.7905</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
         <v>46037.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>56.00261</v>
+        <v>55.05363</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         <v>46037.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>24.10105</v>
+        <v>17.535</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1360,7 +1360,7 @@
         <v>46037.75</v>
       </c>
       <c r="B38" t="n">
-        <v>66.66182000000001</v>
+        <v>57.89137</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>70.09057</v>
+        <v>62.83836</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         <v>46037.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>100.58579</v>
+        <v>80.02</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>106.42876</v>
+        <v>120.01</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>102.84099</v>
+        <v>129.81998</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         <v>46037.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>106.59</v>
+        <v>120.01</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>102.96758</v>
+        <v>90.2877</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>67.89254</v>
+        <v>68.2715</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>58.43705</v>
+        <v>58.42568</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         <v>46038.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>57.92459</v>
+        <v>57.88079</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46038.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.06003</v>
+        <v>59.1159</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
         <v>46038.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>56.98</v>
+        <v>36.07</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         <v>46038.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>57.06003</v>
+        <v>49.23254</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1729,7 +1729,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
         <v>46038.125</v>
       </c>
       <c r="B56" t="n">
-        <v>56.98</v>
+        <v>36.07</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
         <v>46038.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>56.88071</v>
+        <v>36.07</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1780,7 @@
         <v>46038.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>57.96129</v>
+        <v>56.98</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46038.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>59.63457</v>
+        <v>61.77255</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46038.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>60.43567</v>
+        <v>62.9539</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46038.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>65</v>
+        <v>73.20005</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46038.25</v>
       </c>
       <c r="B62" t="n">
-        <v>58.27761</v>
+        <v>60.8552</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>46038.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1906,7 +1906,7 @@
         <v>46038.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>35.88</v>
+        <v>36.06</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
         <v>46038.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>36.06</v>
+        <v>36.05989</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46038.375</v>
       </c>
       <c r="B68" t="n">
-        <v>40.9658</v>
+        <v>45.42611</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>36.06</v>
+        <v>45.51652</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46038.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>40.7954</v>
+        <v>36.05922</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>36.06028</v>
+        <v>36.05989</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46038.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>27.4532</v>
+        <v>36.05952</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46038.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>12.10384</v>
+        <v>36.0601</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46038.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>7.36827</v>
+        <v>8.562340000000001</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46038.625</v>
       </c>
       <c r="B80" t="n">
-        <v>4.71079</v>
+        <v>12.68053</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>29.70035</v>
+        <v>17.07084</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>29.66805</v>
+        <v>17.87116</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>24.42634</v>
+        <v>0.34135</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>18.11114</v>
+        <v>-9.3123</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>16.09187</v>
+        <v>-9.55317</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46038.75</v>
       </c>
       <c r="B86" t="n">
-        <v>5.45427</v>
+        <v>-6</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>40.36512</v>
+        <v>-5.99309</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>55.3303</v>
+        <v>-3.0714</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2431,7 +2431,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>67.39879999999999</v>
+        <v>32.40461</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>59.37278</v>
+        <v>32.40461</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>67.39879999999999</v>
+        <v>32.40461</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46038.875</v>
       </c>
       <c r="B92" t="n">
-        <v>68.21745</v>
+        <v>32.40461</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>57.04922</v>
+        <v>78</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>56.98078</v>
+        <v>64.8901</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>48.38244</v>
+        <v>57.09</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>51.55592</v>
+        <v>57.09</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
         <v>46038.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>57.02639</v>
+        <v>57.06003</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 21)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -527,10 +527,10 @@
         <v>17.01</v>
       </c>
       <c r="E4" t="n">
-        <v>495.6750825</v>
+        <v>497.91622725</v>
       </c>
       <c r="F4" t="n">
-        <v>29.14021649029982</v>
+        <v>29.27197103174603</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +547,10 @@
         <v>34.02</v>
       </c>
       <c r="E5" t="n">
-        <v>417.760239</v>
+        <v>627.4465957500001</v>
       </c>
       <c r="F5" t="n">
-        <v>12.27984241622575</v>
+        <v>18.44346254409172</v>
       </c>
     </row>
   </sheetData>
@@ -1381,7 +1381,7 @@
         <v>46037.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>35.88</v>
+        <v>70.48375</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         <v>46037.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>36.0601</v>
+        <v>101.47343</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
@@ -1444,11 +1444,11 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>85.95</v>
+        <v>57.09</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
@@ -1465,7 +1465,7 @@
         <v>46037.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>85.95</v>
+        <v>80.02</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46037.875</v>
       </c>
       <c r="B44" t="n">
-        <v>85.95</v>
+        <v>80.02</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>80.02</v>
+        <v>85.95</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46038</v>
       </c>
       <c r="B50" t="n">
-        <v>58.17198</v>
+        <v>58.22268</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         <v>46038.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>58.21072</v>
+        <v>58.41034</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46038.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.06003</v>
+        <v>57.88255</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
         <v>46038.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>50.04197</v>
+        <v>56.98</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
         <v>46038.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>56.98</v>
+        <v>51.26774</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
         <v>46038.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>51.17561</v>
+        <v>56.98</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1780,7 @@
         <v>46038.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>50.87011</v>
+        <v>56.98</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46038.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>64.56525000000001</v>
+        <v>64.94638999999999</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46038.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>64.45856000000001</v>
+        <v>65</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46038.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>75.84058</v>
+        <v>76.28136000000001</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46038.25</v>
       </c>
       <c r="B62" t="n">
-        <v>65</v>
+        <v>70.28973999999999</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         <v>46038.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>36.06</v>
+        <v>36.07</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
         <v>46038.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>41.60172</v>
+        <v>36.05989</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>36.06</v>
+        <v>41.72921</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46038.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>36.06</v>
+        <v>46.61275</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>36.05949</v>
+        <v>36.06028</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46038.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>36.06</v>
+        <v>39.065</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46038.5</v>
       </c>
       <c r="B74" t="n">
-        <v>6.4549</v>
+        <v>36.06</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>0.51</v>
+        <v>47.65777</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46038.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-3.6481</v>
+        <v>28.81204</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46038.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-4.81333</v>
+        <v>36.0601</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46038.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>6.79107</v>
+        <v>36.05857</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46038.625</v>
       </c>
       <c r="B80" t="n">
-        <v>4.96539</v>
+        <v>16.83806</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>16.0108</v>
+        <v>26.1512</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>17.3123</v>
+        <v>15.65567</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>8.53261</v>
+        <v>6.48108</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-11.45546</v>
+        <v>5.98882</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-10.83089</v>
+        <v>-9.555009999999999</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46038.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-6.88049</v>
+        <v>-6.88159</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>-6</v>
+        <v>-3.07461</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>-3.09313</v>
+        <v>-3.07143</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>78</v>
+        <v>64.8901</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>64.8901</v>
+        <v>57.09</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 22)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -475,82 +475,82 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46037</v>
+        <v>46037.02083333334</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>46037.20833333334</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D2" t="n">
-        <v>18.9</v>
+        <v>17.01</v>
       </c>
       <c r="E2" t="n">
-        <v>737.8842217499999</v>
+        <v>661.83422175</v>
       </c>
       <c r="F2" t="n">
-        <v>39.04149321428572</v>
+        <v>38.90853743386243</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46037.27083333334</v>
+        <v>46037.29166666666</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>46037.66666666666</v>
       </c>
       <c r="C3" t="n">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
-        <v>35.91</v>
+        <v>34.02</v>
       </c>
       <c r="E3" t="n">
-        <v>674.410308</v>
+        <v>597.29136675</v>
       </c>
       <c r="F3" t="n">
-        <v>18.78057109440267</v>
+        <v>17.55706545414462</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46037.9375</v>
+        <v>46037.89583333334</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46038.125</v>
+        <v>46038.16666666666</v>
       </c>
       <c r="C4" t="n">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="D4" t="n">
-        <v>17.01</v>
+        <v>24.57</v>
       </c>
       <c r="E4" t="n">
-        <v>497.91622725</v>
+        <v>718.032588</v>
       </c>
       <c r="F4" t="n">
-        <v>29.27197103174603</v>
+        <v>29.22395555555556</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46038.29166666666</v>
+        <v>46038.33333333334</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>46038.66666666666</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>34.02</v>
+        <v>30.24</v>
       </c>
       <c r="E5" t="n">
-        <v>627.4465957500001</v>
+        <v>540.6628304999999</v>
       </c>
       <c r="F5" t="n">
-        <v>18.44346254409172</v>
+        <v>17.87906185515873</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +616,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -889,7 +889,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
         <v>46037.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>80.02</v>
+        <v>124.79767</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46037.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>57.09</v>
+        <v>142.36</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1490,7 +1490,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1507,7 +1507,7 @@
         <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>80.02</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1528,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>85.95</v>
+        <v>84.50611000000001</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
         <v>46037.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>56.98</v>
+        <v>74.11642999999999</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.98</v>
+        <v>57.79891</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46038</v>
       </c>
       <c r="B50" t="n">
-        <v>58.22268</v>
+        <v>56.98</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         <v>46038.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>58.41034</v>
+        <v>58.95402</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46038.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.88255</v>
+        <v>58.95394</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
         <v>46038.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>56.98</v>
+        <v>58.16581</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
         <v>46038.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>51.26774</v>
+        <v>36.07</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         <v>46038.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>56.98</v>
+        <v>50.37846</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1738,7 +1738,7 @@
         <v>46038.125</v>
       </c>
       <c r="B56" t="n">
-        <v>56.98</v>
+        <v>36.07</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
         <v>46038.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>56.98</v>
+        <v>36.07</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1801,7 +1801,7 @@
         <v>46038.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>64.94638999999999</v>
+        <v>64.93029</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46038.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>76.28136000000001</v>
+        <v>76.26062</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46038.25</v>
       </c>
       <c r="B62" t="n">
-        <v>70.28973999999999</v>
+        <v>71.95462000000001</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>46038.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>36.06</v>
+        <v>40.54</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
         <v>46038.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>36.07</v>
+        <v>41.26969</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
         <v>46038.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>36.05989</v>
+        <v>48.26714</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
         <v>46038.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>36.06</v>
+        <v>42.04025</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>41.72921</v>
+        <v>36.06</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46038.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>46.61275</v>
+        <v>36.06</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>36.06028</v>
+        <v>23.10045</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46038.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>39.065</v>
+        <v>36.06</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>47.65777</v>
+        <v>36.0601</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46038.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>28.81204</v>
+        <v>36.0601</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46038.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>36.05857</v>
+        <v>32.5543</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46038.625</v>
       </c>
       <c r="B80" t="n">
-        <v>16.83806</v>
+        <v>27.01543</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>26.1512</v>
+        <v>20.94801</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>15.65567</v>
+        <v>38.44817</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>6.48108</v>
+        <v>8.271470000000001</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>5.98882</v>
+        <v>11.08967</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-9.555009999999999</v>
+        <v>-8.068099999999999</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46038.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-6.88159</v>
+        <v>-6.78305</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>-3.07461</v>
+        <v>-3.99001</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>-3.07143</v>
+        <v>-3.07171</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2431,7 +2431,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>29.85322</v>
+        <v>22.01959</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>32.40461</v>
+        <v>29.85322</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46038.875</v>
       </c>
       <c r="B92" t="n">
-        <v>29.85322</v>
+        <v>30.1875</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>64.8901</v>
+        <v>78</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>57.09</v>
+        <v>64.8901</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>57.09</v>
+        <v>57.04922</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 24)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,50 +475,50 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46037.04166666666</v>
+        <v>46037</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46037.20833333334</v>
+        <v>46037.66666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>15.12</v>
+        <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>587.08463775</v>
+        <v>1670.962254</v>
       </c>
       <c r="F2" t="n">
-        <v>38.82834905753968</v>
+        <v>27.62834414682539</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46037.29166666666</v>
+        <v>46038.33333333334</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46037.66666666666</v>
+        <v>46038.66666666666</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>34.02</v>
+        <v>30.24</v>
       </c>
       <c r="E3" t="n">
-        <v>597.29136675</v>
+        <v>620.6932777500001</v>
       </c>
       <c r="F3" t="n">
-        <v>17.55706545414462</v>
+        <v>20.52557135416667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46037.875</v>
+        <v>46038.83333333334</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46038.04166666666</v>
+        <v>46039</v>
       </c>
       <c r="C4" t="n">
         <v>4</v>
@@ -527,50 +527,10 @@
         <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>590.1241807499999</v>
+        <v>331.7085135</v>
       </c>
       <c r="F4" t="n">
-        <v>39.02937703373016</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>46038.375</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>46038.66666666666</v>
-      </c>
-      <c r="C5" t="n">
-        <v>7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>26.46</v>
-      </c>
-      <c r="E5" t="n">
-        <v>468.1814669999999</v>
-      </c>
-      <c r="F5" t="n">
-        <v>17.69393299319728</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>46038.83333333334</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>46039</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E6" t="n">
-        <v>400.345803</v>
-      </c>
-      <c r="F6" t="n">
-        <v>26.47789702380953</v>
+        <v>21.93839375</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +596,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -657,7 +617,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -846,7 +806,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -867,7 +827,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -888,7 +848,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -909,7 +869,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1518,7 +1478,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1487,7 @@
         <v>46037.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>80.02</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1539,7 +1499,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1548,7 +1508,7 @@
         <v>46037.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>85.95</v>
+        <v>65.0001</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1560,7 +1520,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1569,11 +1529,11 @@
         <v>46037.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>71.40000000000001</v>
+        <v>65</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
@@ -1581,7 +1541,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1590,11 +1550,11 @@
         <v>46037.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>65</v>
+        <v>85.95</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
@@ -1602,7 +1562,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1611,11 +1571,11 @@
         <v>46037.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>73.93557</v>
+        <v>84.7901</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D49" s="3" t="n">
@@ -1623,7 +1583,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1632,7 +1592,7 @@
         <v>46038</v>
       </c>
       <c r="B50" t="n">
-        <v>65</v>
+        <v>81.05549000000001</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1644,7 +1604,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1625,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1634,7 @@
         <v>46038.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>58.69504</v>
+        <v>78</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1695,7 +1655,7 @@
         <v>46038.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>58.45285</v>
+        <v>78</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1716,7 +1676,7 @@
         <v>46038.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>59.60656</v>
+        <v>78</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1737,7 +1697,7 @@
         <v>46038.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>64.89</v>
+        <v>69.42238</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1758,7 +1718,7 @@
         <v>46038.125</v>
       </c>
       <c r="B56" t="n">
-        <v>64.89</v>
+        <v>60.46039</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1779,7 +1739,7 @@
         <v>46038.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>58.69131</v>
+        <v>59.40249</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1800,7 +1760,7 @@
         <v>46038.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>64.89</v>
+        <v>59.39334</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1821,7 +1781,7 @@
         <v>46038.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>80.02</v>
+        <v>79.95005</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1842,7 +1802,7 @@
         <v>46038.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>80.02</v>
+        <v>79.95</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1926,7 +1886,7 @@
         <v>46038.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>36.07</v>
+        <v>50.62891</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1947,7 +1907,7 @@
         <v>46038.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>48.49273</v>
+        <v>56.98</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1980,7 +1940,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1949,7 @@
         <v>46038.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>55.27342</v>
+        <v>56.97989</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2001,7 +1961,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2010,7 +1970,7 @@
         <v>46038.375</v>
       </c>
       <c r="B68" t="n">
-        <v>36.06</v>
+        <v>47.31837</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2052,7 +2012,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>36.06</v>
+        <v>45.92104</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2073,7 +2033,7 @@
         <v>46038.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>36.06</v>
+        <v>45.97441</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2094,7 +2054,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>36.05949</v>
+        <v>36.06028</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2157,7 +2117,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>36.0601</v>
+        <v>40.54</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2241,7 +2201,7 @@
         <v>46038.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>33.07075</v>
+        <v>36.0601</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2262,7 +2222,7 @@
         <v>46038.625</v>
       </c>
       <c r="B80" t="n">
-        <v>27.77113</v>
+        <v>28.73596</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2283,7 +2243,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>22.68446</v>
+        <v>25.59822</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2304,7 +2264,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>38.44817</v>
+        <v>18.17021</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2325,7 +2285,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>0.81985</v>
+        <v>8.64973</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2346,7 +2306,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-9.431789999999999</v>
+        <v>-7.981</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2367,7 +2327,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-8.136850000000001</v>
+        <v>-6.80121</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2388,7 +2348,7 @@
         <v>46038.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-6.78314</v>
+        <v>-6</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2409,7 +2369,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>-3.00909</v>
+        <v>-3.03118</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2430,7 +2390,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>-3.07152</v>
+        <v>-3.04997</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2451,7 +2411,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>29.85322</v>
+        <v>22.01959</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2472,7 +2432,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>32.40461</v>
+        <v>22.01959</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2493,7 +2453,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>32.40461</v>
+        <v>29.85322</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2514,7 +2474,7 @@
         <v>46038.875</v>
       </c>
       <c r="B92" t="n">
-        <v>29.85322</v>
+        <v>0.85459</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2535,7 +2495,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>78</v>
+        <v>57.78152</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2556,7 +2516,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>64.8901</v>
+        <v>57.04922</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2577,7 +2537,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>57.04922</v>
+        <v>57.45801</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2598,7 +2558,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>58.94929</v>
+        <v>58.21771</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2619,7 +2579,7 @@
         <v>46038.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 27)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>1167.7417245</v>
+        <v>1161.84723525</v>
       </c>
       <c r="F2" t="n">
-        <v>25.74386517857143</v>
+        <v>25.61391612103175</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>349.523304</v>
+        <v>348.247965</v>
       </c>
       <c r="F3" t="n">
-        <v>23.11662063492064</v>
+        <v>23.03227281746032</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,10 +561,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46038.02083333334</v>
+        <v>46038</v>
       </c>
       <c r="B2" t="n">
-        <v>78.36722</v>
+        <v>81.05549000000001</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -582,10 +582,10 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46038.04166666666</v>
+        <v>46038.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>84.7901</v>
+        <v>78</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -603,14 +603,14 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46038.0625</v>
+        <v>46038.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>84.7901</v>
+        <v>78</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
@@ -624,14 +624,14 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46038.08333333334</v>
+        <v>46038.0625</v>
       </c>
       <c r="B5" t="n">
         <v>84.7901</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
@@ -645,14 +645,14 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46038.10416666666</v>
+        <v>46038.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>78</v>
+        <v>84.7901</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
@@ -666,10 +666,10 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46038.125</v>
+        <v>46038.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>78</v>
+        <v>83.60652</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -687,10 +687,10 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46038.14583333334</v>
+        <v>46038.125</v>
       </c>
       <c r="B8" t="n">
-        <v>80.02</v>
+        <v>84.7901</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -708,10 +708,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46038.16666666666</v>
+        <v>46038.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>78</v>
+        <v>84.7901</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -723,16 +723,16 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46038.1875</v>
+        <v>46038.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>77.94</v>
+        <v>84.7901</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -750,10 +750,10 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46038.20833333334</v>
+        <v>46038.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>80.02</v>
+        <v>77.94</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -771,10 +771,10 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46038.22916666666</v>
+        <v>46038.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>87.16685</v>
+        <v>79.95</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46038.25</v>
+        <v>46038.22916666666</v>
       </c>
       <c r="B13" t="n">
         <v>80.02</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46038.27083333334</v>
+        <v>46038.25</v>
       </c>
       <c r="B14" t="n">
-        <v>57.06003</v>
+        <v>79.95</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -834,10 +834,10 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46038.29166666666</v>
+        <v>46038.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -855,10 +855,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46038.3125</v>
+        <v>46038.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>56.98</v>
+        <v>50.63034</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46038.33333333334</v>
+        <v>46038.3125</v>
       </c>
       <c r="B17" t="n">
         <v>56.98</v>
@@ -897,10 +897,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46038.35416666666</v>
+        <v>46038.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>56.89525</v>
+        <v>56.98</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -918,10 +918,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46038.375</v>
+        <v>46038.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>46.64807</v>
+        <v>56.89739</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -939,10 +939,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46038.39583333334</v>
+        <v>46038.375</v>
       </c>
       <c r="B20" t="n">
-        <v>36.06</v>
+        <v>46.64753</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -960,10 +960,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46038.41666666666</v>
+        <v>46038.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>45.94024</v>
+        <v>36.06</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -981,10 +981,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46038.4375</v>
+        <v>46038.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>41.22326</v>
+        <v>46.76441</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1002,10 +1002,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46038.45833333334</v>
+        <v>46038.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>36.07</v>
+        <v>41.46457</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46038.47916666666</v>
+        <v>46038.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>36.06</v>
+        <v>36.06028</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46038.5</v>
+        <v>46038.47916666666</v>
       </c>
       <c r="B25" t="n">
         <v>36.06</v>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46038.52083333334</v>
+        <v>46038.5</v>
       </c>
       <c r="B26" t="n">
-        <v>36.07</v>
+        <v>36.06</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>46038.54166666666</v>
+        <v>46038.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>36.0601</v>
+        <v>41.10377</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>46038.5625</v>
+        <v>46038.54166666666</v>
       </c>
       <c r="B28" t="n">
         <v>36.0601</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>46038.58333333334</v>
+        <v>46038.5625</v>
       </c>
       <c r="B29" t="n">
         <v>36.0601</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>46038.60416666666</v>
+        <v>46038.58333333334</v>
       </c>
       <c r="B30" t="n">
         <v>36.0601</v>
@@ -1170,10 +1170,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>46038.625</v>
+        <v>46038.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>27.2737</v>
+        <v>36.0601</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>46038.64583333334</v>
+        <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>23.99602</v>
+        <v>27.2786</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>46038.66666666666</v>
+        <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>41.86233</v>
+        <v>18.70077</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1227,16 +1227,16 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>46038.6875</v>
+        <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>7.72669</v>
+        <v>42.25471</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>46038.70833333334</v>
+        <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-6</v>
+        <v>10.34966</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1275,10 +1275,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>46038.72916666666</v>
+        <v>46038.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-6</v>
+        <v>2.10968</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1296,10 +1296,10 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>46038.75</v>
+        <v>46038.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-3.13051</v>
+        <v>-6</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>46038.77083333334</v>
+        <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.05379</v>
+        <v>-3.17523</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1338,10 +1338,10 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>46038.79166666666</v>
+        <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-3.05064</v>
+        <v>-3.03165</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>46038.8125</v>
+        <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>22.01959</v>
+        <v>0.0113</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>46038.83333333334</v>
+        <v>46038.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>22.01959</v>
+        <v>29.85322</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1395,16 +1395,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>46038.85416666666</v>
+        <v>46038.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>32.40461</v>
+        <v>29.85322</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1422,10 +1422,10 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>46038.875</v>
+        <v>46038.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0871</v>
+        <v>29.85322</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>46038.89583333334</v>
+        <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>73.73755</v>
+        <v>8.671720000000001</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1464,10 +1464,10 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>46038.91666666666</v>
+        <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>57.54503</v>
+        <v>59.0817</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>46038.9375</v>
+        <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.46081</v>
+        <v>57.09</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46038.95833333334</v>
+        <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>58.1919</v>
+        <v>57.44405</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1527,20 +1527,41 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
+        <v>46038.95833333334</v>
+      </c>
+      <c r="B48" t="n">
+        <v>58.20349</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
         <v>46038.97916666666</v>
       </c>
-      <c r="B48" t="n">
-        <v>57.03885</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>forecast</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="n">
-        <v>46038</v>
-      </c>
-      <c r="E48" t="inlineStr">
+      <c r="B49" t="n">
+        <v>56.98</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>46038</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>ON</t>
         </is>

</xml_diff>

<commit_message>
Update latest output (run 28)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>1161.84723525</v>
+        <v>1178.2416555</v>
       </c>
       <c r="F2" t="n">
-        <v>25.61391612103175</v>
+        <v>25.97534513888889</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>348.247965</v>
+        <v>354.6176205</v>
       </c>
       <c r="F3" t="n">
-        <v>23.03227281746032</v>
+        <v>23.45354632936508</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +627,7 @@
         <v>46038.0625</v>
       </c>
       <c r="B5" t="n">
-        <v>84.7901</v>
+        <v>78</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -648,7 +648,7 @@
         <v>46038.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>84.7901</v>
+        <v>78</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -669,11 +669,11 @@
         <v>46038.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>83.60652</v>
+        <v>87.05036</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
@@ -694,7 +694,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D8" s="3" t="n">
@@ -711,11 +711,11 @@
         <v>46038.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>84.7901</v>
+        <v>85.44701000000001</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
@@ -753,7 +753,7 @@
         <v>46038.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>77.94</v>
+        <v>80.02</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
         <v>46038.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>79.95</v>
+        <v>80.02</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -795,7 +795,7 @@
         <v>46038.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>80.02</v>
+        <v>93.26281</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -858,7 +858,7 @@
         <v>46038.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>50.63034</v>
+        <v>56.98</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -900,7 +900,7 @@
         <v>46038.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>56.98</v>
+        <v>56.97999</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -921,7 +921,7 @@
         <v>46038.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>56.89739</v>
+        <v>56.90274</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -942,7 +942,7 @@
         <v>46038.375</v>
       </c>
       <c r="B20" t="n">
-        <v>46.64753</v>
+        <v>47.13666</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>46.76441</v>
+        <v>46.68963</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
         <v>46038.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>41.46457</v>
+        <v>41.21992</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>36.06028</v>
+        <v>36.07</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>41.10377</v>
+        <v>36.07</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1194,7 +1194,7 @@
         <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>27.2786</v>
+        <v>27.27348</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>18.70077</v>
+        <v>18.62722</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>42.25471</v>
+        <v>17.79394</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>10.34966</v>
+        <v>7.7265</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>2.10968</v>
+        <v>-6</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1320,7 +1320,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.17523</v>
+        <v>-3.13002</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1341,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-3.03165</v>
+        <v>-3.05272</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0113</v>
+        <v>0.01129</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>8.671720000000001</v>
+        <v>0.08645</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1467,7 +1467,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>59.0817</v>
+        <v>73.73759</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1488,7 +1488,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.09</v>
+        <v>57.55625</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1509,7 +1509,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.44405</v>
+        <v>57.44178</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>58.20349</v>
+        <v>58.20187</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 29)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>1178.2416555</v>
+        <v>1191.14116875</v>
       </c>
       <c r="F2" t="n">
-        <v>25.97534513888889</v>
+        <v>26.25972594246032</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>354.6176205</v>
+        <v>367.04655</v>
       </c>
       <c r="F3" t="n">
-        <v>23.45354632936508</v>
+        <v>24.27556547619048</v>
       </c>
     </row>
   </sheetData>
@@ -669,7 +669,7 @@
         <v>46038.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>87.05036</v>
+        <v>69.42238</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -690,7 +690,7 @@
         <v>46038.125</v>
       </c>
       <c r="B8" t="n">
-        <v>84.7901</v>
+        <v>60.46039</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         <v>46038.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>85.44701000000001</v>
+        <v>84.7901</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -732,11 +732,11 @@
         <v>46038.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>84.7901</v>
+        <v>87.15796</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
@@ -795,7 +795,7 @@
         <v>46038.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>93.26281</v>
+        <v>93.85476</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -858,7 +858,7 @@
         <v>46038.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>56.98</v>
+        <v>50.66923</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -900,7 +900,7 @@
         <v>46038.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>56.97999</v>
+        <v>56.98</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -921,7 +921,7 @@
         <v>46038.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>56.90274</v>
+        <v>56.59029</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -942,7 +942,7 @@
         <v>46038.375</v>
       </c>
       <c r="B20" t="n">
-        <v>47.13666</v>
+        <v>47.14626</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>46.68963</v>
+        <v>46.76395</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
         <v>46038.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>41.21992</v>
+        <v>48.22486</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>36.07</v>
+        <v>40.96027</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1047,7 +1047,7 @@
         <v>46038.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>36.06</v>
+        <v>36.07</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>36.07</v>
+        <v>40.82473</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1194,7 +1194,7 @@
         <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>27.27348</v>
+        <v>27.27351</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>18.62722</v>
+        <v>18.777</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>17.79394</v>
+        <v>17.76526</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>7.7265</v>
+        <v>7.72659</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1320,7 +1320,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.13002</v>
+        <v>-3.13019</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1341,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-3.05272</v>
+        <v>-3.03124</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>0.08645</v>
+        <v>22.01959</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1467,7 +1467,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>73.73759</v>
+        <v>64.8901</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1488,7 +1488,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.55625</v>
+        <v>57.09</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1509,7 +1509,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.44178</v>
+        <v>57.52342</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>58.20187</v>
+        <v>58.1896</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
         <v>46038.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.98</v>
+        <v>57.03885</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 30)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,42 +475,62 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46038.16666666666</v>
+        <v>46038.02083333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46038.66666666666</v>
+        <v>46038.1875</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>45.36</v>
+        <v>15.12</v>
       </c>
       <c r="E2" t="n">
-        <v>1191.14116875</v>
+        <v>546.661635</v>
       </c>
       <c r="F2" t="n">
-        <v>26.25972594246032</v>
+        <v>36.15487003968254</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
+        <v>46038.33333333334</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>46038.66666666666</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>30.24</v>
+      </c>
+      <c r="E3" t="n">
+        <v>599.02786125</v>
+      </c>
+      <c r="F3" t="n">
+        <v>19.80912239583333</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>46038.83333333334</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B4" s="2" t="n">
         <v>46039</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>15.12</v>
       </c>
-      <c r="E3" t="n">
-        <v>367.04655</v>
-      </c>
-      <c r="F3" t="n">
-        <v>24.27556547619048</v>
+      <c r="E4" t="n">
+        <v>332.72408325</v>
+      </c>
+      <c r="F4" t="n">
+        <v>22.00556106150794</v>
       </c>
     </row>
   </sheetData>
@@ -597,7 +617,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -618,7 +638,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -639,7 +659,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -660,7 +680,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -681,7 +701,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -702,7 +722,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -711,7 +731,7 @@
         <v>46038.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>84.7901</v>
+        <v>59.40249</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -723,7 +743,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -732,7 +752,7 @@
         <v>46038.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>87.15796</v>
+        <v>59.39334</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -753,11 +773,11 @@
         <v>46038.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>80.02</v>
+        <v>105</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
@@ -765,7 +785,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -774,11 +794,11 @@
         <v>46038.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>80.02</v>
+        <v>105</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
@@ -786,7 +806,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -795,11 +815,11 @@
         <v>46038.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>93.85476</v>
+        <v>105</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
@@ -807,7 +827,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -816,7 +836,7 @@
         <v>46038.25</v>
       </c>
       <c r="B14" t="n">
-        <v>79.95</v>
+        <v>80.02</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -828,7 +848,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -849,7 +869,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -858,7 +878,7 @@
         <v>46038.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>50.66923</v>
+        <v>53.68744</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -870,7 +890,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -891,7 +911,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -921,7 +941,7 @@
         <v>46038.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>56.59029</v>
+        <v>56.77175</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -942,7 +962,7 @@
         <v>46038.375</v>
       </c>
       <c r="B20" t="n">
-        <v>47.14626</v>
+        <v>47.16364</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -984,7 +1004,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>46.76395</v>
+        <v>36.06</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1005,7 +1025,7 @@
         <v>46038.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>48.22486</v>
+        <v>36.07</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1026,7 +1046,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>40.96027</v>
+        <v>40.72701</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1047,7 +1067,7 @@
         <v>46038.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>36.07</v>
+        <v>36.06</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1089,7 +1109,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>40.82473</v>
+        <v>40.83066</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1194,7 +1214,7 @@
         <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>27.27351</v>
+        <v>27.27134</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1235,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>18.777</v>
+        <v>20.09275</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1256,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>17.76526</v>
+        <v>18.11374</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1277,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>7.72659</v>
+        <v>8.450419999999999</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1320,7 +1340,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.13019</v>
+        <v>-3.17436</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1361,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-3.03124</v>
+        <v>-3.0523</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1362,7 +1382,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>0.01129</v>
+        <v>-0.54575</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1404,7 +1424,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>29.85322</v>
+        <v>22.01959</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1446,7 +1466,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>22.01959</v>
+        <v>0.0858</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1467,7 +1487,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>64.8901</v>
+        <v>59.08295</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1488,7 +1508,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.09</v>
+        <v>57.58853</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1509,7 +1529,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.52342</v>
+        <v>57.45443</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1530,7 +1550,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>58.1896</v>
+        <v>58.19095</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1551,7 +1571,7 @@
         <v>46038.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>57.03885</v>
+        <v>56.98</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 32)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,62 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46038.02083333334</v>
+        <v>46038.16666666666</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46038.1875</v>
+        <v>46038.66666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>15.12</v>
+        <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>546.661635</v>
+        <v>1126.019388</v>
       </c>
       <c r="F2" t="n">
-        <v>36.15487003968254</v>
+        <v>24.82406058201058</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46038.33333333334</v>
+        <v>46038.83333333334</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46038.66666666666</v>
+        <v>46039</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>30.24</v>
+        <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>572.50464375</v>
+        <v>337.0658655</v>
       </c>
       <c r="F3" t="n">
-        <v>18.93203187003968</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>46038.83333333334</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>46039</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E4" t="n">
-        <v>330.5716245</v>
-      </c>
-      <c r="F4" t="n">
-        <v>21.86320267857143</v>
+        <v>22.29271597222222</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +597,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -638,7 +618,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -659,7 +639,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -680,7 +660,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -701,7 +681,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -722,7 +702,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -743,7 +723,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -785,7 +765,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -806,7 +786,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -815,7 +795,7 @@
         <v>46038.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>105</v>
+        <v>85.95</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -827,7 +807,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -836,7 +816,7 @@
         <v>46038.25</v>
       </c>
       <c r="B14" t="n">
-        <v>80.02</v>
+        <v>79.95</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -848,7 +828,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -861,7 +841,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
@@ -869,7 +849,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -882,7 +862,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
@@ -890,7 +870,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -899,7 +879,7 @@
         <v>46038.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>56.98</v>
+        <v>50.38708</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -911,7 +891,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -920,7 +900,7 @@
         <v>46038.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>56.97999</v>
+        <v>56.98</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -941,7 +921,7 @@
         <v>46038.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>48.86725</v>
+        <v>55.25227</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -983,7 +963,7 @@
         <v>46038.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>36.06</v>
+        <v>36.05916</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1046,7 +1026,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>36.07</v>
+        <v>36.06028</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1214,7 +1194,7 @@
         <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>28.9852</v>
+        <v>35.85034</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1235,7 +1215,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>19.62131</v>
+        <v>24.46863</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1256,7 +1236,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>19.23499</v>
+        <v>19.24233</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,7 +1257,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>8.450419999999999</v>
+        <v>10.31216</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1298,7 +1278,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-6</v>
+        <v>-1.5001</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1340,7 +1320,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.17461</v>
+        <v>-3.17664</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1341,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.70941</v>
+        <v>-2.7582</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1382,7 +1362,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>0.01121</v>
+        <v>0.0113</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1445,7 +1425,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>22.01959</v>
+        <v>29.85322</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1446,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>0.04217</v>
+        <v>0.84406</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1487,7 +1467,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>59.01628</v>
+        <v>57.04922</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1529,7 +1509,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.04367</v>
+        <v>57.04922</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1550,7 +1530,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.04367</v>
+        <v>57.03042</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 33)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>1126.019388</v>
+        <v>890.0228512499999</v>
       </c>
       <c r="F2" t="n">
-        <v>24.82406058201058</v>
+        <v>19.62131506283069</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>337.0658655</v>
+        <v>386.1981435</v>
       </c>
       <c r="F3" t="n">
-        <v>22.29271597222222</v>
+        <v>25.54220525793651</v>
       </c>
     </row>
   </sheetData>
@@ -858,7 +858,7 @@
         <v>46038.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>56.98</v>
+        <v>50.62891</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -879,11 +879,11 @@
         <v>46038.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>50.38708</v>
+        <v>36.06</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
@@ -900,11 +900,11 @@
         <v>46038.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>56.98</v>
+        <v>36.06</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
@@ -921,7 +921,7 @@
         <v>46038.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>55.25227</v>
+        <v>57.06003</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -963,7 +963,7 @@
         <v>46038.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>36.05916</v>
+        <v>36.05971</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>36.06028</v>
+        <v>36.07</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>36.0601</v>
+        <v>36.07</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1110,7 +1110,7 @@
         <v>46038.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>36.0601</v>
+        <v>36.07</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>46038.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>36.0601</v>
+        <v>22.07</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1152,7 +1152,7 @@
         <v>46038.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>36.0601</v>
+        <v>-5.50985</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
         <v>46038.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>36.0601</v>
+        <v>-17.43694</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1194,7 +1194,7 @@
         <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>35.85034</v>
+        <v>-17.36059</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>24.46863</v>
+        <v>-15.55074</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>19.24233</v>
+        <v>19.14129</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>10.31216</v>
+        <v>10.3197</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-1.5001</v>
+        <v>2.14574</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1320,7 +1320,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.17664</v>
+        <v>-3.17514</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1341,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.7582</v>
+        <v>3.14796</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0113</v>
+        <v>0.01138</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1383,7 +1383,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>29.85322</v>
+        <v>32.40461</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1404,7 +1404,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>29.85322</v>
+        <v>32.40461</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1425,7 +1425,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>29.85322</v>
+        <v>32.40461</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>0.84406</v>
+        <v>29.85322</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1467,7 +1467,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>57.04922</v>
+        <v>73.20007</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1488,7 +1488,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.04922</v>
+        <v>57.09</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.03042</v>
+        <v>57.0389</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
         <v>46038.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 36)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>592.3275247500002</v>
+        <v>753.22077675</v>
       </c>
       <c r="F2" t="n">
-        <v>13.05836694775133</v>
+        <v>16.60539631283069</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>357.79152825</v>
+        <v>346.9494795</v>
       </c>
       <c r="F3" t="n">
-        <v>23.66346086309524</v>
+        <v>22.9463941468254</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +963,7 @@
         <v>46038.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-11.03101</v>
+        <v>36.06</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         <v>46038.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-8.94445</v>
+        <v>45.92104</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1005,11 +1005,11 @@
         <v>46038.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>36.06</v>
+        <v>45.97441</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
@@ -1026,11 +1026,11 @@
         <v>46038.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>36.06</v>
+        <v>36.06028</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
@@ -1047,11 +1047,11 @@
         <v>46038.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-16.24859</v>
+        <v>21.24005</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
@@ -1068,11 +1068,11 @@
         <v>46038.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-16.86993</v>
+        <v>0</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
@@ -1089,7 +1089,7 @@
         <v>46038.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-17.10346</v>
+        <v>-16.1572</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1110,7 +1110,7 @@
         <v>46038.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-15.51447</v>
+        <v>-16.27493</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         <v>46038.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-17.0409</v>
+        <v>-16.47514</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1152,7 +1152,7 @@
         <v>46038.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-22.18182</v>
+        <v>-21.15844</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
         <v>46038.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-17.11931</v>
+        <v>-21.40354</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1194,7 +1194,7 @@
         <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-16.88235</v>
+        <v>-16.02</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-16.88892</v>
+        <v>-16.45302</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>18.11384</v>
+        <v>5.34014</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>10.27661</v>
+        <v>4.15594</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-10.86954</v>
+        <v>-9.5</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1299,7 +1299,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-9.415330000000001</v>
+        <v>-10.45391</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1320,7 +1320,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-9.253819999999999</v>
+        <v>-9.181150000000001</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1341,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-3.05055</v>
+        <v>-2.98349</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.5508</v>
+        <v>-3.00221</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1383,7 +1383,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>29.85322</v>
+        <v>20.41263</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1404,7 +1404,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>29.85322</v>
+        <v>27.59769</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1425,7 +1425,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>29.85322</v>
+        <v>21.52393</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>22.01959</v>
+        <v>21.52393</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1488,7 +1488,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.09</v>
+        <v>56.98</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1509,7 +1509,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.04922</v>
+        <v>57.09</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.03042</v>
+        <v>57.06007</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 38)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>930.0173805000001</v>
+        <v>1043.1788055</v>
       </c>
       <c r="F2" t="n">
-        <v>20.50302867063492</v>
+        <v>22.99776908068783</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>324.186837</v>
+        <v>368.2275285</v>
       </c>
       <c r="F3" t="n">
-        <v>21.44092837301587</v>
+        <v>24.35367251984127</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>45.36</v>
       </c>
       <c r="E4" t="n">
-        <v>-112.892013</v>
+        <v>-58.6619475</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.488800992063492</v>
+        <v>-1.293252810846561</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1151,7 @@
         <v>46038.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-22.255</v>
+        <v>36.0601</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1172,7 +1172,7 @@
         <v>46038.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-14</v>
+        <v>36.0601</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1193,11 +1193,11 @@
         <v>46038.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-14</v>
+        <v>-4.05321</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D31" s="3" t="n">
@@ -1214,11 +1214,11 @@
         <v>46038.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-15.63074</v>
+        <v>-15.51759</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D32" s="3" t="n">
@@ -1235,11 +1235,11 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-4.20662</v>
+        <v>-6.57876</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D33" s="3" t="n">
@@ -1256,7 +1256,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>2.44544</v>
+        <v>4.29232</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,7 +1277,7 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-4.10876</v>
+        <v>-3.47865</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1298,7 +1298,7 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-6.73245</v>
+        <v>-6</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1319,7 +1319,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-6.60018</v>
+        <v>-1.57063</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-3.12186</v>
+        <v>-3.20521</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.73786</v>
+        <v>1.18622</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>-2.74631</v>
+        <v>0.00045</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>12.41698</v>
+        <v>23.74544</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>12.51189</v>
+        <v>32.79309</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1445,7 +1445,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>20.67595</v>
+        <v>24.74099</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>6.37544</v>
+        <v>21.88816</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1508,7 +1508,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.98</v>
+        <v>64.8901</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1529,7 +1529,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>64.93597</v>
+        <v>62.33685</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         <v>46039.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>56.98</v>
+        <v>57.06017</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1844,7 +1844,7 @@
         <v>46039.25</v>
       </c>
       <c r="B62" t="n">
-        <v>52.585</v>
+        <v>51.15669</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1886,7 +1886,7 @@
         <v>46039.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>36.06</v>
+        <v>36.06029</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         <v>46039.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>0.51</v>
+        <v>6.27504</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46039.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>-5.51</v>
+        <v>-4.56332</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>-5.78275</v>
+        <v>-0.90384</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         <v>46039.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-4.83962</v>
+        <v>0.0094</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46039.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.9809099999999999</v>
+        <v>-0.00776</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.88414</v>
+        <v>-0.89434</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46039.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>22.07</v>
+        <v>-5.50985</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>7.88135</v>
+        <v>6.25571</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46039.5</v>
       </c>
       <c r="B74" t="n">
-        <v>7.21991</v>
+        <v>8.71008</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.83992</v>
+        <v>0.7</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46039.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-4.81333</v>
+        <v>-5.51011</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46039.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-9.99</v>
+        <v>-7.01</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-18.98278</v>
+        <v>-11.17408</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-12.26241</v>
+        <v>-12.11173</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46039.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-10.70447</v>
+        <v>-6.72418</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-12.11173</v>
+        <v>-5.66385</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-13.26203</v>
+        <v>-2.21718</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-22.57861</v>
+        <v>-5.17419</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-13.43756</v>
+        <v>-6.49855</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-9.5</v>
+        <v>-3.05311</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46039.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-7.16571</v>
+        <v>-2.93302</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>-2.88098</v>
+        <v>-2.92219</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>3.05901</v>
+        <v>0.75497</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>16.37244</v>
+        <v>21.60312</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>17.98198</v>
+        <v>51.84959</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>13.59537</v>
+        <v>32.62903</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46039.875</v>
       </c>
       <c r="B92" t="n">
-        <v>55.12255</v>
+        <v>29.54841</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>56.98</v>
+        <v>36.0601</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
         <v>46039.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>47.26597</v>
+        <v>36.06045</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>36.06041</v>
+        <v>57.3</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         <v>46039.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>36.06043</v>
+        <v>57.3</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2579,7 +2579,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>36.0604</v>
+        <v>57.06005</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 40)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>1115.13373725</v>
+        <v>1156.8090495</v>
       </c>
       <c r="F2" t="n">
-        <v>24.58407709986773</v>
+        <v>25.50284500661376</v>
       </c>
     </row>
     <row r="3">
@@ -507,18 +507,18 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>362.944725</v>
+        <v>309.4335659999999</v>
       </c>
       <c r="F3" t="n">
-        <v>24.00428075396826</v>
+        <v>20.46518293650793</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46039.33333333334</v>
+        <v>46039.3125</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46039.83333333334</v>
+        <v>46039.8125</v>
       </c>
       <c r="C4" t="n">
         <v>12</v>
@@ -527,10 +527,10 @@
         <v>45.36</v>
       </c>
       <c r="E4" t="n">
-        <v>-45.41884425000002</v>
+        <v>-117.1090635</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.001297271825397</v>
+        <v>-2.581769477513227</v>
       </c>
     </row>
   </sheetData>
@@ -1235,7 +1235,7 @@
         <v>46038.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-17.14569</v>
+        <v>25.59822</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>46038.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-11.91363</v>
+        <v>18.17021</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,11 +1277,11 @@
         <v>46038.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-7.76371</v>
+        <v>-34.28578</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D35" s="3" t="n">
@@ -1298,11 +1298,11 @@
         <v>46038.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-6.71925</v>
+        <v>-9.77904</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D36" s="3" t="n">
@@ -1319,7 +1319,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-3.18807</v>
+        <v>-6.84011</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.13614</v>
+        <v>-3.13143</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>0.08790000000000001</v>
+        <v>-3.05909</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>10.54681</v>
+        <v>-3.12465</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>23.33001</v>
+        <v>5.07885</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>32.8827</v>
+        <v>10.55942</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1445,7 +1445,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>24.50413</v>
+        <v>21.58386</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>21.974</v>
+        <v>0.19633</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>64.8901</v>
+        <v>57.04922</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1529,7 +1529,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>56.98</v>
+        <v>57.03893</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.06007</v>
+        <v>56.98</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46039.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>58.42372</v>
+        <v>56.98</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1844,7 +1844,7 @@
         <v>46039.25</v>
       </c>
       <c r="B62" t="n">
-        <v>56.98</v>
+        <v>57.06018</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         <v>46039.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>23.90219</v>
+        <v>0.51</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1928,7 +1928,7 @@
         <v>46039.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.8980900000000001</v>
+        <v>-5.51</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>-5.33054</v>
+        <v>-4.81333</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         <v>46039.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-2.83936</v>
+        <v>0.51003</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46039.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.89852</v>
+        <v>0</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-2.54301</v>
+        <v>-0.87926</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46039.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>0.00886</v>
+        <v>-0.87869</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>0.51003</v>
+        <v>-0.85809</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>0.51003</v>
+        <v>-0.84198</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46039.5</v>
       </c>
       <c r="B74" t="n">
-        <v>0.008630000000000001</v>
+        <v>-3.6481</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>6.90404</v>
+        <v>-4.81333</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46039.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-4.81333</v>
+        <v>-8.5</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46039.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-11.16992</v>
+        <v>-14</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-12.08785</v>
+        <v>-14</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46039.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-10.065</v>
+        <v>-12.11173</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-5.92668</v>
+        <v>-7.92844</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>5.27491</v>
+        <v>-2.88008</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-9.060980000000001</v>
+        <v>-6.76678</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-6.69718</v>
+        <v>-7.78482</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-3.05417</v>
+        <v>-4.96609</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46039.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-2.9124</v>
+        <v>-6.19024</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>-2.92257</v>
+        <v>-6</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>6.81655</v>
+        <v>2.23907</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>21.60312</v>
+        <v>17.98199</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -2432,7 +2432,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>57.16514</v>
+        <v>32.58868</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>32.64304</v>
+        <v>29.51425</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46039.875</v>
       </c>
       <c r="B92" t="n">
-        <v>8.499320000000001</v>
+        <v>29.67769</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>57.3</v>
+        <v>64.8901</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         <v>46039.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>57.3</v>
+        <v>64.8901</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2579,7 +2579,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>57.06005</v>
+        <v>64.8901</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 42)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>278.1123345</v>
+        <v>352.1131185</v>
       </c>
       <c r="F3" t="n">
-        <v>18.39367291666667</v>
+        <v>23.28790466269841</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>45.36</v>
       </c>
       <c r="E4" t="n">
-        <v>-131.59852875</v>
+        <v>-149.15047875</v>
       </c>
       <c r="F4" t="n">
-        <v>-2.901202132936508</v>
+        <v>-3.288149884259259</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1319,7 @@
         <v>46038.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-8.90727</v>
+        <v>-6.80121</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46038.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.98843</v>
+        <v>-6</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,11 +1361,11 @@
         <v>46038.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.62019</v>
+        <v>-3.1159</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
@@ -1382,11 +1382,11 @@
         <v>46038.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>3.15941</v>
+        <v>34.26695</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1403,7 +1403,7 @@
         <v>46038.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>24.11812</v>
+        <v>36.25056</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46038.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>25.00316</v>
+        <v>35.87161</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1445,7 +1445,7 @@
         <v>46038.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>17.20654</v>
+        <v>20.51366</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         <v>46038.875</v>
       </c>
       <c r="B44" t="n">
-        <v>16.67999</v>
+        <v>17.88508</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         <v>46038.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>56.98</v>
+        <v>62.33685</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1508,7 +1508,7 @@
         <v>46038.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>36.0601</v>
+        <v>62.33685</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1529,7 +1529,7 @@
         <v>46038.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>53.84201</v>
+        <v>61.94424</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         <v>46038.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>43.41162</v>
+        <v>56.98</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
         <v>46038.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>36.06</v>
+        <v>43.27337</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         <v>46039.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>40.54</v>
+        <v>41.38585</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         <v>46039.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>36.06</v>
+        <v>40.54</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46039.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>65</v>
+        <v>59.08177</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1844,7 +1844,7 @@
         <v>46039.25</v>
       </c>
       <c r="B62" t="n">
-        <v>57.06018</v>
+        <v>56.98</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46039.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.87734</v>
+        <v>-0.88256</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>-5.65164</v>
+        <v>-5.11737</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         <v>46039.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-5.30295</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46039.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.50985</v>
+        <v>-5.2121</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.87893</v>
+        <v>-5.51</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46039.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-4.64736</v>
+        <v>-5.51</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-5.01</v>
+        <v>-5.64248</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-1.092</v>
+        <v>-5.01</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46039.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-5.06248</v>
+        <v>-1.40538</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-5.63691</v>
+        <v>-2.67373</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46039.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-11.16992</v>
+        <v>-9.99</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-12.35725</v>
+        <v>-12.3505</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46039.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-12.11173</v>
+        <v>-17.41389</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-8.222300000000001</v>
+        <v>-13.9999</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>-6.41446</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-7.74498</v>
+        <v>-11</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-7.78104</v>
+        <v>-9.5</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-5.66127</v>
+        <v>-5.17024</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46039.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-6.18295</v>
+        <v>-6.19141</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>-6.02102</v>
+        <v>-5.9299</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>43.04957</v>
+        <v>13.59537</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>56.98</v>
+        <v>9.56921</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46039.875</v>
       </c>
       <c r="B92" t="n">
-        <v>8.320819999999999</v>
+        <v>36.0601</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 48)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>767.3495895000003</v>
+        <v>768.514968</v>
       </c>
       <c r="F2" t="n">
-        <v>12.68765855654762</v>
+        <v>12.70692738095238</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +544,7 @@
         <v>46039</v>
       </c>
       <c r="B2" t="n">
-        <v>57.06003</v>
+        <v>57.09</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -565,7 +565,7 @@
         <v>46039.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>57.06003</v>
+        <v>57.09</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -586,11 +586,11 @@
         <v>46039.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>57.06003</v>
+        <v>57.09</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
@@ -628,7 +628,7 @@
         <v>46039.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>40.54</v>
+        <v>57.06003</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         <v>46039.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>36.06</v>
+        <v>40.54</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -670,7 +670,7 @@
         <v>46039.125</v>
       </c>
       <c r="B8" t="n">
-        <v>36.06</v>
+        <v>40.54</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -691,7 +691,7 @@
         <v>46039.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>36.06</v>
+        <v>56.98</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
         <v>46039.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>36.06</v>
+        <v>56.98</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
         <v>46039.25</v>
       </c>
       <c r="B14" t="n">
-        <v>56.98</v>
+        <v>57.06018</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         <v>46039.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>50.75794</v>
+        <v>50.75171</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>46039.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>36.06029</v>
+        <v>36.2</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>46039.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>5.96508</v>
+        <v>36.06029</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46039.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>36.06011</v>
+        <v>15.43474</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>36.06011</v>
+        <v>13.96726</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46039.375</v>
       </c>
       <c r="B20" t="n">
-        <v>36.06054</v>
+        <v>36.06011</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46039.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>36.06011</v>
+        <v>35.88</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>36.06011</v>
+        <v>36.06057</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>35.88</v>
+        <v>36.06092</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>36.06092</v>
+        <v>36.06046</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>36.06045</v>
+        <v>36.06</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46039.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>36.06045</v>
+        <v>36.0609</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46039.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>34.74038</v>
+        <v>31.0352</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>30.215</v>
+        <v>36.06029</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>28.0606</v>
+        <v>36.06031</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>22.50771</v>
+        <v>22.50263</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.57265</v>
+        <v>-0.57355</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-2.99287</v>
+        <v>-2.99308</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.80956</v>
+        <v>-2.83044</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.7774</v>
+        <v>-2.77762</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>8.572229999999999</v>
+        <v>8.580550000000001</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>9.709530000000001</v>
+        <v>11.92003</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>9.58447</v>
+        <v>11.09544</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>9.520009999999999</v>
+        <v>9.361459999999999</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>9.75056</v>
+        <v>9.751200000000001</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.06008</v>
+        <v>56.98</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.47</v>
+        <v>56.98</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 50)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>781.7284702500003</v>
+        <v>822.923712</v>
       </c>
       <c r="F2" t="n">
-        <v>12.92540460069445</v>
+        <v>13.60654285714286</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +607,7 @@
         <v>46039.0625</v>
       </c>
       <c r="B5" t="n">
-        <v>57.09</v>
+        <v>57.06003</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
         <v>46039.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>56.97996</v>
+        <v>40.54</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -653,7 +653,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
@@ -670,11 +670,11 @@
         <v>46039.125</v>
       </c>
       <c r="B8" t="n">
-        <v>56.97996</v>
+        <v>57.06003</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D8" s="3" t="n">
@@ -691,7 +691,7 @@
         <v>46039.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
         <v>46039.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         <v>46039.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>57.3</v>
+        <v>65</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
         <v>46039.25</v>
       </c>
       <c r="B14" t="n">
-        <v>57.3</v>
+        <v>65</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         <v>46039.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>36.2</v>
+        <v>56.98</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>46039.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>18.4525</v>
+        <v>36.06029</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46039.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>0.7</v>
+        <v>16.50213</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>36.06011</v>
+        <v>26.94954</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46039.375</v>
       </c>
       <c r="B20" t="n">
-        <v>36.06054</v>
+        <v>36.06011</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46039.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>36.06011</v>
+        <v>35.88</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>46.43705</v>
+        <v>36.06011</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>44.73383</v>
+        <v>36.06046</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46039.5</v>
       </c>
       <c r="B26" t="n">
-        <v>36.06046</v>
+        <v>46.49741</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46039.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>36.06029</v>
+        <v>36.06</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>30.01081</v>
+        <v>29.64647</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>25.55134</v>
+        <v>27.14114</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.32102</v>
+        <v>-0.32145</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-3.01589</v>
+        <v>-3.016</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.85215</v>
+        <v>-2.85235</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.79911</v>
+        <v>-2.81987</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0109</v>
+        <v>4.5258</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>9.38786</v>
+        <v>9.627840000000001</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>29.66317</v>
+        <v>29.59904</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>9.42876</v>
+        <v>9.659560000000001</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>9.52481</v>
+        <v>9.36539</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>9.754619999999999</v>
+        <v>9.754899999999999</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>56.98</v>
+        <v>57.06004</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 54)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>772.4833740000001</v>
+        <v>794.102088</v>
       </c>
       <c r="F2" t="n">
-        <v>12.77254255952381</v>
+        <v>13.12999484126984</v>
       </c>
     </row>
   </sheetData>
@@ -754,7 +754,7 @@
         <v>46039.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>65</v>
+        <v>57.1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -775,7 +775,7 @@
         <v>46039.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>73.20003</v>
+        <v>57.3</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -817,11 +817,11 @@
         <v>46039.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>56.98</v>
+        <v>36.2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
@@ -842,7 +842,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
@@ -859,7 +859,7 @@
         <v>46039.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>24.30882</v>
+        <v>36.06029</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46039.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>25.52278</v>
+        <v>29.57649</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>28.96238</v>
+        <v>36.06011</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46039.375</v>
       </c>
       <c r="B20" t="n">
-        <v>36.06054</v>
+        <v>36.06011</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>46039.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>35.88</v>
+        <v>36.06032</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>35.88</v>
+        <v>36.06046</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>36.06092</v>
+        <v>50.35718</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46039.5</v>
       </c>
       <c r="B26" t="n">
-        <v>48.81498</v>
+        <v>36.06092</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>36.06029</v>
+        <v>36.06</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>27.99749</v>
+        <v>36.06031</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46039.625</v>
       </c>
       <c r="B32" t="n">
-        <v>30.21678</v>
+        <v>30.35616</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>36.05863</v>
+        <v>36.06038</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>33.26446</v>
+        <v>33.26801</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>8.26928</v>
+        <v>8.41405</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-3.07654</v>
+        <v>-3.07809</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-2.99582</v>
+        <v>-3.01858</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.91605</v>
+        <v>-2.91738</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.86176</v>
+        <v>-2.86323</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>3.42645</v>
+        <v>3.4639</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>9.65137</v>
+        <v>9.5329</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>9.71463</v>
+        <v>29.71119</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>19.54531</v>
+        <v>9.59267</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>8.333019999999999</v>
+        <v>8.33337</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>6.5735</v>
+        <v>6.57492</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46039.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>30.19777</v>
+        <v>30.05581</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.06008</v>
+        <v>56.98</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>47.60925</v>
+        <v>47.61072</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 55)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>794.102088</v>
+        <v>878.5684342500001</v>
       </c>
       <c r="F2" t="n">
-        <v>13.12999484126984</v>
+        <v>14.52659448164683</v>
       </c>
     </row>
   </sheetData>
@@ -796,7 +796,7 @@
         <v>46039.25</v>
       </c>
       <c r="B14" t="n">
-        <v>65</v>
+        <v>56.98</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         <v>46039.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>36.2</v>
+        <v>50.46272</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -863,7 +863,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
@@ -880,11 +880,11 @@
         <v>46039.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>29.57649</v>
+        <v>12.94586</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
@@ -901,7 +901,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>36.06011</v>
+        <v>18.67563</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46039.375</v>
       </c>
       <c r="B20" t="n">
-        <v>36.06011</v>
+        <v>27.87441</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>36.06011</v>
+        <v>33.86823</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>46039.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>36.06032</v>
+        <v>35.88</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>36.06046</v>
+        <v>36.06092</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>50.35718</v>
+        <v>44.06468</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46039.5</v>
       </c>
       <c r="B26" t="n">
-        <v>36.06092</v>
+        <v>36.06046</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>36.06045</v>
+        <v>43.1301</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46039.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>36.06045</v>
+        <v>46.34072</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>36.06</v>
+        <v>34.78031</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46039.625</v>
       </c>
       <c r="B32" t="n">
-        <v>30.35616</v>
+        <v>36.06033</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>33.26801</v>
+        <v>36.05879</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>8.41405</v>
+        <v>16.07216</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-3.07809</v>
+        <v>-0.41405</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-3.01858</v>
+        <v>-2.99806</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.91738</v>
+        <v>-2.91785</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.86323</v>
+        <v>-2.88418</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>3.4639</v>
+        <v>7.52239</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>9.5329</v>
+        <v>32.87797</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>29.71119</v>
+        <v>56.40935</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>9.59267</v>
+        <v>10.22525</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>8.33337</v>
+        <v>19.64731</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>6.57492</v>
+        <v>22.87055</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46039.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>30.05581</v>
+        <v>36.06045</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>47.61072</v>
+        <v>56.98</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 57)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>789.1812434999999</v>
+        <v>661.6262347500001</v>
       </c>
       <c r="F2" t="n">
-        <v>13.04863167162698</v>
+        <v>10.93958721478175</v>
       </c>
     </row>
   </sheetData>
@@ -901,7 +901,7 @@
         <v>46039.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>36.06011</v>
+        <v>33.22362</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46039.375</v>
       </c>
       <c r="B20" t="n">
-        <v>36.06011</v>
+        <v>35.88</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,11 +943,11 @@
         <v>46039.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>36.06011</v>
+        <v>-9.5031</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
@@ -964,11 +964,11 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>5.98325</v>
+        <v>-7.46266</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
@@ -985,7 +985,7 @@
         <v>46039.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>35.88</v>
+        <v>22.07</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>32.34641</v>
+        <v>0.7</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>36.06046</v>
+        <v>22.07</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46039.5</v>
       </c>
       <c r="B26" t="n">
-        <v>35.88</v>
+        <v>36.06046</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>32.51579</v>
+        <v>36.06045</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>23.63823</v>
+        <v>23.97858</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>23.5144</v>
+        <v>23.50558</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46039.625</v>
       </c>
       <c r="B32" t="n">
-        <v>24.28971</v>
+        <v>28.08235</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>36.061</v>
+        <v>40.54</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>33.26822</v>
+        <v>33.2694</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>23.74211</v>
+        <v>8.34709</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.12629</v>
+        <v>-0.09452000000000001</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-3.02299</v>
+        <v>-2.99905</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.9204</v>
+        <v>-2.89726</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.90758</v>
+        <v>-2.90585</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>32.90602</v>
+        <v>13.59537</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>33.03132</v>
+        <v>29.68591</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>9.53241</v>
+        <v>29.86477</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>19.51387</v>
+        <v>15.46948</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46039.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.98</v>
+        <v>57.06005</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 58)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>661.6262347500001</v>
+        <v>396.92921775</v>
       </c>
       <c r="F2" t="n">
-        <v>10.93958721478175</v>
+        <v>6.562983097718255</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +943,7 @@
         <v>46039.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-9.5031</v>
+        <v>36.06011</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46039.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-7.46266</v>
+        <v>36.06011</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -985,11 +985,11 @@
         <v>46039.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>22.07</v>
+        <v>36.06032</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
@@ -1006,11 +1006,11 @@
         <v>46039.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>0.7</v>
+        <v>35.88</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
@@ -1027,11 +1027,11 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>22.07</v>
+        <v>-18.02293</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
@@ -1048,11 +1048,11 @@
         <v>46039.5</v>
       </c>
       <c r="B26" t="n">
-        <v>36.06046</v>
+        <v>-18.19512</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
@@ -1069,7 +1069,7 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>36.06045</v>
+        <v>-14</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46039.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>36.06045</v>
+        <v>-14</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46039.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>36.06029</v>
+        <v>-8.12561</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>23.97858</v>
+        <v>-4.81333</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>23.50558</v>
+        <v>-6.8</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46039.625</v>
       </c>
       <c r="B32" t="n">
-        <v>28.08235</v>
+        <v>-6.8</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>40.54</v>
+        <v>0.7</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>33.2694</v>
+        <v>18.88451</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>8.34709</v>
+        <v>3.18383</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.09452000000000001</v>
+        <v>-0.31005</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-2.99905</v>
+        <v>-2.94054</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.89726</v>
+        <v>-2.88187</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.90585</v>
+        <v>-2.95405</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>4.5258</v>
+        <v>8.24929</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>13.59537</v>
+        <v>30.48176</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>29.68591</v>
+        <v>30.57917</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>29.86477</v>
+        <v>9.88462</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>15.46948</v>
+        <v>9.816660000000001</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>36.0601</v>
+        <v>22.66264</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.3</v>
+        <v>57.06004</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46039.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.3</v>
+        <v>57.06002</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>57.06005</v>
+        <v>56.98</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 59)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,22 +475,82 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46039.27083333334</v>
+        <v>46039.02083333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46039.9375</v>
+        <v>46039.1875</v>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>60.48</v>
+        <v>15.12</v>
       </c>
       <c r="E2" t="n">
-        <v>396.92921775</v>
+        <v>347.06108775</v>
       </c>
       <c r="F2" t="n">
-        <v>6.562983097718255</v>
+        <v>22.95377564484127</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>46039.29166666666</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>46039.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>313.99407</v>
+      </c>
+      <c r="F3" t="n">
+        <v>16.61344285714286</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>46039.52083333334</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>46039.8125</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>26.46</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9.565959000000007</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.3615252834467123</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>46040.29166666666</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>46040.79166666666</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>45.36</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-95.68104975</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-2.10937058531746</v>
       </c>
     </row>
   </sheetData>
@@ -504,7 +564,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,7 +637,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -598,7 +658,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -619,7 +679,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -640,7 +700,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -661,7 +721,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -682,7 +742,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -703,7 +763,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -724,7 +784,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -829,7 +889,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1087,7 @@
         <v>46039.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-18.02293</v>
+        <v>36.06046</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1108,7 @@
         <v>46039.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-18.19512</v>
+        <v>36.06092</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1060,7 +1120,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1069,11 +1129,11 @@
         <v>46039.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-14</v>
+        <v>36.06045</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
@@ -1090,11 +1150,11 @@
         <v>46039.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-14</v>
+        <v>-9.99</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D28" s="3" t="n">
@@ -1111,11 +1171,11 @@
         <v>46039.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-8.12561</v>
+        <v>-6.8</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
@@ -1132,11 +1192,11 @@
         <v>46039.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-4.81333</v>
+        <v>-9.99</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D30" s="3" t="n">
@@ -1153,7 +1213,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-6.8</v>
+        <v>-7</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1234,7 @@
         <v>46039.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.8</v>
+        <v>-5.51011</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1255,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>0.7</v>
+        <v>-5.01</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1276,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>18.88451</v>
+        <v>0.7</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1297,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>3.18383</v>
+        <v>3.23527</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1318,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.31005</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1339,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-2.94054</v>
+        <v>-3.09373</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1360,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.88187</v>
+        <v>0.00013</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1381,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.95405</v>
+        <v>0</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1402,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>8.24929</v>
+        <v>17.20923</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1423,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>30.48176</v>
+        <v>57.16514</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1375,7 +1435,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1384,7 +1444,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>30.57917</v>
+        <v>57.18142</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1396,7 +1456,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1465,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>9.88462</v>
+        <v>57.16514</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1417,7 +1477,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1426,7 +1486,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>9.816660000000001</v>
+        <v>46.73943</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1438,7 +1498,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1507,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>22.66264</v>
+        <v>46.80565</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1459,7 +1519,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1528,7 @@
         <v>46039.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>36.06045</v>
+        <v>36.05843</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1480,7 +1540,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1549,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.06004</v>
+        <v>47.35317</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1542,6 +1602,1014 @@
         <v>46039</v>
       </c>
       <c r="E49" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>46040</v>
+      </c>
+      <c r="B50" t="n">
+        <v>47.81285</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>46040.02083333334</v>
+      </c>
+      <c r="B51" t="n">
+        <v>36.06032</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>46040.04166666666</v>
+      </c>
+      <c r="B52" t="n">
+        <v>56.98</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>46040.0625</v>
+      </c>
+      <c r="B53" t="n">
+        <v>56.98</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>46040.08333333334</v>
+      </c>
+      <c r="B54" t="n">
+        <v>56.97996</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>46040.10416666666</v>
+      </c>
+      <c r="B55" t="n">
+        <v>57.0602</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>46040.125</v>
+      </c>
+      <c r="B56" t="n">
+        <v>57.06021</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>46040.14583333334</v>
+      </c>
+      <c r="B57" t="n">
+        <v>57.06022</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>46040.16666666666</v>
+      </c>
+      <c r="B58" t="n">
+        <v>57.06022</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>46040.1875</v>
+      </c>
+      <c r="B59" t="n">
+        <v>57.06003</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>46040.20833333334</v>
+      </c>
+      <c r="B60" t="n">
+        <v>57.06003</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>46040.22916666666</v>
+      </c>
+      <c r="B61" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>46040.25</v>
+      </c>
+      <c r="B62" t="n">
+        <v>57.06003</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>46040.27083333334</v>
+      </c>
+      <c r="B63" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>46040.29166666666</v>
+      </c>
+      <c r="B64" t="n">
+        <v>24.71692</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>46040.3125</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>46040.33333333334</v>
+      </c>
+      <c r="B66" t="n">
+        <v>-4.58324</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>46040.35416666666</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.62395</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>46040.375</v>
+      </c>
+      <c r="B68" t="n">
+        <v>2.19121</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>46040.39583333334</v>
+      </c>
+      <c r="B69" t="n">
+        <v>-0.9231200000000001</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>46040.41666666666</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-0.9403</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>46040.4375</v>
+      </c>
+      <c r="B71" t="n">
+        <v>-5.4861</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>46040.45833333334</v>
+      </c>
+      <c r="B72" t="n">
+        <v>-5.51</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>46040.47916666666</v>
+      </c>
+      <c r="B73" t="n">
+        <v>-5.77472</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D73" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>46040.5</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-5.63201</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>46040.52083333334</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-6.30444</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>46040.54166666666</v>
+      </c>
+      <c r="B76" t="n">
+        <v>-7</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D76" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>46040.5625</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-8.452769999999999</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>46040.58333333334</v>
+      </c>
+      <c r="B78" t="n">
+        <v>-10</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D78" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>46040.60416666666</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-14</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D79" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>46040.625</v>
+      </c>
+      <c r="B80" t="n">
+        <v>-19.76767</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>46040.64583333334</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-20.57529</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>46040.66666666666</v>
+      </c>
+      <c r="B82" t="n">
+        <v>-14.35069</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D82" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>46040.6875</v>
+      </c>
+      <c r="B83" t="n">
+        <v>-14.23795</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>46040.70833333334</v>
+      </c>
+      <c r="B84" t="n">
+        <v>-12.30534</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>46040.72916666666</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-6.59911</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>46040.75</v>
+      </c>
+      <c r="B86" t="n">
+        <v>1.94062</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>46040.77083333334</v>
+      </c>
+      <c r="B87" t="n">
+        <v>34.32564</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D87" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>46040.79166666666</v>
+      </c>
+      <c r="B88" t="n">
+        <v>36.0601</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>46040.8125</v>
+      </c>
+      <c r="B89" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>46040.83333333334</v>
+      </c>
+      <c r="B90" t="n">
+        <v>43.32062</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D90" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>46040.85416666666</v>
+      </c>
+      <c r="B91" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>46040.875</v>
+      </c>
+      <c r="B92" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>46040.89583333334</v>
+      </c>
+      <c r="B93" t="n">
+        <v>36.0601</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>46040.91666666666</v>
+      </c>
+      <c r="B94" t="n">
+        <v>47.10825</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>46040.9375</v>
+      </c>
+      <c r="B95" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>46040.95833333334</v>
+      </c>
+      <c r="B96" t="n">
+        <v>36.0601</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D96" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>46040.97916666666</v>
+      </c>
+      <c r="B97" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E97" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>

</xml_diff>

<commit_message>
Update latest output (run 61)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -527,18 +527,18 @@
         <v>26.46</v>
       </c>
       <c r="E4" t="n">
-        <v>216.116355</v>
+        <v>194.72505975</v>
       </c>
       <c r="F4" t="n">
-        <v>8.167662698412698</v>
+        <v>7.359223724489796</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46040.3125</v>
+        <v>46040.29166666666</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>46040.8125</v>
+        <v>46040.79166666666</v>
       </c>
       <c r="C5" t="n">
         <v>12</v>
@@ -547,10 +547,10 @@
         <v>45.36</v>
       </c>
       <c r="E5" t="n">
-        <v>-6.772457249999995</v>
+        <v>95.10621899999998</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.149304613095238</v>
+        <v>2.096697949735449</v>
       </c>
     </row>
   </sheetData>
@@ -1213,7 +1213,7 @@
         <v>46039.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-9.99</v>
+        <v>36.06031</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1234,7 +1234,7 @@
         <v>46039.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.8</v>
+        <v>36.06033</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1255,11 +1255,11 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>22.07</v>
+        <v>-9.99</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D33" s="3" t="n">
@@ -1276,11 +1276,11 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>36.06036</v>
+        <v>-6</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D34" s="3" t="n">
@@ -1297,7 +1297,7 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>25.0354</v>
+        <v>2.55649</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>4.53593</v>
+        <v>-1.77936</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.24301</v>
+        <v>-0.289</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1360,7 +1360,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>0.00014</v>
+        <v>-2.33161</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>0.00014</v>
+        <v>-2.08153</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>17.07182</v>
+        <v>13.59536</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>57.18142</v>
+        <v>46.95824</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>57.18142</v>
+        <v>47.19413</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>46.60383</v>
+        <v>47.00942</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>46.91075</v>
+        <v>46.87831</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>47.4748</v>
+        <v>47.87261</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.83</v>
+        <v>56.78</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46040</v>
       </c>
       <c r="B50" t="n">
-        <v>47.78559</v>
+        <v>48.09522</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46040.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.06016</v>
+        <v>56.98</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         <v>46040.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>57.0602</v>
+        <v>56.97996</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>36.0595</v>
+        <v>24.30295</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
         <v>46040.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>35.87994</v>
+        <v>0.7</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
         <v>46040.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.63134</v>
+        <v>5.738</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.7</v>
+        <v>27.1824</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46040.375</v>
       </c>
       <c r="B68" t="n">
-        <v>0.61554</v>
+        <v>14.8839</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>0.59266</v>
+        <v>0.7</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>8.38785</v>
+        <v>25.82334</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>27.10585</v>
+        <v>22.07</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>0.7</v>
+        <v>22.07</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>0.66306</v>
+        <v>25.80412</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46040.5</v>
       </c>
       <c r="B74" t="n">
-        <v>0</v>
+        <v>22.07</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-5.21817</v>
+        <v>-0.93264</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-5.43091</v>
+        <v>-5.45227</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-5.57994</v>
+        <v>-5.5808</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46040.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-13.5</v>
+        <v>-12.01</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-12.01</v>
+        <v>-11.01</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-7.44788</v>
+        <v>-7.17238</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-8.045170000000001</v>
+        <v>-8.324020000000001</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-7.66355</v>
+        <v>-6.1466</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-6.12644</v>
+        <v>-6.5703</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46040.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-5.85772</v>
+        <v>-3.10096</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>22.15733</v>
+        <v>36.0601</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>44.02345</v>
+        <v>45.86636</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>47.60158</v>
+        <v>54.96565</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>46.82896</v>
+        <v>47.16323</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46040.875</v>
       </c>
       <c r="B92" t="n">
-        <v>46.12397</v>
+        <v>46.5469</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>55.31303</v>
+        <v>55.29915</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 62)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,82 +475,62 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46039.02083333334</v>
+        <v>46039.29166666666</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46039.1875</v>
+        <v>46039.47916666666</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="D2" t="n">
-        <v>15.12</v>
+        <v>17.01</v>
       </c>
       <c r="E2" t="n">
-        <v>347.06108775</v>
+        <v>278.8351215</v>
       </c>
       <c r="F2" t="n">
-        <v>22.95377564484127</v>
+        <v>16.3924233686067</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46039.29166666666</v>
+        <v>46039.52083333334</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46039.5</v>
+        <v>46040</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>11.5</v>
       </c>
       <c r="D3" t="n">
-        <v>18.9</v>
+        <v>43.47</v>
       </c>
       <c r="E3" t="n">
-        <v>313.99407</v>
+        <v>537.543513</v>
       </c>
       <c r="F3" t="n">
-        <v>16.61344285714286</v>
+        <v>12.36585031055901</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46039.52083333334</v>
+        <v>46040.29166666666</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46039.8125</v>
+        <v>46040.79166666666</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>26.46</v>
+        <v>45.36</v>
       </c>
       <c r="E4" t="n">
-        <v>194.72505975</v>
+        <v>25.08997725</v>
       </c>
       <c r="F4" t="n">
-        <v>7.359223724489796</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>46040.29166666666</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>46040.79166666666</v>
-      </c>
-      <c r="C5" t="n">
-        <v>12</v>
-      </c>
-      <c r="D5" t="n">
-        <v>45.36</v>
-      </c>
-      <c r="E5" t="n">
-        <v>95.10621899999998</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2.096697949735449</v>
+        <v>0.553130009920635</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +617,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -658,7 +638,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -679,7 +659,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -700,7 +680,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -721,7 +701,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -742,7 +722,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -763,7 +743,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -784,7 +764,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1079,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1255,7 +1235,7 @@
         <v>46039.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-9.99</v>
+        <v>36.06038</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1276,7 +1256,7 @@
         <v>46039.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-6</v>
+        <v>36.06036</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1297,11 +1277,11 @@
         <v>46039.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>2.55649</v>
+        <v>-7.37172</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D35" s="3" t="n">
@@ -1318,11 +1298,11 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-1.77936</v>
+        <v>-6.48811</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D36" s="3" t="n">
@@ -1339,7 +1319,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.289</v>
+        <v>-2.93457</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1360,7 +1340,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.33161</v>
+        <v>-2.81393</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1361,7 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.08153</v>
+        <v>-2.96975</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1382,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>13.59536</v>
+        <v>2.29449</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1403,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>46.95824</v>
+        <v>13.64807</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1435,7 +1415,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1444,7 +1424,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>47.19413</v>
+        <v>33.18906</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1456,7 +1436,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1465,7 +1445,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>57.18142</v>
+        <v>36.2</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1477,7 +1457,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1466,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>47.00942</v>
+        <v>30.11497</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1498,7 +1478,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1487,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>46.87831</v>
+        <v>36.0601</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1519,7 +1499,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1508,7 @@
         <v>46039.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>36.06045</v>
+        <v>36.05843</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1540,7 +1520,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1529,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>47.87261</v>
+        <v>36.06041</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1561,7 +1541,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1570,7 +1550,7 @@
         <v>46039.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>56.98</v>
+        <v>36.06043</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1582,7 +1562,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1571,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.78</v>
+        <v>36.0604</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1603,7 +1583,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1592,7 @@
         <v>46040</v>
       </c>
       <c r="B50" t="n">
-        <v>48.09522</v>
+        <v>36.06038</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1654,7 +1634,7 @@
         <v>46040.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>56.98</v>
+        <v>36.0603</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1675,7 +1655,7 @@
         <v>46040.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>56.98</v>
+        <v>36.06028</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1696,7 +1676,7 @@
         <v>46040.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>56.97996</v>
+        <v>36.06027</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1717,7 +1697,7 @@
         <v>46040.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>56.97996</v>
+        <v>36.06026</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1738,7 +1718,7 @@
         <v>46040.125</v>
       </c>
       <c r="B56" t="n">
-        <v>57.06021</v>
+        <v>56.97996</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1759,7 +1739,7 @@
         <v>46040.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>57.06022</v>
+        <v>56.98</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1760,7 @@
         <v>46040.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>57.06022</v>
+        <v>56.98</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1781,7 @@
         <v>46040.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1864,7 +1844,7 @@
         <v>46040.25</v>
       </c>
       <c r="B62" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1906,7 +1886,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>24.30295</v>
+        <v>36.0595</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1927,7 +1907,7 @@
         <v>46040.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>0.7</v>
+        <v>23.49478</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1948,7 +1928,7 @@
         <v>46040.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>5.738</v>
+        <v>-0.90707</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1969,7 +1949,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>27.1824</v>
+        <v>0.7</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1990,7 +1970,7 @@
         <v>46040.375</v>
       </c>
       <c r="B68" t="n">
-        <v>14.8839</v>
+        <v>0.7</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +1991,7 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +2012,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>25.82334</v>
+        <v>0.51</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2033,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>22.07</v>
+        <v>35.88</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2054,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>22.07</v>
+        <v>0.66409</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2075,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>25.80412</v>
+        <v>-0.97534</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2096,7 @@
         <v>46040.5</v>
       </c>
       <c r="B74" t="n">
-        <v>22.07</v>
+        <v>0.0003</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2117,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.93264</v>
+        <v>-0.92843</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2138,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-5.45227</v>
+        <v>-5.51</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2159,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-5.5808</v>
+        <v>-5.51</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2180,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-13.5</v>
+        <v>-6.8</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2201,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-14</v>
+        <v>-7</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2222,7 @@
         <v>46040.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-12.01</v>
+        <v>-8.06785</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2243,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-11.01</v>
+        <v>-6.77128</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2264,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-7.17238</v>
+        <v>-7.21403</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2285,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-8.324020000000001</v>
+        <v>-7.00224</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2306,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-6.1466</v>
+        <v>-6.52915</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2327,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-6.5703</v>
+        <v>-6.51864</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2348,7 @@
         <v>46040.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-3.10096</v>
+        <v>-3.05165</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2369,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>0.0001</v>
+        <v>0.00032</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2431,7 +2411,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>45.86636</v>
+        <v>46.21963</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2432,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>54.96565</v>
+        <v>54.93629</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2453,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>47.16323</v>
+        <v>55.52267</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2474,7 @@
         <v>46040.875</v>
       </c>
       <c r="B92" t="n">
-        <v>46.5469</v>
+        <v>46.9203</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2536,7 +2516,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>55.29915</v>
+        <v>47.36052</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 64)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,39 +478,59 @@
         <v>46039.29166666666</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46039.95833333334</v>
+        <v>46039.8125</v>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>12.5</v>
       </c>
       <c r="D2" t="n">
-        <v>60.48</v>
+        <v>47.25</v>
       </c>
       <c r="E2" t="n">
-        <v>838.15197375</v>
+        <v>652.71611925</v>
       </c>
       <c r="F2" t="n">
-        <v>13.85833289930556</v>
+        <v>13.81409776190476</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.29166666666</v>
+        <v>46039.85416666666</v>
       </c>
       <c r="B3" s="2" t="n">
+        <v>46040.02083333334</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15.12</v>
+      </c>
+      <c r="E3" t="n">
+        <v>296.949861</v>
+      </c>
+      <c r="F3" t="n">
+        <v>19.63954107142857</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>46040.3125</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>46040.79166666666</v>
       </c>
-      <c r="C3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D3" t="n">
-        <v>45.36</v>
-      </c>
-      <c r="E3" t="n">
-        <v>19.22750700000002</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.423886838624339</v>
+      <c r="C4" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>43.47</v>
+      </c>
+      <c r="E4" t="n">
+        <v>71.07485774999998</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.635032384403036</v>
       </c>
     </row>
   </sheetData>
@@ -1278,7 +1298,7 @@
         <v>46039.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-10.44271</v>
+        <v>-0.57248</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1299,7 +1319,7 @@
         <v>46039.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-3.94707</v>
+        <v>-2.97056</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1320,7 +1340,7 @@
         <v>46039.75</v>
       </c>
       <c r="B38" t="n">
-        <v>-2.79778</v>
+        <v>-2.80872</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,11 +1361,11 @@
         <v>46039.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>-2.95059</v>
+        <v>-3.69268</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
@@ -1362,11 +1382,11 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>9.143090000000001</v>
+        <v>17.74626</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1383,7 +1403,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>30.21113</v>
+        <v>57.18142</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1395,7 +1415,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1404,7 +1424,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>33.16531</v>
+        <v>56.98</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1416,7 +1436,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1445,7 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>33.21788</v>
+        <v>46.39479</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1446,7 +1466,7 @@
         <v>46039.875</v>
       </c>
       <c r="B44" t="n">
-        <v>9.992010000000001</v>
+        <v>30.53091</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1467,7 +1487,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>30.18307</v>
+        <v>36.2</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1488,7 +1508,7 @@
         <v>46039.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>36.05728</v>
+        <v>36.05933</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1509,7 +1529,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>36.06082</v>
+        <v>36.2</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1530,7 +1550,7 @@
         <v>46039.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>36.2</v>
+        <v>47.05815</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1542,7 +1562,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1571,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>47.40282</v>
+        <v>36.0604</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1563,7 +1583,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1584,7 +1604,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1614,7 +1634,7 @@
         <v>46040.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>40.54</v>
+        <v>31.02048</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1635,7 +1655,7 @@
         <v>46040.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>36.06028</v>
+        <v>36.2</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1698,7 +1718,7 @@
         <v>46040.125</v>
       </c>
       <c r="B56" t="n">
-        <v>37.56308</v>
+        <v>36.2</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1719,7 +1739,7 @@
         <v>46040.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>56.98</v>
+        <v>56.97996</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1740,7 +1760,7 @@
         <v>46040.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>56.98</v>
+        <v>50.31057</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1782,7 +1802,7 @@
         <v>46040.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1803,7 +1823,7 @@
         <v>46040.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1824,7 +1844,7 @@
         <v>46040.25</v>
       </c>
       <c r="B62" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1866,7 +1886,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>30.95328</v>
+        <v>36.0595</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1878,7 +1898,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1907,7 @@
         <v>46040.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>0.9876200000000001</v>
+        <v>28.67846</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1908,7 +1928,7 @@
         <v>46040.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>-5.51</v>
+        <v>0.62605</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1929,7 +1949,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.009509999999999999</v>
+        <v>19.29447</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1992,7 +2012,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>0.00962</v>
+        <v>26.41845</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2013,7 +2033,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>36.06</v>
+        <v>22.07</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2034,7 +2054,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>26.16534</v>
+        <v>0.7</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2055,7 +2075,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>0.009809999999999999</v>
+        <v>20.59504</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2076,7 +2096,7 @@
         <v>46040.5</v>
       </c>
       <c r="B74" t="n">
-        <v>0.009390000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2097,7 +2117,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.94498</v>
+        <v>0.64597</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2118,7 +2138,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-5.29877</v>
+        <v>0.7</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2139,7 +2159,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-5.51</v>
+        <v>0.00025</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2160,7 +2180,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-6.8</v>
+        <v>-4.9548</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2181,7 +2201,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-6.55247</v>
+        <v>-6.70389</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2202,7 +2222,7 @@
         <v>46040.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-7.49179</v>
+        <v>-5.41349</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2223,7 +2243,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-6.77161</v>
+        <v>-6.85668</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2244,7 +2264,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-7.12033</v>
+        <v>-6.73561</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2265,7 +2285,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-6.87758</v>
+        <v>-6.89381</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2286,7 +2306,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-6.52931</v>
+        <v>-7.08241</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2307,7 +2327,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-6.54534</v>
+        <v>-1.8149</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2328,7 +2348,7 @@
         <v>46040.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-3.05181</v>
+        <v>-1.41518</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2349,7 +2369,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>0.00032</v>
+        <v>0.00975</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2391,7 +2411,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>46.21429</v>
+        <v>46.5704</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2412,7 +2432,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>46.00149</v>
+        <v>56.98</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2433,7 +2453,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>55.51195</v>
+        <v>55.47778</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2454,7 +2474,7 @@
         <v>46040.875</v>
       </c>
       <c r="B92" t="n">
-        <v>46.86218</v>
+        <v>46.8495</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2496,7 +2516,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>56.05084</v>
+        <v>56.0398</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 66)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -515,10 +515,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46039.52083333334</v>
+        <v>46039.54166666666</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46039.8125</v>
+        <v>46039.83333333334</v>
       </c>
       <c r="C4" t="n">
         <v>7</v>
@@ -527,18 +527,18 @@
         <v>26.46</v>
       </c>
       <c r="E4" t="n">
-        <v>301.5587835000001</v>
+        <v>260.3643315</v>
       </c>
       <c r="F4" t="n">
-        <v>11.39677942176871</v>
+        <v>9.839921825396827</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46040.29166666666</v>
+        <v>46040.3125</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>46040.79166666666</v>
+        <v>46040.8125</v>
       </c>
       <c r="C5" t="n">
         <v>12</v>
@@ -547,10 +547,10 @@
         <v>45.36</v>
       </c>
       <c r="E5" t="n">
-        <v>149.74963575</v>
+        <v>-29.91509624999999</v>
       </c>
       <c r="F5" t="n">
-        <v>3.301358812830688</v>
+        <v>-0.6595038855820103</v>
       </c>
     </row>
   </sheetData>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1402,7 +1402,7 @@
         <v>46039.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>14.77494</v>
+        <v>0.01082</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>46039.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>57.18142</v>
+        <v>8.57385</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1444,7 +1444,7 @@
         <v>46039.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1465,11 +1465,11 @@
         <v>46039.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1490,7 +1490,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1507,7 +1507,7 @@
         <v>46039.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>46.39404</v>
+        <v>56.98</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>46039.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>47.10776</v>
+        <v>57.06004</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46039.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>40.54</v>
+        <v>36.2</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46040</v>
       </c>
       <c r="B50" t="n">
-        <v>36.06038</v>
+        <v>36.2</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46040.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>31.24649</v>
+        <v>36.0603</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
         <v>46040.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>36.2</v>
+        <v>52.28671</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
         <v>46040.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>36.06027</v>
+        <v>36.2</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         <v>46040.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>36.06026</v>
+        <v>36.2</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1738,7 +1738,7 @@
         <v>46040.125</v>
       </c>
       <c r="B56" t="n">
-        <v>36.2</v>
+        <v>56.97996</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46040.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>36.2</v>
+        <v>56.98</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46040.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>24.28595</v>
+        <v>36.0595</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
         <v>46040.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>28.49947</v>
+        <v>27.51631</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>1.82692</v>
+        <v>21.8653</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46040.375</v>
       </c>
       <c r="B68" t="n">
-        <v>0.7</v>
+        <v>-0.9349499999999999</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>0.7</v>
+        <v>-5.01</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>35.88</v>
+        <v>-3.6481</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>35.88</v>
+        <v>0.51</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>26.63005</v>
+        <v>0.7</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>22.07</v>
+        <v>0.7</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46040.5</v>
       </c>
       <c r="B74" t="n">
-        <v>0.7</v>
+        <v>-5.51</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>0.65374</v>
+        <v>-0.89546</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>0.51</v>
+        <v>-5.51</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>0</v>
+        <v>-5.59641</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-4.42723</v>
+        <v>-9.99</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-0.83768</v>
+        <v>-10.81131</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46040.625</v>
       </c>
       <c r="B80" t="n">
-        <v>0.00025</v>
+        <v>-13.30111</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.32843</v>
+        <v>-11.01</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-1.79043</v>
+        <v>-7.35773</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-6.5608</v>
+        <v>-7.29212</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-6.56595</v>
+        <v>-6.37938</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>-3.90305</v>
+        <v>-0.62352</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46040.75</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.84376</v>
+        <v>-1.38933</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>0.00032</v>
+        <v>0.00023</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>36.0601</v>
+        <v>12.77543</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>46.19147</v>
+        <v>44.0223</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>46.26191</v>
+        <v>45.92752</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>55.49501</v>
+        <v>45.17477</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46040.875</v>
       </c>
       <c r="B92" t="n">
-        <v>46.85269</v>
+        <v>46.84454</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>55.27992</v>
+        <v>56.03123</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 71)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -475,42 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.29166666666</v>
+        <v>46040</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.79166666666</v>
+        <v>46040.16666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>45.36</v>
+        <v>15.12</v>
       </c>
       <c r="E2" t="n">
-        <v>-56.21536049999997</v>
+        <v>363.42217275</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.239315707671957</v>
+        <v>24.03585798611111</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.83333333334</v>
+        <v>46040.29166666666</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46041</v>
+        <v>46040.79166666666</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>15.12</v>
+        <v>45.36</v>
       </c>
       <c r="E3" t="n">
-        <v>371.6685765</v>
+        <v>-62.45913375000001</v>
       </c>
       <c r="F3" t="n">
-        <v>24.58125505952381</v>
+        <v>-1.376965029761905</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,10 +561,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.02083333334</v>
+        <v>46040</v>
       </c>
       <c r="B2" t="n">
-        <v>36.06032</v>
+        <v>56.98</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -576,16 +576,16 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.04166666666</v>
+        <v>46040.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>35.88</v>
+        <v>36.2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -597,20 +597,20 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46040.0625</v>
+        <v>46040.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>36.2</v>
+        <v>36.0603</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
@@ -618,20 +618,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46040.08333333334</v>
+        <v>46040.0625</v>
       </c>
       <c r="B5" t="n">
-        <v>57.06019</v>
+        <v>36.2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
@@ -639,20 +639,20 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46040.10416666666</v>
+        <v>46040.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>57.0602</v>
+        <v>36.2</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
@@ -660,16 +660,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46040.125</v>
+        <v>46040.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>57.06021</v>
+        <v>56.97996</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -681,16 +681,16 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46040.14583333334</v>
+        <v>46040.125</v>
       </c>
       <c r="B8" t="n">
-        <v>57.06022</v>
+        <v>57.06021</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -702,13 +702,13 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46040.16666666666</v>
+        <v>46040.14583333334</v>
       </c>
       <c r="B9" t="n">
         <v>57.06022</v>
@@ -723,16 +723,16 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46040.1875</v>
+        <v>46040.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>57.06003</v>
+        <v>57.06022</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -750,7 +750,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46040.20833333334</v>
+        <v>46040.1875</v>
       </c>
       <c r="B11" t="n">
         <v>57.06003</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46040.22916666666</v>
+        <v>46040.20833333334</v>
       </c>
       <c r="B12" t="n">
         <v>57.06003</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46040.25</v>
+        <v>46040.22916666666</v>
       </c>
       <c r="B13" t="n">
         <v>57.06003</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46040.27083333334</v>
+        <v>46040.25</v>
       </c>
       <c r="B14" t="n">
-        <v>36.06</v>
+        <v>57.06003</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -834,10 +834,10 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46040.29166666666</v>
+        <v>46040.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>36.0595</v>
+        <v>51.00032</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -849,16 +849,16 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46040.3125</v>
+        <v>46040.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>11.56192</v>
+        <v>24.52381</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -876,10 +876,10 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46040.33333333334</v>
+        <v>46040.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>-5.01</v>
+        <v>0.7</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -897,10 +897,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46040.35416666666</v>
+        <v>46040.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5954700000000001</v>
+        <v>-5.51</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -918,10 +918,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46040.375</v>
+        <v>46040.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>0.009549999999999999</v>
+        <v>0.6145699999999999</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -939,10 +939,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46040.39583333334</v>
+        <v>46040.375</v>
       </c>
       <c r="B20" t="n">
-        <v>-3.6481</v>
+        <v>0.00961</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -960,10 +960,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46040.41666666666</v>
+        <v>46040.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-4.55365</v>
+        <v>-1.74343</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -981,7 +981,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46040.4375</v>
+        <v>46040.41666666666</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -1002,10 +1002,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46040.45833333334</v>
+        <v>46040.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-5.51</v>
+        <v>0.7</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46040.47916666666</v>
+        <v>46040.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.31495</v>
+        <v>0</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1044,10 +1044,10 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46040.5</v>
+        <v>46040.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-4.50424</v>
+        <v>-0.91939</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46040.52083333334</v>
+        <v>46040.5</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>-0.90235</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>46040.54166666666</v>
+        <v>46040.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-5.51011</v>
+        <v>0</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1107,10 +1107,10 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>46040.5625</v>
+        <v>46040.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-6.8</v>
+        <v>-5.51011</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1128,10 +1128,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>46040.58333333334</v>
+        <v>46040.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-14</v>
+        <v>-6.8</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>46040.60416666666</v>
+        <v>46040.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-23.5</v>
+        <v>-14</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1170,10 +1170,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>46040.625</v>
+        <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-14</v>
+        <v>-23.5</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>46040.64583333334</v>
+        <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-14</v>
+        <v>-14.7657</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>46040.66666666666</v>
+        <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-7.1156</v>
+        <v>-14</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1233,10 +1233,10 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>46040.6875</v>
+        <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-6.51112</v>
+        <v>-7.15426</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>46040.70833333334</v>
+        <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-6</v>
+        <v>-6.48482</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1275,10 +1275,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>46040.72916666666</v>
+        <v>46040.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>0.63476</v>
+        <v>-6</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1296,10 +1296,10 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>46040.75</v>
+        <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>3.95694</v>
+        <v>0.66143</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>46040.77083333334</v>
+        <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>11.50285</v>
+        <v>3.98333</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1338,10 +1338,10 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>46040.79166666666</v>
+        <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>36.2</v>
+        <v>12.03666</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1353,16 +1353,16 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>46040.8125</v>
+        <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>53.65862</v>
+        <v>36.2</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>46040.83333333334</v>
+        <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
         <v>56.98</v>
@@ -1395,16 +1395,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>46040.85416666666</v>
+        <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1416,13 +1416,13 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>46040.875</v>
+        <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
         <v>56.98</v>
@@ -1437,16 +1437,16 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>46040.89583333334</v>
+        <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>45.73237</v>
+        <v>56.98</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1458,16 +1458,16 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>46040.91666666666</v>
+        <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>56.34597</v>
+        <v>46.20513</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1479,16 +1479,16 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>46040.9375</v>
+        <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>36.0601</v>
+        <v>56.34431</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1500,13 +1500,13 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46040.95833333334</v>
+        <v>46040.9375</v>
       </c>
       <c r="B47" t="n">
         <v>36.0601</v>
@@ -1521,28 +1521,49 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
+        <v>46040.95833333334</v>
+      </c>
+      <c r="B48" t="n">
+        <v>36.0601</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
         <v>46040.97916666666</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B49" t="n">
         <v>36.06</v>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>forecast</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="n">
-        <v>46040</v>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>ON</t>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>forecast</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>46040</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>OFF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update latest output (run 73)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>-27.44120924999999</v>
+        <v>-33.60198075</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.6049649305555554</v>
+        <v>-0.7407844080687831</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>379.85008425</v>
+        <v>372.94961925</v>
       </c>
       <c r="F3" t="n">
-        <v>25.12236006944445</v>
+        <v>24.66598010912698</v>
       </c>
     </row>
   </sheetData>
@@ -669,7 +669,7 @@
         <v>46040.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>36.2</v>
+        <v>56.97996</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -690,7 +690,7 @@
         <v>46040.125</v>
       </c>
       <c r="B8" t="n">
-        <v>56.97996</v>
+        <v>57.06021</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -711,11 +711,11 @@
         <v>46040.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>56.98</v>
+        <v>36.2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
@@ -732,11 +732,11 @@
         <v>46040.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>57.06022</v>
+        <v>56.98</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
@@ -753,7 +753,7 @@
         <v>46040.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
         <v>46040.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>57.06003</v>
+        <v>57.1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -837,7 +837,7 @@
         <v>46040.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>50.98493</v>
+        <v>50.95183</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -858,7 +858,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>32.29746</v>
+        <v>24.36057</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -879,7 +879,7 @@
         <v>46040.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>11.61977</v>
+        <v>0.7</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -900,7 +900,7 @@
         <v>46040.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>-5.51</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -921,7 +921,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>2.80927</v>
+        <v>4.14872</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -963,7 +963,7 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-1.74343</v>
+        <v>-3.6481</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.81333</v>
+        <v>-1.5776</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>0.51</v>
+        <v>11.7995</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1026,7 +1026,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>0.62873</v>
+        <v>0.00976</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1047,7 +1047,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-4.81902</v>
+        <v>-0.93531</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.89155</v>
+        <v>0.00902</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1110,7 +1110,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-5.69904</v>
+        <v>-4.49679</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1152,7 +1152,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-9.99</v>
+        <v>-7</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1173,7 +1173,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-20.40712</v>
+        <v>-20.55932</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1194,7 +1194,7 @@
         <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-12.43825</v>
+        <v>-12.91239</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-12.01</v>
+        <v>-13.5</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-6.71741</v>
+        <v>-7.10129</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-6.51053</v>
+        <v>-6.44164</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1299,7 +1299,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>0.66214</v>
+        <v>0.66476</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1320,7 +1320,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>3.98497</v>
+        <v>3.98635</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1341,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>17.67251</v>
+        <v>15.83019</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>45.74509</v>
+        <v>41.35282</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1404,7 +1404,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>64.8901</v>
+        <v>57.3</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1425,7 +1425,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1467,7 +1467,7 @@
         <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>46.2146</v>
+        <v>46.20722</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1488,7 +1488,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.34493</v>
+        <v>56.54501</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 74)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,42 +475,22 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.29166666666</v>
+        <v>46040.14583333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.79166666666</v>
+        <v>46040.8125</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>45.36</v>
+        <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>-33.60198075</v>
+        <v>295.28607225</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.7407844080687831</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>46040.83333333334</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>46041</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E3" t="n">
-        <v>372.94961925</v>
-      </c>
-      <c r="F3" t="n">
-        <v>24.66598010912698</v>
+        <v>4.882375533234127</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +691,7 @@
         <v>46040.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>36.2</v>
+        <v>57.06022</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -723,7 +703,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -744,7 +724,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -753,11 +733,11 @@
         <v>46040.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>56.98</v>
+        <v>36.06</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
@@ -765,7 +745,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -774,11 +754,11 @@
         <v>46040.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>57.1</v>
+        <v>36.2</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
@@ -786,7 +766,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -795,7 +775,7 @@
         <v>46040.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -807,7 +787,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -828,7 +808,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -837,7 +817,7 @@
         <v>46040.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>50.95183</v>
+        <v>36.06</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -849,7 +829,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -858,7 +838,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>24.36057</v>
+        <v>8.058479999999999</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -921,7 +901,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>4.14872</v>
+        <v>0.009549999999999999</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -942,7 +922,7 @@
         <v>46040.375</v>
       </c>
       <c r="B20" t="n">
-        <v>0.51</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -963,7 +943,7 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-3.6481</v>
+        <v>-0.9066</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -984,7 +964,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.5776</v>
+        <v>-4.72132</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1005,7 +985,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>11.7995</v>
+        <v>0.66745</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1026,7 +1006,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>0.00976</v>
+        <v>0.7</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1047,7 +1027,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.93531</v>
+        <v>-0.93546</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1068,7 +1048,7 @@
         <v>46040.5</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>-4.77113</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1089,7 +1069,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>0.00902</v>
+        <v>-4.61593</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1110,7 +1090,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-4.49679</v>
+        <v>-5.51</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1131,7 +1111,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-6.8</v>
+        <v>-6.4985</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1152,7 +1132,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1173,7 +1153,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-20.55932</v>
+        <v>-20.71215</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1194,7 +1174,7 @@
         <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-12.91239</v>
+        <v>-11.45471</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1195,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-13.5</v>
+        <v>-11.01</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1216,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-7.10129</v>
+        <v>-7.05469</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1237,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-6.44164</v>
+        <v>-6.56987</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1299,7 +1279,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>0.66476</v>
+        <v>0.66377</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1320,7 +1300,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>3.98635</v>
+        <v>3.98566</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1321,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>15.83019</v>
+        <v>16.85794</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1362,7 +1342,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>41.35282</v>
+        <v>41.08477</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1374,7 +1354,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1383,7 +1363,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>56.98</v>
+        <v>57.08646</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1416,7 +1396,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1405,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>57.3</v>
+        <v>56.98</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1437,7 +1417,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1438,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1467,7 +1447,7 @@
         <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>46.20722</v>
+        <v>46.33506</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1479,7 +1459,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1468,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.54501</v>
+        <v>56.33763</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1500,7 +1480,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1501,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1542,7 +1522,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1543,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update latest output (run 75)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,22 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.14583333334</v>
+        <v>46040.29166666666</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.8125</v>
+        <v>46040.79166666666</v>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>60.48</v>
+        <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>295.28607225</v>
+        <v>-59.48107424999998</v>
       </c>
       <c r="F2" t="n">
-        <v>4.882375533234127</v>
+        <v>-1.311311160714285</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>46040.83333333334</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>46041</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15.12</v>
+      </c>
+      <c r="E3" t="n">
+        <v>370.4505674999999</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24.50069890873015</v>
       </c>
     </row>
   </sheetData>
@@ -703,7 +723,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -724,7 +744,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -733,7 +753,7 @@
         <v>46040.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>36.06</v>
+        <v>57.06003</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -745,7 +765,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -754,7 +774,7 @@
         <v>46040.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>36.2</v>
+        <v>57.06003</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -766,7 +786,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -775,11 +795,11 @@
         <v>46040.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>56.98</v>
+        <v>55.33101</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
@@ -787,7 +807,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -796,11 +816,11 @@
         <v>46040.25</v>
       </c>
       <c r="B14" t="n">
-        <v>57.06003</v>
+        <v>56.26125</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
@@ -808,7 +828,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -829,7 +849,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -838,7 +858,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>8.058479999999999</v>
+        <v>36.06</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -859,7 +879,7 @@
         <v>46040.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>0.7</v>
+        <v>0.61797</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +900,7 @@
         <v>46040.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>-5.51</v>
+        <v>-5.4274</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +921,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>0.009549999999999999</v>
+        <v>0</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +942,7 @@
         <v>46040.375</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>-4.66577</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +963,7 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.9066</v>
+        <v>-5.31676</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +984,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.72132</v>
+        <v>-3.6481</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -985,7 +1005,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>0.66745</v>
+        <v>0.64369</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1026,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>0.7</v>
+        <v>0.00976</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1047,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.93546</v>
+        <v>-4.66482</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1068,7 @@
         <v>46040.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-4.77113</v>
+        <v>0.00025</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,7 +1089,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-4.61593</v>
+        <v>-5.51</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1110,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-5.51</v>
+        <v>-5.36283</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1131,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-6.4985</v>
+        <v>-6.0715</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1152,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-10</v>
+        <v>-13.5</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1173,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-20.71215</v>
+        <v>-20.57961</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1194,7 @@
         <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-11.45471</v>
+        <v>-13.5</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1215,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-11.01</v>
+        <v>-11.52252</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1236,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-7.05469</v>
+        <v>-7.11948</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1257,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-6.56987</v>
+        <v>-6.60693</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1279,7 +1299,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>0.66377</v>
+        <v>0.31443</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1320,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>3.98566</v>
+        <v>3.98303</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1341,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>16.85794</v>
+        <v>16.86036</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1362,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>41.08477</v>
+        <v>40.99071</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1354,7 +1374,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1363,7 +1383,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>57.08646</v>
+        <v>53.66969</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1396,7 +1416,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1425,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1417,7 +1437,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1426,7 +1446,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>56.98</v>
+        <v>56.94617</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1438,7 +1458,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1467,7 @@
         <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>46.33506</v>
+        <v>43.56065</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1459,7 +1479,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1488,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.33763</v>
+        <v>56.66228</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1480,7 +1500,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1521,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1542,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1543,7 +1563,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update latest output (run 78)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,42 +475,62 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.29166666666</v>
+        <v>46040.27083333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.79166666666</v>
+        <v>46040.4375</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>45.36</v>
+        <v>15.12</v>
       </c>
       <c r="E2" t="n">
-        <v>-90.22366275</v>
+        <v>140.93824875</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.989057820767196</v>
+        <v>9.321312748015874</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
+        <v>46040.45833333334</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>46040.79166666666</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>30.24</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-13.20846150000001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-0.4367877480158732</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>46040.83333333334</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B4" s="2" t="n">
         <v>46041</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>15.12</v>
       </c>
-      <c r="E3" t="n">
-        <v>370.293807</v>
-      </c>
-      <c r="F3" t="n">
-        <v>24.49033115079365</v>
+      <c r="E4" t="n">
+        <v>333.5945925</v>
+      </c>
+      <c r="F4" t="n">
+        <v>22.06313442460317</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +869,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -858,7 +878,7 @@
         <v>46040.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>0.7</v>
+        <v>24.39469</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -900,7 +920,7 @@
         <v>46040.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>-4.34103</v>
+        <v>-5.51</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -921,11 +941,11 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>11.098</v>
+        <v>36.06</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
@@ -942,11 +962,11 @@
         <v>46040.375</v>
       </c>
       <c r="B20" t="n">
-        <v>0.51</v>
+        <v>20.88924</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
@@ -963,7 +983,7 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-4.61115</v>
+        <v>20.4213</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -984,7 +1004,7 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.90326</v>
+        <v>11.72682</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1005,7 +1025,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-4.83666</v>
+        <v>36.06</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1017,7 +1037,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1046,7 @@
         <v>46040.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-5.51</v>
+        <v>0.7</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1047,7 +1067,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-4.5561</v>
+        <v>0.02018</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1068,7 +1088,7 @@
         <v>46040.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-5.19013</v>
+        <v>0.7</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1089,7 +1109,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-5.01</v>
+        <v>0.7</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1110,7 +1130,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-5.51011</v>
+        <v>-0.9016999999999999</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1131,7 +1151,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-5.51011</v>
+        <v>-0.8791099999999999</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1152,7 +1172,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-7.01</v>
+        <v>-5.51011</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1173,7 +1193,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-12.08785</v>
+        <v>-5.1729</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1194,7 +1214,7 @@
         <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-14.70709</v>
+        <v>-6.13636</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1215,7 +1235,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-14</v>
+        <v>-7.49401</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1236,7 +1256,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-6.85852</v>
+        <v>-6.81821</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1257,7 +1277,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-7.29618</v>
+        <v>-6.44839</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1278,7 +1298,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-6</v>
+        <v>-6.4473</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1299,7 +1319,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>0.66345</v>
+        <v>4.93756</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1320,7 +1340,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>3.98398</v>
+        <v>6.89183</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1341,7 +1361,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>3.93567</v>
+        <v>18.31138</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1383,7 +1403,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>53.77198</v>
+        <v>36.90374</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1404,7 +1424,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>57.3</v>
+        <v>46.53487</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1425,7 +1445,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>56.04515</v>
+        <v>37.61157</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1446,7 +1466,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>56.98</v>
+        <v>56.94145</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1467,7 +1487,7 @@
         <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>45.37537</v>
+        <v>36.2</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1488,7 +1508,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>55.9078</v>
+        <v>56.68021</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 79)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,62 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.27083333334</v>
+        <v>46040.29166666666</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.4375</v>
+        <v>46040.79166666666</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>15.12</v>
+        <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>140.93824875</v>
+        <v>213.75222375</v>
       </c>
       <c r="F2" t="n">
-        <v>9.321312748015874</v>
+        <v>4.712350611772487</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.45833333334</v>
+        <v>46040.83333333334</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46040.79166666666</v>
+        <v>46041</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>30.24</v>
+        <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>-13.20846150000001</v>
+        <v>361.68226575</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.4367877480158732</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>46040.83333333334</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>46041</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E4" t="n">
-        <v>333.5945925</v>
-      </c>
-      <c r="F4" t="n">
-        <v>22.06313442460317</v>
+        <v>23.9207847718254</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +849,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -941,7 +921,7 @@
         <v>46040.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>36.06</v>
+        <v>0.009549999999999999</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -962,7 +942,7 @@
         <v>46040.375</v>
       </c>
       <c r="B20" t="n">
-        <v>20.88924</v>
+        <v>32.97732</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -983,11 +963,11 @@
         <v>46040.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>20.4213</v>
+        <v>35.88</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
@@ -1004,11 +984,11 @@
         <v>46040.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>11.72682</v>
+        <v>36.06</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
@@ -1025,7 +1005,7 @@
         <v>46040.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>36.06</v>
+        <v>34.45798</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1037,7 +1017,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1047,7 @@
         <v>46040.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>0.02018</v>
+        <v>0.7</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1088,7 +1068,7 @@
         <v>46040.5</v>
       </c>
       <c r="B26" t="n">
-        <v>0.7</v>
+        <v>25.09786</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1109,7 +1089,7 @@
         <v>46040.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>0.7</v>
+        <v>33.41567</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1130,7 +1110,7 @@
         <v>46040.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.9016999999999999</v>
+        <v>0.51</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1151,7 +1131,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.8791099999999999</v>
+        <v>0.01819</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1172,7 +1152,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-5.51011</v>
+        <v>-0.32596</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1193,7 +1173,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-5.1729</v>
+        <v>-4.22974</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1214,7 +1194,7 @@
         <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.13636</v>
+        <v>-4.23274</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1235,7 +1215,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-7.49401</v>
+        <v>-7.48187</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1256,7 +1236,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-6.81821</v>
+        <v>-2.81401</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,7 +1257,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-6.44839</v>
+        <v>-5.8994</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1298,7 +1278,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-6.4473</v>
+        <v>-5.79576</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1319,7 +1299,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>4.93756</v>
+        <v>5.18238</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1320,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>6.89183</v>
+        <v>6.98736</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1341,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>18.31138</v>
+        <v>18.62153</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1403,7 +1383,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>36.90374</v>
+        <v>55.05565</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1404,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>46.53487</v>
+        <v>56.72399</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1445,7 +1425,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>37.61157</v>
+        <v>46.34977</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1446,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>56.94145</v>
+        <v>56.98</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1487,7 +1467,7 @@
         <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>36.2</v>
+        <v>45.60231</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1508,7 +1488,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.68021</v>
+        <v>56.98</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1529,7 +1509,7 @@
         <v>46040.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>36.0601</v>
+        <v>36.2</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 82)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>51.02999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>60.30140025000001</v>
+        <v>100.65971175</v>
       </c>
       <c r="F2" t="n">
-        <v>1.181685288065844</v>
+        <v>1.972559509112287</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>20.79</v>
       </c>
       <c r="E3" t="n">
-        <v>450.2433195</v>
+        <v>451.2848925</v>
       </c>
       <c r="F3" t="n">
-        <v>21.65672532467532</v>
+        <v>21.70682503607504</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>34.02</v>
       </c>
       <c r="E4" t="n">
-        <v>-43.64514375000001</v>
+        <v>-2.813537999999978</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.282926036155203</v>
+        <v>-0.08270246913580183</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1151,7 @@
         <v>46040.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-5.58988</v>
+        <v>-7</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1172,7 +1172,7 @@
         <v>46040.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-9.99</v>
+        <v>-12.20552</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1193,7 +1193,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-9.99</v>
+        <v>-7.46266</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1214,11 +1214,11 @@
         <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-8.452769999999999</v>
+        <v>-6.8</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D32" s="3" t="n">
@@ -1235,11 +1235,11 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-7.62043</v>
+        <v>-6.32</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D33" s="3" t="n">
@@ -1256,7 +1256,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-6.32</v>
+        <v>-5.41</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,7 +1277,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-6.34762</v>
+        <v>-4.77891</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1298,7 +1298,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-5.95309</v>
+        <v>5.16051</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1319,7 +1319,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>4.94039</v>
+        <v>6.2382</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>6.91421</v>
+        <v>6.99021</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>12.15556</v>
+        <v>18.34255</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>27.49695</v>
+        <v>36.2</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>36.0601</v>
+        <v>45.74218</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>45.40186</v>
+        <v>49.42693</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>36.2</v>
+        <v>46.19026</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1508,7 +1508,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>46.4787</v>
+        <v>47.91617</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         <v>46041.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         <v>46041.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>56.98</v>
+        <v>56.78</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1697,7 +1697,7 @@
         <v>46041.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>48.84899</v>
+        <v>48.75983</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
         <v>46041.125</v>
       </c>
       <c r="B56" t="n">
-        <v>49.74012</v>
+        <v>49.44748</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1739,7 +1739,7 @@
         <v>46041.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>56.98</v>
+        <v>50.33883</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46041.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>57.06003</v>
+        <v>57.76254</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>58.32151</v>
+        <v>57.06003</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>69.20653</v>
+        <v>58.81169</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1844,7 +1844,7 @@
         <v>46041.25</v>
       </c>
       <c r="B62" t="n">
-        <v>72.94628</v>
+        <v>58.02194</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1886,7 +1886,7 @@
         <v>46041.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>30.36901</v>
+        <v>36.06</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         <v>46041.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>6.75696</v>
+        <v>36.06</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.7</v>
+        <v>5.16569</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>46041.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.64751</v>
+        <v>0.64744</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-6.05409</v>
+        <v>-5.50985</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46041.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-7.79943</v>
+        <v>-6.14712</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46041.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-6.97876</v>
+        <v>-7.02049</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-7.69821</v>
+        <v>-7.15517</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-6.90017</v>
+        <v>-7.67966</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46041.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-7.02264</v>
+        <v>-7.68692</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-6.94073</v>
+        <v>-7.23621</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-6.08034</v>
+        <v>-6.19058</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-5.95857</v>
+        <v>-6.35843</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-5.01</v>
+        <v>-6.06857</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-5.51</v>
+        <v>-5.72243</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46041.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-5.77494</v>
+        <v>-5.51</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46041.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-5.50985</v>
+        <v>-2.53338</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-2.52431</v>
+        <v>0</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-5.13343</v>
+        <v>-2.54896</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-2.63766</v>
+        <v>-2.40408</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>2.2195</v>
+        <v>4.79045</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46041.75</v>
       </c>
       <c r="B86" t="n">
-        <v>20.24437</v>
+        <v>20.78901</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>47.97146</v>
+        <v>54.66255</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>59.14369</v>
+        <v>57.85505</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>77.94</v>
+        <v>71.91437000000001</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>73.20007</v>
+        <v>68.63066999999999</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         <v>46041.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>66.89706</v>
+        <v>66.50706</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46041.875</v>
       </c>
       <c r="B92" t="n">
-        <v>67.11141000000001</v>
+        <v>63.83273</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>62.40577</v>
+        <v>61.9517</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>57.54921</v>
+        <v>58.95387</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 83)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -478,39 +478,39 @@
         <v>46040.27083333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.83333333334</v>
+        <v>46040.85416666666</v>
       </c>
       <c r="C2" t="n">
-        <v>13.5</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>51.02999999999999</v>
+        <v>52.91999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>100.65971175</v>
+        <v>149.216769</v>
       </c>
       <c r="F2" t="n">
-        <v>1.972559509112287</v>
+        <v>2.819666836734695</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.89583333334</v>
+        <v>46040.91666666666</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>46041.125</v>
       </c>
       <c r="C3" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>20.79</v>
+        <v>18.9</v>
       </c>
       <c r="E3" t="n">
-        <v>451.2848925</v>
+        <v>520.6762177499999</v>
       </c>
       <c r="F3" t="n">
-        <v>21.70682503607504</v>
+        <v>27.54900623015872</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>34.02</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.813537999999978</v>
+        <v>20.29469325000004</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.08270246913580183</v>
+        <v>0.5965518298059976</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1193,7 @@
         <v>46040.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-7.46266</v>
+        <v>-23.5</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1214,7 +1214,7 @@
         <v>46040.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.8</v>
+        <v>-14.53915</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1235,7 +1235,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-6.32</v>
+        <v>-11.93964</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1256,11 +1256,11 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-5.41</v>
+        <v>-5.43826</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D34" s="3" t="n">
@@ -1277,7 +1277,7 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-4.77891</v>
+        <v>-5.41</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1298,7 +1298,7 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>5.16051</v>
+        <v>8.2301</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1319,7 +1319,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>6.2382</v>
+        <v>9.78525</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>6.99021</v>
+        <v>14.2512</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>18.34255</v>
+        <v>29.00544</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>36.2</v>
+        <v>30.91231</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>45.74218</v>
+        <v>56.98</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>49.42693</v>
+        <v>49.36694</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>46.19026</v>
+        <v>56.98</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>36.0601</v>
+        <v>56.98</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1508,7 +1508,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>47.91617</v>
+        <v>56.98</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1529,7 +1529,7 @@
         <v>46040.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>36.0601</v>
+        <v>50.56345</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
         <v>46040.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>36.06</v>
+        <v>49.15555</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1592,7 +1592,7 @@
         <v>46041</v>
       </c>
       <c r="B50" t="n">
-        <v>36.06</v>
+        <v>56.20781</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         <v>46041.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>36.06</v>
+        <v>56.98</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         <v>46041.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         <v>46041.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>56.78</v>
+        <v>57.06003</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1676,7 +1676,7 @@
         <v>46041.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>36.06</v>
+        <v>56.97996</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1697,7 +1697,7 @@
         <v>46041.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>48.75983</v>
+        <v>56.97996</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
         <v>46041.125</v>
       </c>
       <c r="B56" t="n">
-        <v>49.44748</v>
+        <v>57.06003</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1739,7 +1739,7 @@
         <v>46041.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>50.33883</v>
+        <v>57.06003</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1760,7 +1760,7 @@
         <v>46041.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46041.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>57.76254</v>
+        <v>59.1451</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>57.06003</v>
+        <v>57.99562</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>58.81169</v>
+        <v>65</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1844,7 +1844,7 @@
         <v>46041.25</v>
       </c>
       <c r="B62" t="n">
-        <v>58.02194</v>
+        <v>65</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1886,7 +1886,7 @@
         <v>46041.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>36.06</v>
+        <v>35.88</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>5.16569</v>
+        <v>23.61013</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>46041.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.64744</v>
+        <v>0.7</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46041.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.14712</v>
+        <v>-6.23257</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46041.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-7.02049</v>
+        <v>-6.09194</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-7.15517</v>
+        <v>-6.17304</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-7.67966</v>
+        <v>-6.02722</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46041.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-7.68692</v>
+        <v>-6.94065</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-7.23621</v>
+        <v>-6.98156</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-6.19058</v>
+        <v>-7.47989</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-6.35843</v>
+        <v>-6.06786</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-6.06857</v>
+        <v>-5.95332</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-5.72243</v>
+        <v>-5.51</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46041.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-5.51</v>
+        <v>-5.50985</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46041.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-2.53338</v>
+        <v>-0.95731</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>0.00025</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.54896</v>
+        <v>-2.54783</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-2.40408</v>
+        <v>0.01029</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>4.79045</v>
+        <v>5.04892</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46041.75</v>
       </c>
       <c r="B86" t="n">
-        <v>20.78901</v>
+        <v>20.67051</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>54.66255</v>
+        <v>55.45586</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>57.85505</v>
+        <v>57.40696</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>71.91437000000001</v>
+        <v>73.20007</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>68.63066999999999</v>
+        <v>68.75594</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         <v>46041.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>66.50706</v>
+        <v>67.64812000000001</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46041.875</v>
       </c>
       <c r="B92" t="n">
-        <v>63.83273</v>
+        <v>64.6053</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2495,7 +2495,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>61.9517</v>
+        <v>65</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>58.95387</v>
+        <v>62.95723</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>57.3</v>
+        <v>57.98162</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>57.06007</v>
+        <v>57.3</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2579,7 +2579,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>57.06003</v>
+        <v>60.2337</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 84)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -478,39 +478,39 @@
         <v>46040.27083333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.85416666666</v>
+        <v>46040.83333333334</v>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="D2" t="n">
-        <v>52.91999999999999</v>
+        <v>51.02999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>149.216769</v>
+        <v>102.29225175</v>
       </c>
       <c r="F2" t="n">
-        <v>2.819666836734695</v>
+        <v>2.004551278659612</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.91666666666</v>
+        <v>46040.89583333334</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>46041.125</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="D3" t="n">
-        <v>18.9</v>
+        <v>20.79</v>
       </c>
       <c r="E3" t="n">
-        <v>520.6762177499999</v>
+        <v>553.9420672499999</v>
       </c>
       <c r="F3" t="n">
-        <v>27.54900623015872</v>
+        <v>26.64464007936508</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>34.02</v>
       </c>
       <c r="E4" t="n">
-        <v>20.29469325000004</v>
+        <v>9.400169999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5965518298059976</v>
+        <v>0.2763130511463845</v>
       </c>
     </row>
   </sheetData>
@@ -1235,7 +1235,7 @@
         <v>46040.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-11.93964</v>
+        <v>-14</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>46040.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-5.43826</v>
+        <v>-6.93618</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,11 +1277,11 @@
         <v>46040.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.41</v>
+        <v>-7.32882</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D35" s="3" t="n">
@@ -1298,11 +1298,11 @@
         <v>46040.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>8.2301</v>
+        <v>-5.01</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D36" s="3" t="n">
@@ -1319,7 +1319,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>9.78525</v>
+        <v>8.12758</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>14.2512</v>
+        <v>23.75089</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>29.00544</v>
+        <v>36.0601</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>30.91231</v>
+        <v>36.2</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>56.98</v>
+        <v>56.75206</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>49.36694</v>
+        <v>56.98</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1445,7 +1445,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
         <v>46040.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>50.56345</v>
+        <v>48.69693</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
         <v>46040.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>49.15555</v>
+        <v>49.00283</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1592,7 +1592,7 @@
         <v>46041</v>
       </c>
       <c r="B50" t="n">
-        <v>56.20781</v>
+        <v>49.71727</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         <v>46041.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>56.98</v>
+        <v>56.67913</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         <v>46041.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>57.06003</v>
+        <v>56.98</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1676,7 +1676,7 @@
         <v>46041.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>56.97996</v>
+        <v>49.66961</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1697,7 +1697,7 @@
         <v>46041.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>56.97996</v>
+        <v>50.31981</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
         <v>46041.125</v>
       </c>
       <c r="B56" t="n">
-        <v>57.06003</v>
+        <v>56.97996</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46041.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>59.1451</v>
+        <v>58.7939</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>57.99562</v>
+        <v>57.99491</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>65</v>
+        <v>60.22599</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         <v>46041.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>36.06</v>
+        <v>35.87995</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>23.61013</v>
+        <v>6.22283</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>46041.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.7</v>
+        <v>0.65994</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         <v>46041.375</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>2e-05</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.50985</v>
+        <v>-5.74313</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46041.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.23257</v>
+        <v>-6.16607</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46041.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-6.09194</v>
+        <v>-5.58973</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-6.17304</v>
+        <v>-5.02552</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-6.02722</v>
+        <v>-5.74313</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46041.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-6.94065</v>
+        <v>-5.97681</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-6.98156</v>
+        <v>-6.81508</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-7.47989</v>
+        <v>-6.75779</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-6.06786</v>
+        <v>-6.0733</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-5.95332</v>
+        <v>-5.01</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-5.51</v>
+        <v>-5.35398</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46041.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-5.50985</v>
+        <v>-4.74702</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46041.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.95731</v>
+        <v>2e-05</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>0.00025</v>
+        <v>0.00549</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.54783</v>
+        <v>-2.5268</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>0.01029</v>
+        <v>0.19949</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>5.04892</v>
+        <v>6.29329</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46041.75</v>
       </c>
       <c r="B86" t="n">
-        <v>20.67051</v>
+        <v>28.30083</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>55.45586</v>
+        <v>55.97213</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>57.40696</v>
+        <v>58.25818</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>73.20007</v>
+        <v>75.95748</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>68.75594</v>
+        <v>77.03646999999999</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         <v>46041.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>67.64812000000001</v>
+        <v>68.94773000000001</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46041.875</v>
       </c>
       <c r="B92" t="n">
-        <v>64.6053</v>
+        <v>66.7355</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>62.95723</v>
+        <v>63.40191</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>57.98162</v>
+        <v>58.67257</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>57.3</v>
+        <v>58.20539</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2579,7 +2579,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>60.2337</v>
+        <v>62.16997</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 86)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -475,42 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.27083333334</v>
+        <v>46040.25</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.875</v>
+        <v>46040.8125</v>
       </c>
       <c r="C2" t="n">
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="D2" t="n">
-        <v>54.81</v>
+        <v>51.02999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>206.949366</v>
+        <v>82.64275499999999</v>
       </c>
       <c r="F2" t="n">
-        <v>3.775759277504105</v>
+        <v>1.619493533215755</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.9375</v>
+        <v>46040.89583333334</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>46041.125</v>
       </c>
       <c r="C3" t="n">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D3" t="n">
-        <v>17.01</v>
+        <v>20.79</v>
       </c>
       <c r="E3" t="n">
-        <v>426.3550785</v>
+        <v>564.4766399999999</v>
       </c>
       <c r="F3" t="n">
-        <v>25.0649664021164</v>
+        <v>27.15135353535353</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>34.02</v>
       </c>
       <c r="E4" t="n">
-        <v>-34.45792349999999</v>
+        <v>23.43251625</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.012872530864197</v>
+        <v>0.6887864858906527</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +848,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
         <v>46040.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-6</v>
+        <v>0.29323</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46040.75</v>
       </c>
       <c r="B38" t="n">
-        <v>17.71906</v>
+        <v>2.26942</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,11 +1361,11 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>30.58443</v>
+        <v>25.70442</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
@@ -1382,11 +1382,11 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>55.38427</v>
+        <v>55.67285</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1424,7 +1424,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>56.52615</v>
+        <v>57.53438</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1445,7 +1445,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>56.98</v>
+        <v>65</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>57.3</v>
+        <v>63.40828</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
         <v>46040.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>49.04675</v>
+        <v>56.45174</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         <v>46040.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>36.2</v>
+        <v>48.49694</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
         <v>46040.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>36.2</v>
+        <v>48.98648</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1592,7 +1592,7 @@
         <v>46041</v>
       </c>
       <c r="B50" t="n">
-        <v>47.31324</v>
+        <v>49.10815</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         <v>46041.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>56.36108</v>
+        <v>56.66584</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         <v>46041.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.06003</v>
+        <v>48.59637</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1676,7 +1676,7 @@
         <v>46041.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>48.4027</v>
+        <v>49.63741</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1697,7 +1697,7 @@
         <v>46041.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>49.72346</v>
+        <v>49.9874</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
         <v>46041.125</v>
       </c>
       <c r="B56" t="n">
-        <v>50.63512</v>
+        <v>56.97996</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46041.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>59.11391</v>
+        <v>58.75342</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>57.82778</v>
+        <v>57.95516</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>60.21199</v>
+        <v>60.18442</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         <v>46041.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>4.45932</v>
+        <v>29.2867</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.51</v>
+        <v>6.03759</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         <v>46041.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-2.83936</v>
+        <v>2e-05</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-6.13408</v>
+        <v>-5.7216</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46041.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.33411</v>
+        <v>-6.03995</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46041.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-6.12189</v>
+        <v>-6.12917</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-6.50816</v>
+        <v>-5.01</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-6.25482</v>
+        <v>-5.01</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46041.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-6.07918</v>
+        <v>-5.54648</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-6.73139</v>
+        <v>-6.11947</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-6.49292</v>
+        <v>-5.50985</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-6.21235</v>
+        <v>-2.5945</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-5.51</v>
+        <v>2e-05</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-5.51</v>
+        <v>2e-05</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46041.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-5.01</v>
+        <v>0</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46041.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.96252</v>
+        <v>2e-05</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>0.00025</v>
+        <v>0.00047</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.48837</v>
+        <v>-2.48761</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-0.50876</v>
+        <v>0.43069</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>0.91882</v>
+        <v>0.9195</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46041.75</v>
       </c>
       <c r="B86" t="n">
-        <v>20.22705</v>
+        <v>12.59745</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>53.6751</v>
+        <v>53.45632</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>57.3908</v>
+        <v>56.95316</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>77.49445</v>
+        <v>76.92748</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>75.93411</v>
+        <v>73.20007</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46041.875</v>
       </c>
       <c r="B92" t="n">
-        <v>68.44318</v>
+        <v>68.44448</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>62.9353</v>
+        <v>62.93811</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>59.00814</v>
+        <v>58.95394</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>58.18858</v>
+        <v>57.97171</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 87)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -475,42 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.25</v>
+        <v>46040.27083333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46040.8125</v>
+        <v>46040.85416666666</v>
       </c>
       <c r="C2" t="n">
-        <v>13.5</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>51.02999999999999</v>
+        <v>52.91999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>82.64275499999999</v>
+        <v>118.342185</v>
       </c>
       <c r="F2" t="n">
-        <v>1.619493533215755</v>
+        <v>2.236246882086168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.89583333334</v>
+        <v>46040.91666666666</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>46041.125</v>
       </c>
       <c r="C3" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>20.79</v>
+        <v>18.9</v>
       </c>
       <c r="E3" t="n">
-        <v>564.4766399999999</v>
+        <v>427.33517775</v>
       </c>
       <c r="F3" t="n">
-        <v>27.15135353535353</v>
+        <v>22.61032686507937</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>34.02</v>
       </c>
       <c r="E4" t="n">
-        <v>23.43251625</v>
+        <v>9.549998250000009</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6887864858906527</v>
+        <v>0.2807171737213407</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +848,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1361,7 +1361,7 @@
         <v>46040.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>25.70442</v>
+        <v>4.23686</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>55.67285</v>
+        <v>56.85524</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1403,11 +1403,11 @@
         <v>46040.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>57.3</v>
+        <v>56.98</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1424,11 +1424,11 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>57.53438</v>
+        <v>56.98</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1445,7 +1445,7 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>65</v>
+        <v>57.3</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>63.40828</v>
+        <v>57.8068</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         <v>46040.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1508,7 +1508,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.06007</v>
+        <v>56.98</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1529,7 +1529,7 @@
         <v>46040.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>56.45174</v>
+        <v>47.11292</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         <v>46040.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>48.49694</v>
+        <v>36.2</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
         <v>46040.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>48.98648</v>
+        <v>36.2</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1592,7 +1592,7 @@
         <v>46041</v>
       </c>
       <c r="B50" t="n">
-        <v>49.10815</v>
+        <v>36.2</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         <v>46041.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>56.66584</v>
+        <v>36.2</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         <v>46041.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>48.59637</v>
+        <v>36.2</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1676,7 +1676,7 @@
         <v>46041.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>49.63741</v>
+        <v>47.79916</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1697,7 +1697,7 @@
         <v>46041.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>49.9874</v>
+        <v>48.42041</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
         <v>46041.125</v>
       </c>
       <c r="B56" t="n">
-        <v>56.97996</v>
+        <v>49.90902</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46041.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>58.75342</v>
+        <v>57.06003</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>57.95516</v>
+        <v>58.29092</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>60.18442</v>
+        <v>60.17508</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
         <v>46041.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>29.2867</v>
+        <v>36.06</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>6.03759</v>
+        <v>0.7</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         <v>46041.375</v>
       </c>
       <c r="B68" t="n">
-        <v>2e-05</v>
+        <v>0.01003</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.7216</v>
+        <v>-5.6862</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46041.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.03995</v>
+        <v>-6.14423</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46041.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-6.12917</v>
+        <v>-6.11853</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
         <v>46041.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-5.54648</v>
+        <v>-5.50985</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-6.11947</v>
+        <v>-5.50985</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-5.50985</v>
+        <v>-6.01122</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-2.5945</v>
+        <v>-6.07128</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>2e-05</v>
+        <v>-5.01</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>2e-05</v>
+        <v>-4.70876</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46041.625</v>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>-2.57526</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>0.00047</v>
+        <v>0.0003</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.48761</v>
+        <v>-2.48809</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>0.43069</v>
+        <v>0.00976</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>0.9195</v>
+        <v>0.40914</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46041.75</v>
       </c>
       <c r="B86" t="n">
-        <v>12.59745</v>
+        <v>12.60083</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>53.45632</v>
+        <v>44.45378</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>56.95316</v>
+        <v>57.38802</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>76.92748</v>
+        <v>77.18000000000001</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>73.20007</v>
+        <v>77.61297999999999</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46041.875</v>
       </c>
       <c r="B92" t="n">
-        <v>68.44448</v>
+        <v>65</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>62.93811</v>
+        <v>61.17796</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>58.95394</v>
+        <v>58.65468</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>57.97171</v>
+        <v>57.64573</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2579,7 +2579,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>61.96632</v>
+        <v>61.65027</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 88)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -475,42 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46040.27083333334</v>
+        <v>46040.25</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>46040.85416666666</v>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>14.5</v>
       </c>
       <c r="D2" t="n">
-        <v>52.91999999999999</v>
+        <v>54.81</v>
       </c>
       <c r="E2" t="n">
-        <v>118.342185</v>
+        <v>143.6525415</v>
       </c>
       <c r="F2" t="n">
-        <v>2.236246882086168</v>
+        <v>2.620918472906404</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46040.91666666666</v>
+        <v>46040.9375</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>46041.125</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D3" t="n">
-        <v>18.9</v>
+        <v>17.01</v>
       </c>
       <c r="E3" t="n">
-        <v>427.33517775</v>
+        <v>398.40378825</v>
       </c>
       <c r="F3" t="n">
-        <v>22.61032686507937</v>
+        <v>23.42173946208113</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>34.02</v>
       </c>
       <c r="E4" t="n">
-        <v>9.549998250000009</v>
+        <v>69.74660550000003</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2807171737213407</v>
+        <v>2.050164770723105</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +848,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1382,7 +1382,7 @@
         <v>46040.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>56.85524</v>
+        <v>36.2</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46040.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>56.98</v>
+        <v>46.53455</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1445,11 +1445,11 @@
         <v>46040.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>57.3</v>
+        <v>62.21582</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1466,11 +1466,11 @@
         <v>46040.875</v>
       </c>
       <c r="B44" t="n">
-        <v>57.8068</v>
+        <v>62.97041</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1508,7 +1508,7 @@
         <v>46040.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.98</v>
+        <v>57.06007</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
         <v>46040.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>47.11292</v>
+        <v>56.98</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         <v>46040.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>36.2</v>
+        <v>55.57436</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
         <v>46040.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>36.2</v>
+        <v>49.23901</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1592,7 +1592,7 @@
         <v>46041</v>
       </c>
       <c r="B50" t="n">
-        <v>36.2</v>
+        <v>49.34509</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
         <v>46041.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>36.2</v>
+        <v>55.94746</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1634,7 +1634,7 @@
         <v>46041.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>36.2</v>
+        <v>40.54</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
         <v>46041.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>56.98</v>
+        <v>35.86</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1676,7 +1676,7 @@
         <v>46041.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>47.79916</v>
+        <v>29.25339</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1697,7 +1697,7 @@
         <v>46041.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>48.42041</v>
+        <v>35.87996</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
         <v>46041.125</v>
       </c>
       <c r="B56" t="n">
-        <v>49.90902</v>
+        <v>36.2</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1739,7 +1739,7 @@
         <v>46041.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>56.98</v>
+        <v>45.21307</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         <v>46041.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>57.06003</v>
+        <v>58.71596</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>58.29092</v>
+        <v>58.95696</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>60.17508</v>
+        <v>65</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1886,7 +1886,7 @@
         <v>46041.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>35.88</v>
+        <v>36.06</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.7</v>
+        <v>24.92768</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
         <v>46041.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.51</v>
+        <v>22.07</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         <v>46041.375</v>
       </c>
       <c r="B68" t="n">
-        <v>0.01003</v>
+        <v>0.51</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.6862</v>
+        <v>-5.01</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>46041.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.14423</v>
+        <v>-5.50985</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>46041.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-6.11853</v>
+        <v>-5.79092</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-5.01</v>
+        <v>-4.83724</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2075,7 +2075,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-5.01</v>
+        <v>-5.50985</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2117,7 +2117,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-5.50985</v>
+        <v>-4.85271</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-6.01122</v>
+        <v>-5.01</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2159,7 +2159,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-6.07128</v>
+        <v>-2.5711</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-5.01</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2201,7 +2201,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-4.70876</v>
+        <v>-0.91982</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2222,7 +2222,7 @@
         <v>46041.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-2.57526</v>
+        <v>-2.57161</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>46041.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>2e-05</v>
+        <v>0.00025</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2264,7 +2264,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>0.0003</v>
+        <v>0.00048</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2285,7 +2285,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.48809</v>
+        <v>-5.25561</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2306,7 +2306,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>0.00976</v>
+        <v>-2.53803</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>0.40914</v>
+        <v>0.01346</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>46041.75</v>
       </c>
       <c r="B86" t="n">
-        <v>12.60083</v>
+        <v>12.05992</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>44.45378</v>
+        <v>52.67227</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2390,7 +2390,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>57.38802</v>
+        <v>57.46321</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2411,7 +2411,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>77.18000000000001</v>
+        <v>62.05077</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>77.61297999999999</v>
+        <v>73.20007</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2474,7 +2474,7 @@
         <v>46041.875</v>
       </c>
       <c r="B92" t="n">
-        <v>65</v>
+        <v>69.62199</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>61.17796</v>
+        <v>62.98392</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2537,7 +2537,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>58.65468</v>
+        <v>58.98682</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>57.64573</v>
+        <v>58.15428</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2579,7 +2579,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>61.65027</v>
+        <v>61.96632</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 92)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,22 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46041</v>
+        <v>46041.16666666666</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>46041.66666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>60.48</v>
+        <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>691.8912779999998</v>
+        <v>341.6364315</v>
       </c>
       <c r="F2" t="n">
-        <v>11.44000128968254</v>
+        <v>7.53166736111111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>46041.83333333334</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>46042</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>15.12</v>
+      </c>
+      <c r="E3" t="n">
+        <v>484.6414267499999</v>
+      </c>
+      <c r="F3" t="n">
+        <v>32.05300441468254</v>
       </c>
     </row>
   </sheetData>
@@ -504,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,7 +561,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46041</v>
+        <v>46041.02083333334</v>
       </c>
       <c r="B2" t="n">
         <v>57.06003</v>
@@ -556,20 +576,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46041.02083333334</v>
+        <v>46041.04166666666</v>
       </c>
       <c r="B3" t="n">
         <v>57.06003</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
@@ -577,13 +597,13 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46041.04166666666</v>
+        <v>46041.0625</v>
       </c>
       <c r="B4" t="n">
         <v>56.98</v>
@@ -598,16 +618,16 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46041.0625</v>
+        <v>46041.08333333334</v>
       </c>
       <c r="B5" t="n">
-        <v>48.17243</v>
+        <v>47.65133</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -619,16 +639,16 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46041.08333333334</v>
+        <v>46041.10416666666</v>
       </c>
       <c r="B6" t="n">
-        <v>35.87995</v>
+        <v>47.99544</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -640,16 +660,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46041.10416666666</v>
+        <v>46041.125</v>
       </c>
       <c r="B7" t="n">
-        <v>35.87996</v>
+        <v>48.31738</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -661,16 +681,16 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46041.125</v>
+        <v>46041.14583333334</v>
       </c>
       <c r="B8" t="n">
-        <v>35.87996</v>
+        <v>57.06003</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -682,16 +702,16 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46041.14583333334</v>
+        <v>46041.16666666666</v>
       </c>
       <c r="B9" t="n">
-        <v>36.2</v>
+        <v>57.06003</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -709,10 +729,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46041.16666666666</v>
+        <v>46041.1875</v>
       </c>
       <c r="B10" t="n">
-        <v>57.06003</v>
+        <v>58.82614</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -730,10 +750,10 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46041.1875</v>
+        <v>46041.20833333334</v>
       </c>
       <c r="B11" t="n">
-        <v>57.08</v>
+        <v>57.83627</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -751,10 +771,10 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46041.20833333334</v>
+        <v>46041.22916666666</v>
       </c>
       <c r="B12" t="n">
-        <v>58.91675</v>
+        <v>60.45412</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -772,10 +792,10 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46041.22916666666</v>
+        <v>46041.25</v>
       </c>
       <c r="B13" t="n">
-        <v>60.00348</v>
+        <v>60.20735</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -793,10 +813,10 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46041.25</v>
+        <v>46041.27083333334</v>
       </c>
       <c r="B14" t="n">
-        <v>60.36248</v>
+        <v>57.06003</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -814,10 +834,10 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46041.27083333334</v>
+        <v>46041.29166666666</v>
       </c>
       <c r="B15" t="n">
-        <v>57.06003</v>
+        <v>32.50105</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -835,10 +855,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46041.29166666666</v>
+        <v>46041.3125</v>
       </c>
       <c r="B16" t="n">
-        <v>35.88</v>
+        <v>1.302</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -856,10 +876,10 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46041.3125</v>
+        <v>46041.33333333334</v>
       </c>
       <c r="B17" t="n">
-        <v>2.75359</v>
+        <v>0.51</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -877,10 +897,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46041.33333333334</v>
+        <v>46041.35416666666</v>
       </c>
       <c r="B18" t="n">
-        <v>0.7</v>
+        <v>6.66416</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -898,10 +918,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46041.35416666666</v>
+        <v>46041.375</v>
       </c>
       <c r="B19" t="n">
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -919,10 +939,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46041.375</v>
+        <v>46041.39583333334</v>
       </c>
       <c r="B20" t="n">
-        <v>0.51</v>
+        <v>-0.9374400000000001</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -940,10 +960,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46041.39583333334</v>
+        <v>46041.41666666666</v>
       </c>
       <c r="B21" t="n">
-        <v>-2.83936</v>
+        <v>-5.50985</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -961,10 +981,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46041.41666666666</v>
+        <v>46041.4375</v>
       </c>
       <c r="B22" t="n">
-        <v>-5.01</v>
+        <v>-5.92186</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -982,10 +1002,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46041.4375</v>
+        <v>46041.45833333334</v>
       </c>
       <c r="B23" t="n">
-        <v>-5.99221</v>
+        <v>-0.93203</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1003,10 +1023,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46041.45833333334</v>
+        <v>46041.47916666666</v>
       </c>
       <c r="B24" t="n">
-        <v>-5.50985</v>
+        <v>-4.93017</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1024,7 +1044,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46041.47916666666</v>
+        <v>46041.5</v>
       </c>
       <c r="B25" t="n">
         <v>-5.01</v>
@@ -1045,10 +1065,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46041.5</v>
+        <v>46041.52083333334</v>
       </c>
       <c r="B26" t="n">
-        <v>-5.01</v>
+        <v>-5.75827</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1066,10 +1086,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>46041.52083333334</v>
+        <v>46041.54166666666</v>
       </c>
       <c r="B27" t="n">
-        <v>-5.01</v>
+        <v>-5.50985</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1087,10 +1107,10 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>46041.54166666666</v>
+        <v>46041.5625</v>
       </c>
       <c r="B28" t="n">
-        <v>-5.36218</v>
+        <v>-5.01</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1108,10 +1128,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>46041.5625</v>
+        <v>46041.58333333334</v>
       </c>
       <c r="B29" t="n">
-        <v>-2.83936</v>
+        <v>-2.61261</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1129,10 +1149,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>46041.58333333334</v>
+        <v>46041.60416666666</v>
       </c>
       <c r="B30" t="n">
-        <v>-2.633</v>
+        <v>-0.91299</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1150,10 +1170,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>46041.60416666666</v>
+        <v>46041.625</v>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>0.00026</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1171,10 +1191,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>46041.625</v>
+        <v>46041.64583333334</v>
       </c>
       <c r="B32" t="n">
-        <v>0.00932</v>
+        <v>0.51</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1192,7 +1212,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>46041.64583333334</v>
+        <v>46041.66666666666</v>
       </c>
       <c r="B33" t="n">
         <v>0.7</v>
@@ -1207,16 +1227,16 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>46041.66666666666</v>
+        <v>46041.6875</v>
       </c>
       <c r="B34" t="n">
-        <v>0.7</v>
+        <v>-2.47201</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1234,10 +1254,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>46041.6875</v>
+        <v>46041.70833333334</v>
       </c>
       <c r="B35" t="n">
-        <v>-2.47112</v>
+        <v>-2.54304</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1255,10 +1275,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>46041.70833333334</v>
+        <v>46041.72916666666</v>
       </c>
       <c r="B36" t="n">
-        <v>-2.561</v>
+        <v>0.00957</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1276,10 +1296,10 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>46041.72916666666</v>
+        <v>46041.75</v>
       </c>
       <c r="B37" t="n">
-        <v>0.85345</v>
+        <v>11.99698</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1297,10 +1317,10 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>46041.75</v>
+        <v>46041.77083333334</v>
       </c>
       <c r="B38" t="n">
-        <v>11.98884</v>
+        <v>52.39947</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1318,10 +1338,10 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>46041.77083333334</v>
+        <v>46041.79166666666</v>
       </c>
       <c r="B39" t="n">
-        <v>53.24872</v>
+        <v>56.74129</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1339,10 +1359,10 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>46041.79166666666</v>
+        <v>46041.8125</v>
       </c>
       <c r="B40" t="n">
-        <v>56.70352</v>
+        <v>62.07578</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1360,10 +1380,10 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>46041.8125</v>
+        <v>46041.83333333334</v>
       </c>
       <c r="B41" t="n">
-        <v>64.02524</v>
+        <v>65</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1375,16 +1395,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>46041.83333333334</v>
+        <v>46041.85416666666</v>
       </c>
       <c r="B42" t="n">
-        <v>67.83107</v>
+        <v>65</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1396,13 +1416,13 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>46041.85416666666</v>
+        <v>46041.875</v>
       </c>
       <c r="B43" t="n">
         <v>65</v>
@@ -1417,16 +1437,16 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>46041.875</v>
+        <v>46041.89583333334</v>
       </c>
       <c r="B44" t="n">
-        <v>65</v>
+        <v>62.49071</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1438,16 +1458,16 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>46041.89583333334</v>
+        <v>46041.91666666666</v>
       </c>
       <c r="B45" t="n">
-        <v>65</v>
+        <v>61.16151</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1459,16 +1479,16 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>46041.91666666666</v>
+        <v>46041.9375</v>
       </c>
       <c r="B46" t="n">
-        <v>61.25461</v>
+        <v>58.63887</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1480,16 +1500,16 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46041.9375</v>
+        <v>46041.95833333334</v>
       </c>
       <c r="B47" t="n">
-        <v>59.32564</v>
+        <v>58.14989</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1501,16 +1521,16 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>46041.95833333334</v>
+        <v>46041.97916666666</v>
       </c>
       <c r="B48" t="n">
-        <v>58.48649</v>
+        <v>61.62715</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1522,28 +1542,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OFF</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
-        <v>46041.97916666666</v>
-      </c>
-      <c r="B49" t="n">
-        <v>62.04825</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>forecast</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="n">
-        <v>46041</v>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update latest output (run 95)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>772.50727125</v>
+        <v>751.1665979999999</v>
       </c>
       <c r="F2" t="n">
-        <v>12.77293768601191</v>
+        <v>12.42008263888889</v>
       </c>
     </row>
   </sheetData>
@@ -649,7 +649,7 @@
         <v>46041.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>57.06003</v>
+        <v>35.87996</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -670,7 +670,7 @@
         <v>46041.125</v>
       </c>
       <c r="B8" t="n">
-        <v>57.06003</v>
+        <v>57.50228</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -691,11 +691,11 @@
         <v>46041.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>57.83179</v>
+        <v>58.03822</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
@@ -712,11 +712,11 @@
         <v>46041.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>57.48786</v>
+        <v>57.52849</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
@@ -733,7 +733,7 @@
         <v>46041.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>60.39169</v>
+        <v>61.43135</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>60.34276</v>
+        <v>60.04433</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -775,7 +775,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>71.95779</v>
+        <v>65</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>46041.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>7.82154</v>
+        <v>10.07303</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>0.7</v>
+        <v>7.0734</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46041.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>7.00436</v>
+        <v>7.08291</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46041.375</v>
       </c>
       <c r="B20" t="n">
-        <v>0.7</v>
+        <v>0.68371</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.94872</v>
+        <v>-3.6481</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         <v>46041.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-5.01</v>
+        <v>-5.74313</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>-6.1096</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-5.82017</v>
+        <v>-2.83936</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46041.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-4.658</v>
+        <v>-5.50985</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-5.17224</v>
+        <v>-5.01</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-5.50985</v>
+        <v>-0.89316</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-2.83936</v>
+        <v>-5.01</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.93813</v>
+        <v>2e-05</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46041.625</v>
       </c>
       <c r="B32" t="n">
-        <v>0.009469999999999999</v>
+        <v>0.00848</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>1.21401</v>
+        <v>1.68233</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.91614</v>
+        <v>-2.49239</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>0.33937</v>
+        <v>0.85381</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46041.75</v>
       </c>
       <c r="B38" t="n">
-        <v>12.09882</v>
+        <v>12.09485</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>43.32325</v>
+        <v>42.36398</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>56.77711</v>
+        <v>56.76084</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>60.96077</v>
+        <v>64.02197</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>65</v>
+        <v>59.67565</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46041.875</v>
       </c>
       <c r="B44" t="n">
-        <v>62.69405</v>
+        <v>65</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>62.96752</v>
+        <v>62.50682</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>61.4952</v>
+        <v>61.52231</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>58.97571</v>
+        <v>58.9823</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>58.48808</v>
+        <v>58.49509</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>62.01329</v>
+        <v>62.01673</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 96)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>751.1665979999999</v>
+        <v>719.6379644999998</v>
       </c>
       <c r="F2" t="n">
-        <v>12.42008263888889</v>
+        <v>11.89877586805555</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +670,7 @@
         <v>46041.125</v>
       </c>
       <c r="B8" t="n">
-        <v>57.50228</v>
+        <v>36.2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -691,7 +691,7 @@
         <v>46041.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>58.03822</v>
+        <v>48.37963</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
         <v>46041.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>57.52849</v>
+        <v>57.08</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -733,11 +733,11 @@
         <v>46041.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>61.43135</v>
+        <v>61.81795</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
@@ -754,11 +754,11 @@
         <v>46041.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>60.04433</v>
+        <v>60.49589</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
@@ -775,7 +775,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>65</v>
+        <v>71.97167</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
         <v>46041.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>35.88</v>
+        <v>36.06</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -859,7 +859,7 @@
         <v>46041.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>10.07303</v>
+        <v>8.797459999999999</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>7.0734</v>
+        <v>0.7</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46041.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>7.08291</v>
+        <v>0.7</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46041.375</v>
       </c>
       <c r="B20" t="n">
-        <v>0.68371</v>
+        <v>0.7</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-3.6481</v>
+        <v>-2.83936</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-6.1096</v>
+        <v>-5.74313</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-2.83936</v>
+        <v>0</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46041.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-5.50985</v>
+        <v>-2.83936</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-5.01</v>
+        <v>-4.6323</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.89316</v>
+        <v>-4.73809</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-5.01</v>
+        <v>-2.69309</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>2e-05</v>
+        <v>-0.93819</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>2e-05</v>
+        <v>3e-05</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46041.625</v>
       </c>
       <c r="B32" t="n">
-        <v>0.00848</v>
+        <v>0.51</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>1.68233</v>
+        <v>1.67481</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-2.49239</v>
+        <v>-2.49115</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>0.85381</v>
+        <v>0.009650000000000001</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46041.75</v>
       </c>
       <c r="B38" t="n">
-        <v>12.09485</v>
+        <v>12.0924</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>42.36398</v>
+        <v>42.36428</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>56.76084</v>
+        <v>56.7552</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>64.02197</v>
+        <v>59.19183</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>59.67565</v>
+        <v>65</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>62.50682</v>
+        <v>62.96274</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>61.52231</v>
+        <v>61.15479</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>58.9823</v>
+        <v>58.98416</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>58.49509</v>
+        <v>58.49624</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>62.01673</v>
+        <v>62.01821</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 98)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>667.18018575</v>
+        <v>683.2300507500001</v>
       </c>
       <c r="F2" t="n">
-        <v>11.03141841517857</v>
+        <v>11.2967931671627</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +775,7 @@
         <v>46041.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>59.72842</v>
+        <v>59.38996</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
         <v>46041.25</v>
       </c>
       <c r="B14" t="n">
-        <v>65</v>
+        <v>58.22729</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -821,7 +821,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
@@ -838,11 +838,11 @@
         <v>46041.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>33.08222</v>
+        <v>35.88</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
@@ -859,7 +859,7 @@
         <v>46041.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>0.98766</v>
+        <v>18.52411</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         <v>46041.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46041.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>0.51</v>
+        <v>0.0101</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46041.375</v>
       </c>
       <c r="B20" t="n">
-        <v>4e-05</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
         <v>46041.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-5.01</v>
+        <v>-5.50985</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46041.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-5.50985</v>
+        <v>-5.74313</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46041.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-5.17224</v>
+        <v>-5.50985</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46041.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-5.50985</v>
+        <v>-2.83936</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46041.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-5.17224</v>
+        <v>-5.82892</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>46041.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-6.03975</v>
+        <v>-5.50985</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46041.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-5.74313</v>
+        <v>-6.00674</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46041.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-4.82081</v>
+        <v>-5.50985</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46041.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-3.6481</v>
+        <v>-0.93941</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46041.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-2.5941</v>
+        <v>-2.59483</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0003</v>
+        <v>0.00025</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>-0.8372000000000001</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>0.20106</v>
+        <v>0.20113</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46041.75</v>
       </c>
       <c r="B38" t="n">
-        <v>12.27791</v>
+        <v>12.28008</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>42.27416</v>
+        <v>42.27439</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>56.22722</v>
+        <v>56.23621</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>62.41906</v>
+        <v>60.86769</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>65</v>
+        <v>59.25265</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46041.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>59.92511</v>
+        <v>65</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46041.875</v>
       </c>
       <c r="B44" t="n">
-        <v>61.34626</v>
+        <v>65</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>62.95966</v>
+        <v>62.96535</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>61.72504</v>
+        <v>61.73186</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>60.03504</v>
+        <v>60.03598</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>62.07511</v>
+        <v>62.07428</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 105)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -507,10 +507,10 @@
         <v>35.91</v>
       </c>
       <c r="E3" t="n">
-        <v>52.77443925000003</v>
+        <v>52.26773175000002</v>
       </c>
       <c r="F3" t="n">
-        <v>1.469630722639934</v>
+        <v>1.455520238095239</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>457.1512432499999</v>
+        <v>471.5901352499999</v>
       </c>
       <c r="F4" t="n">
-        <v>30.23487058531746</v>
+        <v>31.18982375992063</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +547,10 @@
         <v>34.02</v>
       </c>
       <c r="E5" t="n">
-        <v>-59.26747124999999</v>
+        <v>-60.296652</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.742136133156966</v>
+        <v>-1.77238835978836</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1234,7 @@
         <v>46041.625</v>
       </c>
       <c r="B32" t="n">
-        <v>0.01929</v>
+        <v>0.00016</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1255,7 +1255,7 @@
         <v>46041.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>0.51</v>
+        <v>0.009429999999999999</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1276,11 +1276,11 @@
         <v>46041.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D34" s="3" t="n">
@@ -1297,7 +1297,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.92309</v>
+        <v>0.7</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>0.264</v>
+        <v>4.80008</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>12.24467</v>
+        <v>8.264950000000001</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1360,7 +1360,7 @@
         <v>46041.75</v>
       </c>
       <c r="B38" t="n">
-        <v>26.68735</v>
+        <v>26.89449</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>45.84936</v>
+        <v>57.19078</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>59.11456</v>
+        <v>60.89812</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>64.01260000000001</v>
+        <v>64.93597</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>65</v>
+        <v>68.31175</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         <v>46041.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>62.62134</v>
+        <v>71.46543</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46041.875</v>
       </c>
       <c r="B44" t="n">
-        <v>64.05184</v>
+        <v>67.32592</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>65</v>
+        <v>66.65888</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>59.37719</v>
+        <v>64.8901</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.96819</v>
+        <v>59.37938</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1570,7 +1570,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>58.16113</v>
+        <v>60.76462</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>63.63924</v>
+        <v>64.04767</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46042</v>
       </c>
       <c r="B50" t="n">
-        <v>61.77255</v>
+        <v>63.00946</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         <v>46042.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>57.06003</v>
+        <v>61.57869</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46042.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.06003</v>
+        <v>63.10166</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46042.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>57.06003</v>
+        <v>57.49046</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46042.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>64.89</v>
+        <v>65</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46042.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>65.67543000000001</v>
+        <v>77.94</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46042.25</v>
       </c>
       <c r="B62" t="n">
-        <v>65.2897</v>
+        <v>78</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>46042.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>61.31557</v>
+        <v>66.67346999999999</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         <v>46042.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>8.71917</v>
+        <v>8.718500000000001</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
         <v>46042.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.7</v>
+        <v>0.5099399999999999</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46042.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-2.535</v>
+        <v>-2.55434</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         <v>46042.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.68809</v>
+        <v>-5.62917</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.48267</v>
+        <v>-6.96628</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46042.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-7.87948</v>
+        <v>-6.60898</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-8.815630000000001</v>
+        <v>-8.66264</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-8.67817</v>
+        <v>-8.643409999999999</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46042.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-9.99</v>
+        <v>-9.68276</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-9.99</v>
+        <v>-10</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         <v>46042.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-8.3056</v>
+        <v>-9.551170000000001</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-8.293850000000001</v>
+        <v>-8.70303</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46042.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-8.12302</v>
+        <v>-8.271380000000001</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-7.98411</v>
+        <v>-7.88906</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46042.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-7.00778</v>
+        <v>-7.96894</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-6.49292</v>
+        <v>-6</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-5.51</v>
+        <v>-2.84369</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-5.16677</v>
+        <v>-5.5912</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-2.9952</v>
+        <v>-2.96533</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>0.01019</v>
+        <v>0.01012</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46042.75</v>
       </c>
       <c r="B86" t="n">
-        <v>9.523630000000001</v>
+        <v>9.522930000000001</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>55.62763</v>
+        <v>46.32246</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>72.86584000000001</v>
+        <v>57.3</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2431,7 +2431,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>72.78848000000001</v>
+        <v>69.61881</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>71.8766</v>
+        <v>65</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46042.875</v>
       </c>
       <c r="B92" t="n">
-        <v>59.15606</v>
+        <v>59.15624</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>57.3</v>
+        <v>58.33176</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>59.93919</v>
+        <v>59.93754</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>63.27752</v>
+        <v>63.27623</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
         <v>46042.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>64.12223</v>
+        <v>64.12067</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 107)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -527,10 +527,10 @@
         <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>456.8181149999999</v>
+        <v>460.8246629999999</v>
       </c>
       <c r="F4" t="n">
-        <v>30.21283829365079</v>
+        <v>30.47782162698412</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +547,10 @@
         <v>34.02</v>
       </c>
       <c r="E5" t="n">
-        <v>-61.9336575</v>
+        <v>-38.58871575000001</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.820507275132275</v>
+        <v>-1.134294995590829</v>
       </c>
     </row>
   </sheetData>
@@ -1297,7 +1297,7 @@
         <v>46041.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.16887</v>
+        <v>-2.47052</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
         <v>46041.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-3.42323</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.99633</v>
+        <v>-2.58035</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1360,11 +1360,11 @@
         <v>46041.75</v>
       </c>
       <c r="B38" t="n">
-        <v>9.87266</v>
+        <v>3.34464</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D38" s="3" t="n">
@@ -1381,7 +1381,7 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>38.23834</v>
+        <v>38.55471</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>59.50248</v>
+        <v>57.18142</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>63.57365</v>
+        <v>64.53386</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>64.46451</v>
+        <v>65</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46041.875</v>
       </c>
       <c r="B44" t="n">
-        <v>67.39644</v>
+        <v>65.37398</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>65.14413999999999</v>
+        <v>65.74816</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>64.8901</v>
+        <v>59.50728</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>58.35781</v>
+        <v>64.8901</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1570,7 +1570,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>58.02218</v>
+        <v>59.04126</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>63.67826</v>
+        <v>63.32463</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46042</v>
       </c>
       <c r="B50" t="n">
-        <v>61.53081</v>
+        <v>61.17037</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         <v>46042.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>57.06003</v>
+        <v>60.8643</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
         <v>46042.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>57.06003</v>
+        <v>61.1294</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1780,7 @@
         <v>46042.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>57.06003</v>
+        <v>63.69192</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46042.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>57.13092</v>
+        <v>65</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46042.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>65</v>
+        <v>65.21083</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46042.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>67.7428</v>
+        <v>75.57516</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46042.25</v>
       </c>
       <c r="B62" t="n">
-        <v>67.60051</v>
+        <v>77.94</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>46042.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>67.13655</v>
+        <v>75.76638</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>46042.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>36.06</v>
+        <v>56.98</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         <v>46042.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>8.78514</v>
+        <v>8.85098</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
         <v>46042.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.01001</v>
+        <v>0.01108</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46042.375</v>
       </c>
       <c r="B68" t="n">
-        <v>0.00953</v>
+        <v>-2.57556</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         <v>46042.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.50985</v>
+        <v>-6</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.58192</v>
+        <v>-7.01255</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46042.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-7.59468</v>
+        <v>-6.7961</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-9.99</v>
+        <v>-8.13832</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-8.222060000000001</v>
+        <v>-7.78537</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46042.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-9.70499</v>
+        <v>-7.78335</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-10.47783</v>
+        <v>-10.7155</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-9.55391</v>
+        <v>-8.28947</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46042.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-8.21705</v>
+        <v>-8.179539999999999</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-9.465059999999999</v>
+        <v>-8.558400000000001</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46042.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-7.40455</v>
+        <v>-7.86778</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-6.37448</v>
+        <v>-6.42829</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-1.25798</v>
+        <v>-2.80319</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.72939</v>
+        <v>-5.51</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-0.1267</v>
+        <v>-1.01549</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>9.53589</v>
+        <v>9.46617</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46042.75</v>
       </c>
       <c r="B86" t="n">
-        <v>9.66465</v>
+        <v>9.59477</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>54.14803</v>
+        <v>31.01719</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>64.8901</v>
+        <v>57.3</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>64.8901</v>
+        <v>60.56861</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>59.32108</v>
+        <v>58.94198</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46042.875</v>
       </c>
       <c r="B92" t="n">
-        <v>58.56705</v>
+        <v>58.58436</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>57.98785</v>
+        <v>57.84212</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46042.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>59.44475</v>
+        <v>57.3</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>60.44065</v>
+        <v>58.86227</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>62.50152</v>
+        <v>61.45254</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 108)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -478,19 +478,19 @@
         <v>46041</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46041.22916666666</v>
+        <v>46041.25</v>
       </c>
       <c r="C2" t="n">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>20.79</v>
+        <v>22.68</v>
       </c>
       <c r="E2" t="n">
-        <v>509.8020524999999</v>
+        <v>567.7072635</v>
       </c>
       <c r="F2" t="n">
-        <v>24.52150324675324</v>
+        <v>25.03118445767196</v>
       </c>
     </row>
     <row r="3">
@@ -515,10 +515,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46041.95833333334</v>
+        <v>46041.97916666666</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46042.125</v>
+        <v>46042.14583333334</v>
       </c>
       <c r="C4" t="n">
         <v>4</v>
@@ -527,30 +527,30 @@
         <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>460.8246629999999</v>
+        <v>449.6219714999999</v>
       </c>
       <c r="F4" t="n">
-        <v>30.47782162698412</v>
+        <v>29.73690287698412</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46042.29166666666</v>
+        <v>46042.3125</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>46042.66666666666</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D5" t="n">
-        <v>34.02</v>
+        <v>32.13</v>
       </c>
       <c r="E5" t="n">
-        <v>-38.58871575000001</v>
+        <v>-105.39780225</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.134294995590829</v>
+        <v>-3.280354878618114</v>
       </c>
     </row>
   </sheetData>
@@ -847,7 +847,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
         <v>46041.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>-2.58035</v>
+        <v>0.45799</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1360,7 +1360,7 @@
         <v>46041.75</v>
       </c>
       <c r="B38" t="n">
-        <v>3.34464</v>
+        <v>11.89734</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,11 +1381,11 @@
         <v>46041.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>38.55471</v>
+        <v>0.01116</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
@@ -1402,11 +1402,11 @@
         <v>46041.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>57.18142</v>
+        <v>47.73914</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1423,7 +1423,7 @@
         <v>46041.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>64.53386</v>
+        <v>57.3</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46041.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>65</v>
+        <v>64.8901</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46041.875</v>
       </c>
       <c r="B44" t="n">
-        <v>65.37398</v>
+        <v>65</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>65.74816</v>
+        <v>65</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>59.50728</v>
+        <v>59.20766</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>64.8901</v>
+        <v>65</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1570,7 +1570,7 @@
         <v>46041.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>59.04126</v>
+        <v>59.77009</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
         <v>46041.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>63.32463</v>
+        <v>61.73053</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46042</v>
       </c>
       <c r="B50" t="n">
-        <v>61.17037</v>
+        <v>57.06003</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         <v>46042.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>60.8643</v>
+        <v>57.06003</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
         <v>46042.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>61.1294</v>
+        <v>57.06003</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1780,7 @@
         <v>46042.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>63.69192</v>
+        <v>64.06528</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46042.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>65</v>
+        <v>63.37713</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46042.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>65.21083</v>
+        <v>64.89</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46042.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>75.57516</v>
+        <v>68.88809999999999</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46042.25</v>
       </c>
       <c r="B62" t="n">
-        <v>77.94</v>
+        <v>76.59223</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>46042.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>75.76638</v>
+        <v>69.14248000000001</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
         <v>46042.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>8.85098</v>
+        <v>4.78431</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
         <v>46042.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.7</v>
+        <v>0.05444</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
         <v>46042.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.01108</v>
+        <v>0.0101</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46042.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-2.57556</v>
+        <v>-2.54301</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-7.01255</v>
+        <v>-7.17554</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46042.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-6.7961</v>
+        <v>-7.11442</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-8.13832</v>
+        <v>-7.93212</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-7.78537</v>
+        <v>-7.92499</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46042.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-7.78335</v>
+        <v>-6.91615</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-10.7155</v>
+        <v>-9.99</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         <v>46042.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-9.99</v>
+        <v>-10</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-8.28947</v>
+        <v>-11.01</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46042.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-8.179539999999999</v>
+        <v>-11.01</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-8.558400000000001</v>
+        <v>-11</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46042.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-7.86778</v>
+        <v>-7.86626</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-6.42829</v>
+        <v>-6.46667</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-2.80319</v>
+        <v>-5.14727</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-5.51</v>
+        <v>-5.74039</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-1.01549</v>
+        <v>-1.00044</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>9.46617</v>
+        <v>5.03982</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46042.75</v>
       </c>
       <c r="B86" t="n">
-        <v>9.59477</v>
+        <v>9.316129999999999</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>31.01719</v>
+        <v>33.11565</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>57.3</v>
+        <v>56.98</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2431,7 +2431,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>64.8901</v>
+        <v>59.2087</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>60.56861</v>
+        <v>60.12181</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>58.94198</v>
+        <v>58.92354</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46042.875</v>
       </c>
       <c r="B92" t="n">
-        <v>58.58436</v>
+        <v>58.14193</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>57.84212</v>
+        <v>57.82439</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>58.86227</v>
+        <v>58.85642</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>61.45254</v>
+        <v>61.43326</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 111)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -527,10 +527,10 @@
         <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>444.8536169999999</v>
+        <v>445.0877047499999</v>
       </c>
       <c r="F4" t="n">
-        <v>29.42153551587301</v>
+        <v>29.43701750992063</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +547,10 @@
         <v>34.02</v>
       </c>
       <c r="E5" t="n">
-        <v>-73.51220174999999</v>
+        <v>-67.72324649999999</v>
       </c>
       <c r="F5" t="n">
-        <v>-2.160852491181658</v>
+        <v>-1.990689197530864</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1465,7 @@
         <v>46041.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>59.9853</v>
+        <v>64.73678</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1507,11 +1507,11 @@
         <v>46041.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>59.14887</v>
+        <v>57.97172</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
@@ -1528,11 +1528,11 @@
         <v>46041.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>59.46714</v>
+        <v>64.30929</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
@@ -1549,7 +1549,7 @@
         <v>46041.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>58.71986</v>
+        <v>64.8901</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46042.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
         <v>46042.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
         <v>46042.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46042.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>64.89</v>
+        <v>63.21738</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46042.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>64.89</v>
+        <v>65</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46042.25</v>
       </c>
       <c r="B62" t="n">
-        <v>73.20005</v>
+        <v>74.81213</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>46042.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>61.4478</v>
+        <v>65</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         <v>46042.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>0.98766</v>
+        <v>4.56392</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1969,7 +1969,7 @@
         <v>46042.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>0.51</v>
+        <v>0.01106</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46042.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-1.17721</v>
+        <v>-1.16932</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-7.12181</v>
+        <v>-6.62984</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46042.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-7.42877</v>
+        <v>-6.67988</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-7.78472</v>
+        <v>-7.78287</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-7.73401</v>
+        <v>-7.77869</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46042.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-7.82489</v>
+        <v>-7.77671</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-9.99</v>
+        <v>-9.49592</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         <v>46042.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-9.99</v>
+        <v>-9.661490000000001</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-12.01</v>
+        <v>-11.01</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-10.39703</v>
+        <v>-11</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46042.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-8.38635</v>
+        <v>-8</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-5.56366</v>
+        <v>-5.7635</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>-1.01654</v>
+        <v>-2.71703</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>9.338240000000001</v>
+        <v>9.33845</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46042.75</v>
       </c>
       <c r="B86" t="n">
-        <v>9.46283</v>
+        <v>9.462870000000001</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>33.1597</v>
+        <v>33.16046</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>57.3</v>
+        <v>57.045</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>60.00844</v>
+        <v>60.58156</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>57.3</v>
+        <v>57.2442</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
         <v>46042.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>57.3</v>
+        <v>57.06003</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 114)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>15.12</v>
       </c>
       <c r="E2" t="n">
-        <v>471.22731825</v>
+        <v>472.3902105</v>
       </c>
       <c r="F2" t="n">
-        <v>31.1658279265873</v>
+        <v>31.24273878968254</v>
       </c>
     </row>
     <row r="3">
@@ -507,10 +507,10 @@
         <v>30.24</v>
       </c>
       <c r="E3" t="n">
-        <v>-96.83826750000001</v>
+        <v>-102.3364875</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.202323660714286</v>
+        <v>-3.384143105158731</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>459.2190524999999</v>
+        <v>456.03580425</v>
       </c>
       <c r="F4" t="n">
-        <v>30.3716304563492</v>
+        <v>30.16109816468254</v>
       </c>
     </row>
   </sheetData>
@@ -584,7 +584,7 @@
         <v>46042</v>
       </c>
       <c r="B2" t="n">
-        <v>60.66042</v>
+        <v>61.17104</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -605,7 +605,7 @@
         <v>46042.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>61.71008</v>
+        <v>61.72549</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -626,11 +626,11 @@
         <v>46042.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>60.73062</v>
+        <v>59.52981</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
@@ -689,7 +689,7 @@
         <v>46042.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>61.42246</v>
+        <v>61.97292</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -710,7 +710,7 @@
         <v>46042.125</v>
       </c>
       <c r="B8" t="n">
-        <v>61.45569</v>
+        <v>62.40669</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         <v>46042.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>63.21074</v>
+        <v>63.57677</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         <v>46042.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>63.70887</v>
+        <v>64.16336</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -773,7 +773,7 @@
         <v>46042.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>63.79789</v>
+        <v>64.66199</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -794,7 +794,7 @@
         <v>46042.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>73.20005</v>
+        <v>64.89</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
         <v>46042.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>77.31724</v>
+        <v>77.94</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -836,7 +836,7 @@
         <v>46042.25</v>
       </c>
       <c r="B14" t="n">
-        <v>77.55432999999999</v>
+        <v>82.12125</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
         <v>46042.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>65.01728</v>
+        <v>77.94</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
         <v>46042.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>56.98</v>
+        <v>57.06003</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -899,7 +899,7 @@
         <v>46042.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>8.664619999999999</v>
+        <v>8.663399999999999</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -941,7 +941,7 @@
         <v>46042.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>0.51</v>
+        <v>0.009979999999999999</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -962,7 +962,7 @@
         <v>46042.375</v>
       </c>
       <c r="B20" t="n">
-        <v>-2.57167</v>
+        <v>-1.16884</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -983,7 +983,7 @@
         <v>46042.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-5.79863</v>
+        <v>-6</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1004,7 +1004,7 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-6.69312</v>
+        <v>-6.77322</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         <v>46042.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-6.6436</v>
+        <v>-6.80232</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-8.16282</v>
+        <v>-8.71813</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1067,7 +1067,7 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-7.36918</v>
+        <v>-7.77209</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1088,7 +1088,7 @@
         <v>46042.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-7.78096</v>
+        <v>-7.82869</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1109,7 +1109,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-8.21973</v>
+        <v>-7.91751</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1130,7 +1130,7 @@
         <v>46042.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-8.30405</v>
+        <v>-9.95445</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1151,7 +1151,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-8.154210000000001</v>
+        <v>-10.15931</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1172,7 +1172,7 @@
         <v>46042.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-8.124079999999999</v>
+        <v>-9.41441</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1193,7 +1193,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-8.19622</v>
+        <v>-8.92239</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1214,7 +1214,7 @@
         <v>46042.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-7.71303</v>
+        <v>-7.86259</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1235,7 +1235,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-6.8</v>
+        <v>-6.37653</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1256,7 +1256,7 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-5.62569</v>
+        <v>-5.62607</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,7 +1277,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.75426</v>
+        <v>-5.84518</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1298,7 +1298,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-4.69714</v>
+        <v>-5.01</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1319,7 +1319,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>5.19843</v>
+        <v>5.19816</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>46042.75</v>
       </c>
       <c r="B38" t="n">
-        <v>13.93958</v>
+        <v>13.93879</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>46.7996</v>
+        <v>46.79821</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>57.3</v>
+        <v>59.66673</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1424,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>60.15202</v>
+        <v>59.05034</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1445,7 +1445,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>58.93813</v>
+        <v>57.3</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1466,7 +1466,7 @@
         <v>46042.875</v>
       </c>
       <c r="B44" t="n">
-        <v>57.78072</v>
+        <v>57.3</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>57.82215</v>
+        <v>57.77467</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1529,7 +1529,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>58.63908</v>
+        <v>58.63955</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1550,7 +1550,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>61.09695</v>
+        <v>61.09745</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1571,7 +1571,7 @@
         <v>46042.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>59.26485</v>
+        <v>59.26702</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 115)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,62 +475,42 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46042</v>
+        <v>46042.16666666666</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46042.16666666666</v>
+        <v>46042.66666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>15.12</v>
+        <v>45.36</v>
       </c>
       <c r="E2" t="n">
-        <v>472.3902105</v>
+        <v>353.00907525</v>
       </c>
       <c r="F2" t="n">
-        <v>31.24273878968254</v>
+        <v>7.782387020502645</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46042.33333333334</v>
+        <v>46042.83333333334</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46042.66666666666</v>
+        <v>46043</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>30.24</v>
+        <v>15.12</v>
       </c>
       <c r="E3" t="n">
-        <v>-102.3364875</v>
+        <v>458.182335</v>
       </c>
       <c r="F3" t="n">
-        <v>-3.384143105158731</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>46042.83333333334</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>46043</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E4" t="n">
-        <v>456.03580425</v>
-      </c>
-      <c r="F4" t="n">
-        <v>30.16109816468254</v>
+        <v>30.30306448412698</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,10 +561,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46042</v>
+        <v>46042.04166666666</v>
       </c>
       <c r="B2" t="n">
-        <v>61.17104</v>
+        <v>63.36879</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -596,16 +576,16 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46042.02083333334</v>
+        <v>46042.0625</v>
       </c>
       <c r="B3" t="n">
-        <v>61.72549</v>
+        <v>62.9731</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -617,16 +597,16 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46042.04166666666</v>
+        <v>46042.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>59.52981</v>
+        <v>61.92013</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -638,16 +618,16 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46042.0625</v>
+        <v>46042.10416666666</v>
       </c>
       <c r="B5" t="n">
-        <v>57.06003</v>
+        <v>62.75597</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -659,16 +639,16 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46042.08333333334</v>
+        <v>46042.125</v>
       </c>
       <c r="B6" t="n">
-        <v>57.06003</v>
+        <v>63.09551</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -680,16 +660,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46042.10416666666</v>
+        <v>46042.14583333334</v>
       </c>
       <c r="B7" t="n">
-        <v>61.97292</v>
+        <v>63.20409</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -701,16 +681,16 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46042.125</v>
+        <v>46042.16666666666</v>
       </c>
       <c r="B8" t="n">
-        <v>62.40669</v>
+        <v>63.68422</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -728,10 +708,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46042.14583333334</v>
+        <v>46042.1875</v>
       </c>
       <c r="B9" t="n">
-        <v>63.57677</v>
+        <v>62.87124</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -749,10 +729,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46042.16666666666</v>
+        <v>46042.20833333334</v>
       </c>
       <c r="B10" t="n">
-        <v>64.16336</v>
+        <v>65.27337</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -764,16 +744,16 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46042.1875</v>
+        <v>46042.22916666666</v>
       </c>
       <c r="B11" t="n">
-        <v>64.66199</v>
+        <v>65</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -785,16 +765,16 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46042.20833333334</v>
+        <v>46042.25</v>
       </c>
       <c r="B12" t="n">
-        <v>64.89</v>
+        <v>72.64717</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -806,16 +786,16 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46042.22916666666</v>
+        <v>46042.27083333334</v>
       </c>
       <c r="B13" t="n">
-        <v>77.94</v>
+        <v>65.80869</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -827,16 +807,16 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46042.25</v>
+        <v>46042.29166666666</v>
       </c>
       <c r="B14" t="n">
-        <v>82.12125</v>
+        <v>57.06003</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -848,16 +828,16 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46042.27083333334</v>
+        <v>46042.3125</v>
       </c>
       <c r="B15" t="n">
-        <v>77.94</v>
+        <v>8.661809999999999</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -869,16 +849,16 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46042.29166666666</v>
+        <v>46042.33333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>57.06003</v>
+        <v>0.7</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -890,16 +870,16 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46042.3125</v>
+        <v>46042.35416666666</v>
       </c>
       <c r="B17" t="n">
-        <v>8.663399999999999</v>
+        <v>0.009979999999999999</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -911,16 +891,16 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46042.33333333334</v>
+        <v>46042.375</v>
       </c>
       <c r="B18" t="n">
-        <v>0.7</v>
+        <v>-0.94718</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -938,10 +918,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46042.35416666666</v>
+        <v>46042.39583333334</v>
       </c>
       <c r="B19" t="n">
-        <v>0.009979999999999999</v>
+        <v>-5.50985</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -959,10 +939,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46042.375</v>
+        <v>46042.41666666666</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.16884</v>
+        <v>-7.22542</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -980,10 +960,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46042.39583333334</v>
+        <v>46042.4375</v>
       </c>
       <c r="B21" t="n">
-        <v>-6</v>
+        <v>-6.69694</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1001,10 +981,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46042.41666666666</v>
+        <v>46042.45833333334</v>
       </c>
       <c r="B22" t="n">
-        <v>-6.77322</v>
+        <v>-8.01695</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1022,10 +1002,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46042.4375</v>
+        <v>46042.47916666666</v>
       </c>
       <c r="B23" t="n">
-        <v>-6.80232</v>
+        <v>-8.06132</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1043,10 +1023,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46042.45833333334</v>
+        <v>46042.5</v>
       </c>
       <c r="B24" t="n">
-        <v>-8.71813</v>
+        <v>-8.16812</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1064,10 +1044,10 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46042.47916666666</v>
+        <v>46042.52083333334</v>
       </c>
       <c r="B25" t="n">
-        <v>-7.77209</v>
+        <v>-7.91811</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1085,10 +1065,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46042.5</v>
+        <v>46042.54166666666</v>
       </c>
       <c r="B26" t="n">
-        <v>-7.82869</v>
+        <v>-8.165319999999999</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1106,10 +1086,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>46042.52083333334</v>
+        <v>46042.5625</v>
       </c>
       <c r="B27" t="n">
-        <v>-7.91751</v>
+        <v>-8.23887</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1127,10 +1107,10 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>46042.54166666666</v>
+        <v>46042.58333333334</v>
       </c>
       <c r="B28" t="n">
-        <v>-9.95445</v>
+        <v>-8.676970000000001</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1148,10 +1128,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>46042.5625</v>
+        <v>46042.60416666666</v>
       </c>
       <c r="B29" t="n">
-        <v>-10.15931</v>
+        <v>-8.08089</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1169,10 +1149,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>46042.58333333334</v>
+        <v>46042.625</v>
       </c>
       <c r="B30" t="n">
-        <v>-9.41441</v>
+        <v>-7.6109</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1190,10 +1170,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>46042.60416666666</v>
+        <v>46042.64583333334</v>
       </c>
       <c r="B31" t="n">
-        <v>-8.92239</v>
+        <v>-6.33908</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1211,10 +1191,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>46042.625</v>
+        <v>46042.66666666666</v>
       </c>
       <c r="B32" t="n">
-        <v>-7.86259</v>
+        <v>-5.66097</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1226,16 +1206,16 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>46042.64583333334</v>
+        <v>46042.6875</v>
       </c>
       <c r="B33" t="n">
-        <v>-6.37653</v>
+        <v>-5.78922</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1247,16 +1227,16 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>46042.66666666666</v>
+        <v>46042.70833333334</v>
       </c>
       <c r="B34" t="n">
-        <v>-5.62607</v>
+        <v>-4.62645</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1274,10 +1254,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>46042.6875</v>
+        <v>46042.72916666666</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.84518</v>
+        <v>5.10151</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1295,10 +1275,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>46042.70833333334</v>
+        <v>46042.75</v>
       </c>
       <c r="B36" t="n">
-        <v>-5.01</v>
+        <v>13.92238</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1316,10 +1296,10 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>46042.72916666666</v>
+        <v>46042.77083333334</v>
       </c>
       <c r="B37" t="n">
-        <v>5.19816</v>
+        <v>46.71435</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1337,10 +1317,10 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>46042.75</v>
+        <v>46042.79166666666</v>
       </c>
       <c r="B38" t="n">
-        <v>13.93879</v>
+        <v>57.3</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1358,10 +1338,10 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>46042.77083333334</v>
+        <v>46042.8125</v>
       </c>
       <c r="B39" t="n">
-        <v>46.79821</v>
+        <v>57.3</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1379,10 +1359,10 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>46042.79166666666</v>
+        <v>46042.83333333334</v>
       </c>
       <c r="B40" t="n">
-        <v>57.3</v>
+        <v>60.10762</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1394,16 +1374,16 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>46042.8125</v>
+        <v>46042.85416666666</v>
       </c>
       <c r="B41" t="n">
-        <v>59.66673</v>
+        <v>58.10932</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1415,16 +1395,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>46042.83333333334</v>
+        <v>46042.875</v>
       </c>
       <c r="B42" t="n">
-        <v>59.05034</v>
+        <v>57.3</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1442,10 +1422,10 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>46042.85416666666</v>
+        <v>46042.89583333334</v>
       </c>
       <c r="B43" t="n">
-        <v>57.3</v>
+        <v>57.77405</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1463,7 +1443,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>46042.875</v>
+        <v>46042.91666666666</v>
       </c>
       <c r="B44" t="n">
         <v>57.3</v>
@@ -1484,10 +1464,10 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>46042.89583333334</v>
+        <v>46042.9375</v>
       </c>
       <c r="B45" t="n">
-        <v>57.77467</v>
+        <v>58.98951</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1505,10 +1485,10 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>46042.91666666666</v>
+        <v>46042.95833333334</v>
       </c>
       <c r="B46" t="n">
-        <v>57.3</v>
+        <v>61.09895</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1526,10 +1506,10 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46042.9375</v>
+        <v>46042.97916666666</v>
       </c>
       <c r="B47" t="n">
-        <v>58.63955</v>
+        <v>59.25115</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1540,48 +1520,6 @@
         <v>46042</v>
       </c>
       <c r="E47" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
-        <v>46042.95833333334</v>
-      </c>
-      <c r="B48" t="n">
-        <v>61.09745</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>forecast</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="n">
-        <v>46042</v>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
-        <v>46042.97916666666</v>
-      </c>
-      <c r="B49" t="n">
-        <v>59.26702</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>forecast</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="n">
-        <v>46042</v>
-      </c>
-      <c r="E49" t="inlineStr">
         <is>
           <t>ON</t>
         </is>

</xml_diff>

<commit_message>
Update latest output (run 122)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,62 +475,22 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46042.02083333334</v>
+        <v>46042</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46042.1875</v>
+        <v>46042.66666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>15.12</v>
+        <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>445.0682339999999</v>
+        <v>807.3803789999996</v>
       </c>
       <c r="F2" t="n">
-        <v>29.43572976190476</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>46042.33333333334</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>46042.66666666666</v>
-      </c>
-      <c r="C3" t="n">
-        <v>8</v>
-      </c>
-      <c r="D3" t="n">
-        <v>30.24</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-90.41875049999999</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-2.99003804563492</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>46042.83333333334</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>46043</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E4" t="n">
-        <v>455.88185175</v>
-      </c>
-      <c r="F4" t="n">
-        <v>30.15091612103175</v>
+        <v>13.34954330357142</v>
       </c>
     </row>
   </sheetData>
@@ -596,7 +556,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -785,7 +745,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -806,7 +766,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -827,7 +787,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -848,7 +808,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -869,7 +829,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -878,7 +838,7 @@
         <v>46042.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>59.50691</v>
+        <v>56.98</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -890,7 +850,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -899,7 +859,7 @@
         <v>46042.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>55.74071</v>
+        <v>8.61645</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -911,7 +871,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -920,7 +880,7 @@
         <v>46042.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>0.7</v>
+        <v>0.01928</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -941,11 +901,11 @@
         <v>46042.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>0.7</v>
+        <v>8.682</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
@@ -962,11 +922,11 @@
         <v>46042.375</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.10419</v>
+        <v>-5.51</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
@@ -983,7 +943,7 @@
         <v>46042.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-6</v>
+        <v>-6.19659</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1004,7 +964,7 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-6.96611</v>
+        <v>-6.32</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1025,7 +985,7 @@
         <v>46042.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-6.52029</v>
+        <v>-6.36387</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1046,7 +1006,7 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-8.36323</v>
+        <v>-7.22044</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1067,7 +1027,7 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-7.52604</v>
+        <v>-7.25296</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1088,7 +1048,7 @@
         <v>46042.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-7.07444</v>
+        <v>-6.09234</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1109,7 +1069,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-7.23757</v>
+        <v>-7.2065</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1130,7 +1090,7 @@
         <v>46042.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-7.39814</v>
+        <v>-8.84238</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1151,7 +1111,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-7.79441</v>
+        <v>-7.79956</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1172,7 +1132,7 @@
         <v>46042.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-7.86722</v>
+        <v>-7.37432</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1193,7 +1153,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-7.94014</v>
+        <v>-7.37879</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1214,7 +1174,7 @@
         <v>46042.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.3454</v>
+        <v>-6.36144</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1235,7 +1195,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-6</v>
+        <v>-5.51</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1256,7 +1216,7 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.93093</v>
+        <v>0.7</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1277,7 +1237,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.07225</v>
+        <v>-1.11816</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1298,7 +1258,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>-2.78511</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1319,7 +1279,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>9.63571</v>
+        <v>9.916370000000001</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1340,7 +1300,7 @@
         <v>46042.75</v>
       </c>
       <c r="B38" t="n">
-        <v>14.17313</v>
+        <v>9.979480000000001</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1361,7 +1321,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>33.15789</v>
+        <v>33.15828</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1403,7 +1363,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1424,7 +1384,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>62.17261</v>
+        <v>59.77564</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1436,7 +1396,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1445,7 +1405,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>58.2352</v>
+        <v>59.66166</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1457,7 +1417,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1426,7 @@
         <v>46042.875</v>
       </c>
       <c r="B44" t="n">
-        <v>57.47977</v>
+        <v>57.91165</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1478,7 +1438,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1447,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>57.3</v>
+        <v>56.98</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1499,7 +1459,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1480,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1541,7 +1501,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1550,7 +1510,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>60.80355</v>
+        <v>57.3</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1562,7 +1522,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1531,7 @@
         <v>46042.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>57.3</v>
+        <v>57.06003</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1583,7 +1543,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update latest output (run 123)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>807.3803789999996</v>
+        <v>824.4666592499998</v>
       </c>
       <c r="F2" t="n">
-        <v>13.34954330357142</v>
+        <v>13.63205455109127</v>
       </c>
     </row>
   </sheetData>
@@ -880,7 +880,7 @@
         <v>46042.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>0.01928</v>
+        <v>3.55269</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>46042.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>8.682</v>
+        <v>0.7</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         <v>46042.375</v>
       </c>
       <c r="B20" t="n">
-        <v>-5.51</v>
+        <v>0.009379999999999999</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -943,11 +943,11 @@
         <v>46042.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-6.19659</v>
+        <v>0.0005</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
@@ -964,11 +964,11 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-6.32</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
@@ -985,7 +985,7 @@
         <v>46042.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-6.36387</v>
+        <v>-2.91592</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1006,7 +1006,7 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-7.22044</v>
+        <v>-6.40473</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-7.25296</v>
+        <v>-6.14838</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1048,7 +1048,7 @@
         <v>46042.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-6.09234</v>
+        <v>-6.33429</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-7.2065</v>
+        <v>-7.11669</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46042.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-8.84238</v>
+        <v>-8.96598</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-7.79956</v>
+        <v>-8.18792</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46042.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-7.37432</v>
+        <v>-8.118080000000001</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-7.37879</v>
+        <v>-7.54132</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46042.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.36144</v>
+        <v>-6.46636</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-5.51</v>
+        <v>-5.26642</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-1.11816</v>
+        <v>-0.9120200000000001</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>1e-05</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>9.916370000000001</v>
+        <v>22.05184</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46042.75</v>
       </c>
       <c r="B38" t="n">
-        <v>9.979480000000001</v>
+        <v>30.06361</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>33.15828</v>
+        <v>47.37894</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>56.98</v>
+        <v>60.85009</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>57.3</v>
+        <v>57.22391</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>59.77564</v>
+        <v>62.22274</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>59.66166</v>
+        <v>57.59874</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46042.875</v>
       </c>
       <c r="B44" t="n">
-        <v>57.91165</v>
+        <v>58.85308</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>56.98</v>
+        <v>57.3</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46042.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.98</v>
+        <v>57.06007</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.3</v>
+        <v>58.6455</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.3</v>
+        <v>61.33335</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>46042.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>57.06003</v>
+        <v>57.3</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 124)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -487,10 +487,10 @@
         <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>824.4666592499998</v>
+        <v>848.1402832499998</v>
       </c>
       <c r="F2" t="n">
-        <v>13.63205455109127</v>
+        <v>14.02348351934524</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +943,7 @@
         <v>46042.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0005</v>
+        <v>-5.01</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -964,7 +964,7 @@
         <v>46042.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>-6.73332</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -985,11 +985,11 @@
         <v>46042.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-2.91592</v>
+        <v>-6.52883</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
@@ -1006,11 +1006,11 @@
         <v>46042.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-6.40473</v>
+        <v>-7.88121</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
@@ -1027,11 +1027,11 @@
         <v>46042.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-6.14838</v>
+        <v>0</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
@@ -1048,11 +1048,11 @@
         <v>46042.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-6.33429</v>
+        <v>0.7</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
@@ -1069,7 +1069,7 @@
         <v>46042.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-7.11669</v>
+        <v>0.02274</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
         <v>46042.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-8.96598</v>
+        <v>-1.16054</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         <v>46042.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-8.18792</v>
+        <v>-5.58973</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         <v>46042.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-8.118080000000001</v>
+        <v>-5.48208</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>46042.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-7.54132</v>
+        <v>-2.54301</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>46042.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.46636</v>
+        <v>-6</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-5.26642</v>
+        <v>-2.97897</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>0.7</v>
+        <v>36.0601</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.9120200000000001</v>
+        <v>24.59223</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>1e-05</v>
+        <v>9.847939999999999</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>22.05184</v>
+        <v>36.0601</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1300,7 +1300,7 @@
         <v>46042.75</v>
       </c>
       <c r="B38" t="n">
-        <v>30.06361</v>
+        <v>47.41716</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>47.37894</v>
+        <v>64.02958</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>60.85009</v>
+        <v>64.82379</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1363,7 +1363,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>57.22391</v>
+        <v>64.8901</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1384,7 +1384,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>62.22274</v>
+        <v>63.94385</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>57.59874</v>
+        <v>60.4431</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
         <v>46042.875</v>
       </c>
       <c r="B44" t="n">
-        <v>58.85308</v>
+        <v>59.81888</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>57.3</v>
+        <v>58.2941</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
         <v>46042.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.06007</v>
+        <v>57.3</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1489,7 +1489,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>58.6455</v>
+        <v>58.81822</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1510,7 +1510,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>61.33335</v>
+        <v>61.0907</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 127)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -507,10 +507,10 @@
         <v>34.02</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.811704999999982</v>
+        <v>-10.54730624999998</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0826485890652552</v>
+        <v>-0.3100325176366838</v>
       </c>
     </row>
     <row r="4">
@@ -527,10 +527,10 @@
         <v>18.9</v>
       </c>
       <c r="E4" t="n">
-        <v>575.5282845</v>
+        <v>572.3830124999999</v>
       </c>
       <c r="F4" t="n">
-        <v>30.45123198412699</v>
+        <v>30.28481547619048</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +547,10 @@
         <v>34.02</v>
       </c>
       <c r="E5" t="n">
-        <v>-185.71424625</v>
+        <v>-168.28144125</v>
       </c>
       <c r="F5" t="n">
-        <v>-5.458972552910054</v>
+        <v>-4.946544422398589</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1234,7 @@
         <v>46042.625</v>
       </c>
       <c r="B32" t="n">
-        <v>14.00051</v>
+        <v>-7.85287</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1255,7 +1255,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>0.00048</v>
+        <v>13.91991</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1276,11 +1276,11 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>10.31935</v>
+        <v>24.7014</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D34" s="3" t="n">
@@ -1297,7 +1297,7 @@
         <v>46042.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>22.07</v>
+        <v>26.41646</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>25.73712</v>
+        <v>54.0145</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>49.80515</v>
+        <v>50.52352</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1360,7 +1360,7 @@
         <v>46042.75</v>
       </c>
       <c r="B38" t="n">
-        <v>57.3</v>
+        <v>58.57113</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>63.92984</v>
+        <v>64.31851</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>65</v>
+        <v>67.69738</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>66.16136</v>
+        <v>76.61194</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>73.20007</v>
+        <v>77.94</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>71.92849</v>
+        <v>72.82266</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46042.875</v>
       </c>
       <c r="B44" t="n">
-        <v>68.79257</v>
+        <v>71.72403</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>63.47425</v>
+        <v>63.77459</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>63.96083</v>
+        <v>63.57817</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1570,7 +1570,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>62.40305</v>
+        <v>62.04848</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46042.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>61.34585</v>
+        <v>61.77267</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46043</v>
       </c>
       <c r="B50" t="n">
-        <v>59.97554</v>
+        <v>57.06003</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46043.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>67.70496</v>
+        <v>72.00874</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46043.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>73.20005</v>
+        <v>77.71132</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46043.25</v>
       </c>
       <c r="B62" t="n">
-        <v>79.95016</v>
+        <v>81.40685999999999</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>46043.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>67.70788</v>
+        <v>73.20005</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>46043.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>56.98</v>
+        <v>53.27499</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         <v>46043.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>0.7</v>
+        <v>0.9831800000000001</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
         <v>46043.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.51002</v>
+        <v>0.009650000000000001</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46043.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-6.54017</v>
+        <v>-6.08274</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         <v>46043.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-6.96691</v>
+        <v>-6.96614</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46043.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-8.566689999999999</v>
+        <v>-8.786479999999999</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46043.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-9.75165</v>
+        <v>-9.5</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46043.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-15.60246</v>
+        <v>-15.04586</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46043.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-22.35626</v>
+        <v>-18.19399</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46043.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-22.90284</v>
+        <v>-16.79318</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46043.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-23.5</v>
+        <v>-22.40926</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
         <v>46043.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-27</v>
+        <v>-23.5</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46043.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-23.93719</v>
+        <v>-21.03239</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46043.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-23.13936</v>
+        <v>-23.5</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46043.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-22.06328</v>
+        <v>-18.71477</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46043.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-5.74405</v>
+        <v>-5.72703</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46043.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>46.3101</v>
+        <v>46.59793</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46043.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>65</v>
+        <v>69.05019</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46043.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>78</v>
+        <v>100.01</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46043.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>86.97678000000001</v>
+        <v>87.00089</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46043.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>73.75449</v>
+        <v>73.78428</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46043.875</v>
       </c>
       <c r="B92" t="n">
-        <v>70.0634</v>
+        <v>70.50577</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46043.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>60.2421</v>
+        <v>60.25514</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 128)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -507,10 +507,10 @@
         <v>34.02</v>
       </c>
       <c r="E3" t="n">
-        <v>-10.54730624999998</v>
+        <v>-30.35730749999998</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3100325176366838</v>
+        <v>-0.8923370811287473</v>
       </c>
     </row>
     <row r="4">
@@ -518,39 +518,39 @@
         <v>46042.91666666666</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46043.125</v>
+        <v>46043.14583333334</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="D4" t="n">
-        <v>18.9</v>
+        <v>20.79</v>
       </c>
       <c r="E4" t="n">
-        <v>572.3830124999999</v>
+        <v>619.4632859999999</v>
       </c>
       <c r="F4" t="n">
-        <v>30.28481547619048</v>
+        <v>29.79621385281385</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46043.29166666666</v>
+        <v>46043.3125</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>46043.66666666666</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D5" t="n">
-        <v>34.02</v>
+        <v>32.13</v>
       </c>
       <c r="E5" t="n">
-        <v>-168.28144125</v>
+        <v>-226.12220475</v>
       </c>
       <c r="F5" t="n">
-        <v>-4.946544422398589</v>
+        <v>-7.037728127917834</v>
       </c>
     </row>
   </sheetData>
@@ -1255,7 +1255,7 @@
         <v>46042.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>13.91991</v>
+        <v>-6.39804</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1276,7 +1276,7 @@
         <v>46042.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>24.7014</v>
+        <v>-5.51</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1297,11 +1297,11 @@
         <v>46042.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>26.41646</v>
+        <v>22.07</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D35" s="3" t="n">
@@ -1318,11 +1318,11 @@
         <v>46042.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>54.0145</v>
+        <v>36.07</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D36" s="3" t="n">
@@ -1339,11 +1339,11 @@
         <v>46042.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>50.52352</v>
+        <v>50.8425</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D37" s="3" t="n">
@@ -1360,7 +1360,7 @@
         <v>46042.75</v>
       </c>
       <c r="B38" t="n">
-        <v>58.57113</v>
+        <v>60.35108</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
         <v>46042.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>64.31851</v>
+        <v>63.74797</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         <v>46042.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>67.69738</v>
+        <v>73.94592</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>46042.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>76.61194</v>
+        <v>75.72364</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1444,7 +1444,7 @@
         <v>46042.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>77.94</v>
+        <v>78</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         <v>46042.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>72.82266</v>
+        <v>76.20085</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1486,7 +1486,7 @@
         <v>46042.875</v>
       </c>
       <c r="B44" t="n">
-        <v>71.72403</v>
+        <v>69.69265</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         <v>46042.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>63.77459</v>
+        <v>63.79708</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>46042.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>63.57817</v>
+        <v>64.26672000000001</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1570,7 +1570,7 @@
         <v>46042.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>62.04848</v>
+        <v>57.3</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
         <v>46042.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>61.77267</v>
+        <v>57.06003</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1780,7 +1780,7 @@
         <v>46043.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>65</v>
+        <v>65.94062</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1801,7 @@
         <v>46043.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>72.00874</v>
+        <v>67.70805</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         <v>46043.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>77.71132</v>
+        <v>72.01038</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46043.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>79.95022</v>
+        <v>79.36201</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46043.25</v>
       </c>
       <c r="B62" t="n">
-        <v>81.40685999999999</v>
+        <v>80.45009</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>46043.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>73.20005</v>
+        <v>68.98878999999999</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>46043.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>53.27499</v>
+        <v>57.06012</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
         <v>46043.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>0.9831800000000001</v>
+        <v>0.7</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
         <v>46043.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.009650000000000001</v>
+        <v>0.009719999999999999</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>46043.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-6.08274</v>
+        <v>-6.62812</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +2011,7 @@
         <v>46043.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-6.96614</v>
+        <v>-6.99226</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         <v>46043.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-8.786479999999999</v>
+        <v>-8.691649999999999</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46043.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-9.5</v>
+        <v>-8.85641</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46043.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-15.04586</v>
+        <v>-14</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46043.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-18.19399</v>
+        <v>-14.49854</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46043.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-16.79318</v>
+        <v>-16.35771</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46043.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-22.40926</v>
+        <v>-23.07171</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         <v>46043.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-23.5</v>
+        <v>-22.40654</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2200,7 +2200,7 @@
         <v>46043.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>-21.03239</v>
+        <v>-23.5</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2221,7 @@
         <v>46043.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-23.5</v>
+        <v>-23.78763</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         <v>46043.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-18.71477</v>
+        <v>-23.5</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>46043.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
         <v>46043.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>-5.72703</v>
+        <v>-6.40066</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46043.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.03998</v>
+        <v>-4.61188</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46043.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>46.59793</v>
+        <v>46.9682</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46043.75</v>
       </c>
       <c r="B86" t="n">
-        <v>56.98</v>
+        <v>56.52321</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46043.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>69.05019</v>
+        <v>65</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46043.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>100.01</v>
+        <v>77.94</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2431,7 +2431,7 @@
         <v>46043.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>105.0001</v>
+        <v>105.79</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46043.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>87.00089</v>
+        <v>79.95</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46043.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>73.78428</v>
+        <v>73.82011</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46043.875</v>
       </c>
       <c r="B92" t="n">
-        <v>70.50577</v>
+        <v>70.12006</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2536,7 +2536,7 @@
         <v>46043.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>60.25514</v>
+        <v>60.27702</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 135)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,30 +475,30 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46046</v>
+        <v>46047.125</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46046.16666666666</v>
+        <v>46047.79166666666</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>15.12</v>
+        <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>484.598634</v>
+        <v>1032.875181</v>
       </c>
       <c r="F2" t="n">
-        <v>32.05017420634921</v>
+        <v>17.07796264880953</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46046.25</v>
+        <v>46048.16666666666</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46046.75</v>
+        <v>46048.66666666666</v>
       </c>
       <c r="C3" t="n">
         <v>12</v>
@@ -507,30 +507,10 @@
         <v>45.36</v>
       </c>
       <c r="E3" t="n">
-        <v>-31.60218749999996</v>
+        <v>602.3204655</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.6966972552910045</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>46047.25</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>46047.75</v>
-      </c>
-      <c r="C4" t="n">
-        <v>12</v>
-      </c>
-      <c r="D4" t="n">
-        <v>45.36</v>
-      </c>
-      <c r="E4" t="n">
-        <v>363.4444515000001</v>
-      </c>
-      <c r="F4" t="n">
-        <v>8.012443816137568</v>
+        <v>13.27866987433862</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +561,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="B2" t="n">
-        <v>58.62625</v>
+        <v>105.79</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -592,20 +572,20 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46046.02083333334</v>
+        <v>46047.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>62.9804</v>
+        <v>106.85676</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -613,20 +593,20 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46046.04166666666</v>
+        <v>46047.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>60.41283</v>
+        <v>102.06314</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -634,20 +614,20 @@
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46046.0625</v>
+        <v>46047.0625</v>
       </c>
       <c r="B5" t="n">
-        <v>59.44281</v>
+        <v>103.56233</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -655,20 +635,20 @@
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46046.08333333334</v>
+        <v>46047.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>62.15064</v>
+        <v>103.26745</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -676,20 +656,20 @@
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46046.10416666666</v>
+        <v>46047.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>63.41131</v>
+        <v>105.00005</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -697,20 +677,20 @@
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46046.125</v>
+        <v>46047.125</v>
       </c>
       <c r="B8" t="n">
-        <v>65</v>
+        <v>103.7033</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -718,7 +698,7 @@
         </is>
       </c>
       <c r="D8" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -728,10 +708,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46046.14583333334</v>
+        <v>46047.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>65</v>
+        <v>96.28724</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -739,7 +719,7 @@
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -749,10 +729,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46046.16666666666</v>
+        <v>46047.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>65</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -760,20 +740,20 @@
         </is>
       </c>
       <c r="D10" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46046.1875</v>
+        <v>46047.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>64.41839</v>
+        <v>85.39851</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -781,20 +761,20 @@
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46046.20833333334</v>
+        <v>46047.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>64.78185000000001</v>
+        <v>100.52719</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -802,20 +782,20 @@
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46046.22916666666</v>
+        <v>46047.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>65</v>
+        <v>101.25</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -823,20 +803,20 @@
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46046.25</v>
+        <v>46047.25</v>
       </c>
       <c r="B14" t="n">
-        <v>63.63117</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -844,7 +824,7 @@
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -854,10 +834,10 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46046.27083333334</v>
+        <v>46047.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>57.06</v>
+        <v>62.29062</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -865,7 +845,7 @@
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -875,10 +855,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46046.29166666666</v>
+        <v>46047.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>36.06</v>
+        <v>51.08363</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -886,7 +866,7 @@
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -896,10 +876,10 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46046.3125</v>
+        <v>46047.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>0.009560000000000001</v>
+        <v>14.25158</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -907,7 +887,7 @@
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -917,10 +897,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46046.33333333334</v>
+        <v>46047.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>-5.66875</v>
+        <v>4.97668</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -928,7 +908,7 @@
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -938,10 +918,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46046.35416666666</v>
+        <v>46047.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>-6.5916</v>
+        <v>-1.05379</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -949,7 +929,7 @@
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -959,10 +939,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46046.375</v>
+        <v>46047.375</v>
       </c>
       <c r="B20" t="n">
-        <v>-7.6138</v>
+        <v>-2.83936</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -970,7 +950,7 @@
         </is>
       </c>
       <c r="D20" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -980,10 +960,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46046.39583333334</v>
+        <v>46047.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>-13.5</v>
+        <v>-5.50985</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -991,7 +971,7 @@
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1001,10 +981,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46046.41666666666</v>
+        <v>46047.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>-21.22764</v>
+        <v>-6.14392</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1012,7 +992,7 @@
         </is>
       </c>
       <c r="D22" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1022,10 +1002,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46046.4375</v>
+        <v>46047.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>-20.5462</v>
+        <v>-6.16116</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1033,7 +1013,7 @@
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1043,10 +1023,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46046.45833333334</v>
+        <v>46047.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>-17.19456</v>
+        <v>-6.08048</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1054,7 +1034,7 @@
         </is>
       </c>
       <c r="D24" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1064,10 +1044,10 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46046.47916666666</v>
+        <v>46047.47916666666</v>
       </c>
       <c r="B25" t="n">
-        <v>-19.98</v>
+        <v>-6.31978</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1075,7 +1055,7 @@
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1085,10 +1065,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46046.5</v>
+        <v>46047.5</v>
       </c>
       <c r="B26" t="n">
-        <v>-23.5</v>
+        <v>-6.3699</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1096,7 +1076,7 @@
         </is>
       </c>
       <c r="D26" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1106,10 +1086,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>46046.52083333334</v>
+        <v>46047.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-19.1221</v>
+        <v>-7.07031</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1117,7 +1097,7 @@
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1127,10 +1107,10 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>46046.54166666666</v>
+        <v>46047.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-23.5</v>
+        <v>-6.44209</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1138,7 +1118,7 @@
         </is>
       </c>
       <c r="D28" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1148,10 +1128,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>46046.5625</v>
+        <v>46047.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-19.90312</v>
+        <v>-5.06689</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1159,7 +1139,7 @@
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1169,10 +1149,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>46046.58333333334</v>
+        <v>46047.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>-12.01</v>
+        <v>5.65972</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1180,7 +1160,7 @@
         </is>
       </c>
       <c r="D30" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1190,10 +1170,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>46046.60416666666</v>
+        <v>46047.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>-6.83624</v>
+        <v>-0.89269</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1201,7 +1181,7 @@
         </is>
       </c>
       <c r="D31" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1211,10 +1191,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>46046.625</v>
+        <v>46047.625</v>
       </c>
       <c r="B32" t="n">
-        <v>-5.92803</v>
+        <v>-1.49465</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1222,7 +1202,7 @@
         </is>
       </c>
       <c r="D32" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1232,10 +1212,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>46046.64583333334</v>
+        <v>46047.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>-6</v>
+        <v>0.40115</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1243,7 +1223,7 @@
         </is>
       </c>
       <c r="D33" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1253,10 +1233,10 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>46046.66666666666</v>
+        <v>46047.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>-4.89</v>
+        <v>2.68496</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1264,7 +1244,7 @@
         </is>
       </c>
       <c r="D34" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1274,10 +1254,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>46046.6875</v>
+        <v>46047.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>-4.91236</v>
+        <v>48.75844</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1285,7 +1265,7 @@
         </is>
       </c>
       <c r="D35" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1295,10 +1275,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>46046.70833333334</v>
+        <v>46047.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>0.51</v>
+        <v>71.27915</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1306,7 +1286,7 @@
         </is>
       </c>
       <c r="D36" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1316,10 +1296,10 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>46046.72916666666</v>
+        <v>46047.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>49.24117</v>
+        <v>36.25</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1327,7 +1307,7 @@
         </is>
       </c>
       <c r="D37" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1337,10 +1317,10 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>46046.75</v>
+        <v>46047.75</v>
       </c>
       <c r="B38" t="n">
-        <v>66.35997</v>
+        <v>64.65661</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1348,49 +1328,49 @@
         </is>
       </c>
       <c r="D38" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>46046.77083333334</v>
+        <v>46047.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>83.01918999999999</v>
+        <v>101.76525</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>46046.79166666666</v>
+        <v>46047.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>119.83444</v>
+        <v>190</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1400,18 +1380,18 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>46046.8125</v>
+        <v>46047.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>147.04151</v>
+        <v>146.77654</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1421,18 +1401,18 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>46046.83333333334</v>
+        <v>46047.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>147.51746</v>
+        <v>146.9771</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1442,18 +1422,18 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>46046.85416666666</v>
+        <v>46047.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>186.23306</v>
+        <v>234.34183</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1463,18 +1443,18 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>46046.875</v>
+        <v>46047.875</v>
       </c>
       <c r="B44" t="n">
-        <v>138.42</v>
+        <v>206.08201</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1484,18 +1464,18 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>46046.89583333334</v>
+        <v>46047.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>116.49262</v>
+        <v>147.51</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1505,18 +1485,18 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>46046.91666666666</v>
+        <v>46047.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>108.89</v>
+        <v>120.89</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1526,18 +1506,18 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46046.9375</v>
+        <v>46047.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>101.25</v>
+        <v>147.52</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1547,18 +1527,18 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>46046.95833333334</v>
+        <v>46047.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>102.30723</v>
+        <v>108.89</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1568,10 +1548,10 @@
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>46046.97916666666</v>
+        <v>46047.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>105.79</v>
+        <v>101.25</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1579,7 +1559,7 @@
         </is>
       </c>
       <c r="D49" s="3" t="n">
-        <v>46046</v>
+        <v>46047</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1589,10 +1569,10 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="B50" t="n">
-        <v>105.79</v>
+        <v>96.54971</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1600,7 +1580,7 @@
         </is>
       </c>
       <c r="D50" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1610,10 +1590,10 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>46047.02083333334</v>
+        <v>46048.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>124.32627</v>
+        <v>89.76787</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1621,7 +1601,7 @@
         </is>
       </c>
       <c r="D51" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1631,10 +1611,10 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>46047.04166666666</v>
+        <v>46048.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>105.79</v>
+        <v>72.58583</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1642,7 +1622,7 @@
         </is>
       </c>
       <c r="D52" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1652,10 +1632,10 @@
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>46047.0625</v>
+        <v>46048.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>105.79</v>
+        <v>65</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1663,7 +1643,7 @@
         </is>
       </c>
       <c r="D53" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1673,10 +1653,10 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>46047.08333333334</v>
+        <v>46048.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>103.78068</v>
+        <v>58.71341</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1684,7 +1664,7 @@
         </is>
       </c>
       <c r="D54" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1694,10 +1674,10 @@
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>46047.10416666666</v>
+        <v>46048.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>105.00005</v>
+        <v>58.46663</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1705,7 +1685,7 @@
         </is>
       </c>
       <c r="D55" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1715,10 +1695,10 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>46047.125</v>
+        <v>46048.125</v>
       </c>
       <c r="B56" t="n">
-        <v>105.00005</v>
+        <v>59.2025</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1726,7 +1706,7 @@
         </is>
       </c>
       <c r="D56" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1736,10 +1716,10 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>46047.14583333334</v>
+        <v>46048.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>105.35984</v>
+        <v>59.60614</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1747,7 +1727,7 @@
         </is>
       </c>
       <c r="D57" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1757,10 +1737,10 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>46047.16666666666</v>
+        <v>46048.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>87.60003</v>
+        <v>58.60513</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1768,20 +1748,20 @@
         </is>
       </c>
       <c r="D58" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>46047.1875</v>
+        <v>46048.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>98.25972</v>
+        <v>65</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1789,20 +1769,20 @@
         </is>
       </c>
       <c r="D59" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>46047.20833333334</v>
+        <v>46048.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>103.39668</v>
+        <v>66.64578</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1810,20 +1790,20 @@
         </is>
       </c>
       <c r="D60" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>46047.22916666666</v>
+        <v>46048.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>102.36287</v>
+        <v>69.79337</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1831,20 +1811,20 @@
         </is>
       </c>
       <c r="D61" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>46047.25</v>
+        <v>46048.25</v>
       </c>
       <c r="B62" t="n">
-        <v>99.50184</v>
+        <v>65</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1852,7 +1832,7 @@
         </is>
       </c>
       <c r="D62" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1862,10 +1842,10 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>46047.27083333334</v>
+        <v>46048.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>62.29726</v>
+        <v>41.74372</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1873,7 +1853,7 @@
         </is>
       </c>
       <c r="D63" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1883,10 +1863,10 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>46047.29166666666</v>
+        <v>46048.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>51.22225</v>
+        <v>35.88</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1894,7 +1874,7 @@
         </is>
       </c>
       <c r="D64" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1904,10 +1884,10 @@
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>46047.3125</v>
+        <v>46048.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>19.80149</v>
+        <v>35.88</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1915,7 +1895,7 @@
         </is>
       </c>
       <c r="D65" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1925,10 +1905,10 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>46047.33333333334</v>
+        <v>46048.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>5.70924</v>
+        <v>32.94468</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1936,7 +1916,7 @@
         </is>
       </c>
       <c r="D66" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -1946,10 +1926,10 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>46047.35416666666</v>
+        <v>46048.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>-1.06044</v>
+        <v>0.7</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1957,7 +1937,7 @@
         </is>
       </c>
       <c r="D67" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -1967,10 +1947,10 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>46047.375</v>
+        <v>46048.375</v>
       </c>
       <c r="B68" t="n">
-        <v>-5.50985</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1978,7 +1958,7 @@
         </is>
       </c>
       <c r="D68" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -1988,10 +1968,10 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>46047.39583333334</v>
+        <v>46048.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>-6</v>
+        <v>0.00991</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -1999,7 +1979,7 @@
         </is>
       </c>
       <c r="D69" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2009,10 +1989,10 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>46047.41666666666</v>
+        <v>46048.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>-6.19359</v>
+        <v>0.7</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2020,7 +2000,7 @@
         </is>
       </c>
       <c r="D70" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2030,10 +2010,10 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>46047.4375</v>
+        <v>46048.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>-6.16627</v>
+        <v>-0.97701</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2041,7 +2021,7 @@
         </is>
       </c>
       <c r="D71" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2051,10 +2031,10 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>46047.45833333334</v>
+        <v>46048.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>-6.08061</v>
+        <v>-0.21959</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2062,7 +2042,7 @@
         </is>
       </c>
       <c r="D72" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2072,10 +2052,10 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>46047.47916666666</v>
+        <v>46048.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2083,7 +2063,7 @@
         </is>
       </c>
       <c r="D73" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2093,10 +2073,10 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>46047.5</v>
+        <v>46048.5</v>
       </c>
       <c r="B74" t="n">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2104,7 +2084,7 @@
         </is>
       </c>
       <c r="D74" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2114,10 +2094,10 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>46047.52083333334</v>
+        <v>46048.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>-6.52693</v>
+        <v>0.28508</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2125,7 +2105,7 @@
         </is>
       </c>
       <c r="D75" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2135,10 +2115,10 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>46047.54166666666</v>
+        <v>46048.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>-6</v>
+        <v>0.7</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2146,7 +2126,7 @@
         </is>
       </c>
       <c r="D76" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2156,10 +2136,10 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>46047.5625</v>
+        <v>46048.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>-5.50985</v>
+        <v>31.11445</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2167,7 +2147,7 @@
         </is>
       </c>
       <c r="D77" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2177,10 +2157,10 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>46047.58333333334</v>
+        <v>46048.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>2e-05</v>
+        <v>36.06</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2188,7 +2168,7 @@
         </is>
       </c>
       <c r="D78" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2198,10 +2178,10 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>46047.60416666666</v>
+        <v>46048.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-2.54301</v>
+        <v>35.99355</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2209,7 +2189,7 @@
         </is>
       </c>
       <c r="D79" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2219,10 +2199,10 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>46047.625</v>
+        <v>46048.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-1.49771</v>
+        <v>22.07</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2230,7 +2210,7 @@
         </is>
       </c>
       <c r="D80" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2240,10 +2220,10 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>46047.64583333334</v>
+        <v>46048.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>0.41892</v>
+        <v>19.83551</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2251,7 +2231,7 @@
         </is>
       </c>
       <c r="D81" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2261,10 +2241,10 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>46047.66666666666</v>
+        <v>46048.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>2.68504</v>
+        <v>10.36161</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2272,20 +2252,20 @@
         </is>
       </c>
       <c r="D82" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>46047.6875</v>
+        <v>46048.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>48.75908</v>
+        <v>6.36081</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2293,20 +2273,20 @@
         </is>
       </c>
       <c r="D83" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>46047.70833333334</v>
+        <v>46048.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>70.50918</v>
+        <v>9.500030000000001</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2314,20 +2294,20 @@
         </is>
       </c>
       <c r="D84" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>46047.72916666666</v>
+        <v>46048.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>76.94748</v>
+        <v>7.6655</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2335,20 +2315,20 @@
         </is>
       </c>
       <c r="D85" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>46047.75</v>
+        <v>46048.75</v>
       </c>
       <c r="B86" t="n">
-        <v>184.43252</v>
+        <v>-3.97723</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2356,7 +2336,7 @@
         </is>
       </c>
       <c r="D86" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2366,10 +2346,10 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>46047.77083333334</v>
+        <v>46048.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>349.81754</v>
+        <v>-6</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2377,7 +2357,7 @@
         </is>
       </c>
       <c r="D87" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2387,10 +2367,10 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>46047.79166666666</v>
+        <v>46048.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>408.81344</v>
+        <v>-38.16</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2398,7 +2378,7 @@
         </is>
       </c>
       <c r="D88" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2408,10 +2388,10 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>46047.8125</v>
+        <v>46048.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>286.65072</v>
+        <v>-38.16</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2419,7 +2399,7 @@
         </is>
       </c>
       <c r="D89" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2429,10 +2409,10 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>46047.83333333334</v>
+        <v>46048.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>330.17155</v>
+        <v>-38.16</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2440,7 +2420,7 @@
         </is>
       </c>
       <c r="D90" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2450,10 +2430,10 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>46047.85416666666</v>
+        <v>46048.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>168.29492</v>
+        <v>87.4353</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2461,7 +2441,7 @@
         </is>
       </c>
       <c r="D91" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2471,10 +2451,10 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>46047.875</v>
+        <v>46048.875</v>
       </c>
       <c r="B92" t="n">
-        <v>279.10835</v>
+        <v>77.02996</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2482,7 +2462,7 @@
         </is>
       </c>
       <c r="D92" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2492,10 +2472,10 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>46047.89583333334</v>
+        <v>46048.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>240.89</v>
+        <v>64.01339</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2503,7 +2483,7 @@
         </is>
       </c>
       <c r="D93" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2513,10 +2493,10 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>46047.91666666666</v>
+        <v>46048.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>138.57805</v>
+        <v>62.46015</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2524,7 +2504,7 @@
         </is>
       </c>
       <c r="D94" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2534,10 +2514,10 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>46047.9375</v>
+        <v>46048.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>147.52</v>
+        <v>73.35365</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2545,7 +2525,7 @@
         </is>
       </c>
       <c r="D95" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2555,10 +2535,10 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>46047.95833333334</v>
+        <v>46048.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>101.25</v>
+        <v>75.69112</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2566,7 +2546,7 @@
         </is>
       </c>
       <c r="D96" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2576,10 +2556,10 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>46047.97916666666</v>
+        <v>46048.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>91.65622999999999</v>
+        <v>70.47257</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -2587,7 +2567,7 @@
         </is>
       </c>
       <c r="D97" s="3" t="n">
-        <v>46047</v>
+        <v>46048</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 177)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -475,62 +475,62 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46067.04166666666</v>
+        <v>46068.14583333334</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46067.22916666666</v>
+        <v>46068.77083333334</v>
       </c>
       <c r="C2" t="n">
-        <v>4.5</v>
+        <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>17.01</v>
+        <v>56.7</v>
       </c>
       <c r="E2" t="n">
-        <v>499.4363595</v>
+        <v>770.9686529999999</v>
       </c>
       <c r="F2" t="n">
-        <v>29.36133800705468</v>
+        <v>13.59733074074074</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46067.3125</v>
+        <v>46068.95833333334</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46067.79166666666</v>
+        <v>46069.14583333334</v>
       </c>
       <c r="C3" t="n">
-        <v>11.5</v>
+        <v>4.5</v>
       </c>
       <c r="D3" t="n">
-        <v>43.47</v>
+        <v>17.01</v>
       </c>
       <c r="E3" t="n">
-        <v>681.1232219999997</v>
+        <v>465.6658792499999</v>
       </c>
       <c r="F3" t="n">
-        <v>15.66881118012422</v>
+        <v>27.37600701058201</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46068.27083333334</v>
+        <v>46069.3125</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46068.77083333334</v>
+        <v>46069.66666666666</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>8.5</v>
       </c>
       <c r="D4" t="n">
-        <v>45.36</v>
+        <v>32.13</v>
       </c>
       <c r="E4" t="n">
-        <v>462.74472075</v>
+        <v>275.6391885</v>
       </c>
       <c r="F4" t="n">
-        <v>10.20160319113757</v>
+        <v>8.578872969187678</v>
       </c>
     </row>
   </sheetData>
@@ -581,10 +581,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="B2" t="n">
-        <v>73.42098</v>
+        <v>56.98</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -602,10 +602,10 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46067.02083333334</v>
+        <v>46068.02083333334</v>
       </c>
       <c r="B3" t="n">
-        <v>71.34744999999999</v>
+        <v>56.98</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -623,10 +623,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46067.04166666666</v>
+        <v>46068.04166666666</v>
       </c>
       <c r="B4" t="n">
-        <v>61.01486</v>
+        <v>53.87364</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -634,20 +634,20 @@
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46067.0625</v>
+        <v>46068.0625</v>
       </c>
       <c r="B5" t="n">
-        <v>57.06014</v>
+        <v>56.79006</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -655,20 +655,20 @@
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46067.08333333334</v>
+        <v>46068.08333333334</v>
       </c>
       <c r="B6" t="n">
-        <v>57.06007</v>
+        <v>53.26316</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -676,20 +676,20 @@
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46067.10416666666</v>
+        <v>46068.10416666666</v>
       </c>
       <c r="B7" t="n">
-        <v>56.98</v>
+        <v>55.08303</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -697,20 +697,20 @@
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46067.125</v>
+        <v>46068.125</v>
       </c>
       <c r="B8" t="n">
-        <v>53.23796</v>
+        <v>54.7739</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -718,20 +718,20 @@
         </is>
       </c>
       <c r="D8" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46067.14583333334</v>
+        <v>46068.14583333334</v>
       </c>
       <c r="B9" t="n">
-        <v>53.24036</v>
+        <v>54.77339</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -739,7 +739,7 @@
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -749,10 +749,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46067.16666666666</v>
+        <v>46068.16666666666</v>
       </c>
       <c r="B10" t="n">
-        <v>54.22002</v>
+        <v>56.83994</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="D10" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -770,10 +770,10 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46067.1875</v>
+        <v>46068.1875</v>
       </c>
       <c r="B11" t="n">
-        <v>57.06007</v>
+        <v>54.35372</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -781,7 +781,7 @@
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -791,10 +791,10 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46067.20833333334</v>
+        <v>46068.20833333334</v>
       </c>
       <c r="B12" t="n">
-        <v>62.36894</v>
+        <v>56.98</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -812,10 +812,10 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46067.22916666666</v>
+        <v>46068.22916666666</v>
       </c>
       <c r="B13" t="n">
-        <v>76.13726</v>
+        <v>56.98</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -823,20 +823,20 @@
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46067.25</v>
+        <v>46068.25</v>
       </c>
       <c r="B14" t="n">
-        <v>84.79000000000001</v>
+        <v>56.98</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -844,20 +844,20 @@
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46067.27083333334</v>
+        <v>46068.27083333334</v>
       </c>
       <c r="B15" t="n">
-        <v>84.79000000000001</v>
+        <v>53.16496</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -865,20 +865,20 @@
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46067.29166666666</v>
+        <v>46068.29166666666</v>
       </c>
       <c r="B16" t="n">
-        <v>73.19</v>
+        <v>36.0601</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -886,20 +886,20 @@
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46067.3125</v>
+        <v>46068.3125</v>
       </c>
       <c r="B17" t="n">
-        <v>51.59311</v>
+        <v>36.07</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -917,10 +917,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46067.33333333334</v>
+        <v>46068.33333333334</v>
       </c>
       <c r="B18" t="n">
-        <v>56.98</v>
+        <v>36.0601</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -938,10 +938,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46067.35416666666</v>
+        <v>46068.35416666666</v>
       </c>
       <c r="B19" t="n">
-        <v>47.45981</v>
+        <v>36.0601</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -959,10 +959,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46067.375</v>
+        <v>46068.375</v>
       </c>
       <c r="B20" t="n">
-        <v>36.07</v>
+        <v>36.0601</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="D20" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -980,10 +980,10 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46067.39583333334</v>
+        <v>46068.39583333334</v>
       </c>
       <c r="B21" t="n">
-        <v>31.1147</v>
+        <v>36.0601</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1001,10 +1001,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46067.41666666666</v>
+        <v>46068.41666666666</v>
       </c>
       <c r="B22" t="n">
-        <v>22.07</v>
+        <v>32.84175</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="D22" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46067.4375</v>
+        <v>46068.4375</v>
       </c>
       <c r="B23" t="n">
-        <v>30.94737</v>
+        <v>36.0601</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1033,7 +1033,7 @@
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1043,10 +1043,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>46067.45833333334</v>
+        <v>46068.45833333334</v>
       </c>
       <c r="B24" t="n">
-        <v>30.52819</v>
+        <v>22.07</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1054,7 +1054,7 @@
         </is>
       </c>
       <c r="D24" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>46067.47916666666</v>
+        <v>46068.47916666666</v>
       </c>
       <c r="B25" t="n">
         <v>22.07</v>
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1085,10 +1085,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>46067.5</v>
+        <v>46068.5</v>
       </c>
       <c r="B26" t="n">
-        <v>8.03814</v>
+        <v>4.38659</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="D26" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1106,10 +1106,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>46067.52083333334</v>
+        <v>46068.52083333334</v>
       </c>
       <c r="B27" t="n">
-        <v>-4.68971</v>
+        <v>0.51</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1127,10 +1127,10 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>46067.54166666666</v>
+        <v>46068.54166666666</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.99369</v>
+        <v>0.51</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1138,7 +1138,7 @@
         </is>
       </c>
       <c r="D28" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1148,10 +1148,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>46067.5625</v>
+        <v>46068.5625</v>
       </c>
       <c r="B29" t="n">
-        <v>-2.66469</v>
+        <v>0.44703</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1169,10 +1169,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>46067.58333333334</v>
+        <v>46068.58333333334</v>
       </c>
       <c r="B30" t="n">
-        <v>2.9527</v>
+        <v>-3.11157</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="D30" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1190,10 +1190,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>46067.60416666666</v>
+        <v>46068.60416666666</v>
       </c>
       <c r="B31" t="n">
-        <v>9.45477</v>
+        <v>-7.04692</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="D31" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1211,10 +1211,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>46067.625</v>
+        <v>46068.625</v>
       </c>
       <c r="B32" t="n">
-        <v>21.73531</v>
+        <v>-1.02238</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="D32" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>46067.64583333334</v>
+        <v>46068.64583333334</v>
       </c>
       <c r="B33" t="n">
-        <v>36.0601</v>
+        <v>0.01038</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1243,7 +1243,7 @@
         </is>
       </c>
       <c r="D33" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1253,10 +1253,10 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>46067.66666666666</v>
+        <v>46068.66666666666</v>
       </c>
       <c r="B34" t="n">
-        <v>44.72673</v>
+        <v>9.089130000000001</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1264,7 +1264,7 @@
         </is>
       </c>
       <c r="D34" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1274,10 +1274,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>46067.6875</v>
+        <v>46068.6875</v>
       </c>
       <c r="B35" t="n">
-        <v>36.0601</v>
+        <v>8.8331</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="D35" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>46067.70833333334</v>
+        <v>46068.70833333334</v>
       </c>
       <c r="B36" t="n">
-        <v>47.91498</v>
+        <v>8.984669999999999</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1306,7 +1306,7 @@
         </is>
       </c>
       <c r="D36" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1316,10 +1316,10 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>46067.72916666666</v>
+        <v>46068.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>57.09</v>
+        <v>12.32016</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="D37" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>46067.75</v>
+        <v>46068.75</v>
       </c>
       <c r="B38" t="n">
-        <v>57.09</v>
+        <v>37.34253</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="D38" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>46067.77083333334</v>
+        <v>46068.77083333334</v>
       </c>
       <c r="B39" t="n">
         <v>56.98</v>
@@ -1369,28 +1369,28 @@
         </is>
       </c>
       <c r="D39" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>46067.79166666666</v>
+        <v>46068.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>63.60109</v>
+        <v>64.89</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1400,18 +1400,18 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>46067.8125</v>
+        <v>46068.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>64.89</v>
+        <v>73.27</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1421,18 +1421,18 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>46067.83333333334</v>
+        <v>46068.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>64.89</v>
+        <v>76.76687</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1442,18 +1442,18 @@
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>46067.85416666666</v>
+        <v>46068.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>65.00005</v>
+        <v>73.29000000000001</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1463,18 +1463,18 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>46067.875</v>
+        <v>46068.875</v>
       </c>
       <c r="B44" t="n">
-        <v>64.89</v>
+        <v>59.01826</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1484,18 +1484,18 @@
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>46067.89583333334</v>
+        <v>46068.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>57.60478</v>
+        <v>59.11256</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1505,18 +1505,18 @@
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>46067.91666666666</v>
+        <v>46068.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>57.31</v>
+        <v>58.95819</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1526,18 +1526,18 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>46067.9375</v>
+        <v>46068.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>57.09</v>
+        <v>56.98</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1547,31 +1547,31 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>46067.95833333334</v>
+        <v>46068.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>56.98</v>
+        <v>48.41499</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>historical</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>46067.97916666666</v>
+        <v>46068.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.98</v>
+        <v>49.73329</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1579,20 +1579,20 @@
         </is>
       </c>
       <c r="D49" s="3" t="n">
-        <v>46067</v>
+        <v>46068</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="B50" t="n">
-        <v>53.12933</v>
+        <v>49.37423</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1600,17 +1600,17 @@
         </is>
       </c>
       <c r="D50" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>46068.02083333334</v>
+        <v>46069.02083333334</v>
       </c>
       <c r="B51" t="n">
         <v>56.98</v>
@@ -1621,20 +1621,20 @@
         </is>
       </c>
       <c r="D51" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>46068.04166666666</v>
+        <v>46069.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>53.53295</v>
+        <v>56.98</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1642,20 +1642,20 @@
         </is>
       </c>
       <c r="D52" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>46068.0625</v>
+        <v>46069.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>53.94375</v>
+        <v>52.30742</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1663,20 +1663,20 @@
         </is>
       </c>
       <c r="D53" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>46068.08333333334</v>
+        <v>46069.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>54.01585</v>
+        <v>51.8802</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1684,20 +1684,20 @@
         </is>
       </c>
       <c r="D54" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>46068.10416666666</v>
+        <v>46069.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>52.6617</v>
+        <v>55.14573</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1705,20 +1705,20 @@
         </is>
       </c>
       <c r="D55" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>46068.125</v>
+        <v>46069.125</v>
       </c>
       <c r="B56" t="n">
-        <v>52.37068</v>
+        <v>56.79017</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1726,20 +1726,20 @@
         </is>
       </c>
       <c r="D56" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>46068.14583333334</v>
+        <v>46069.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>52.37048</v>
+        <v>56.98</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="D57" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1757,10 +1757,10 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>46068.16666666666</v>
+        <v>46069.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>54.43034</v>
+        <v>56.98</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1768,7 +1768,7 @@
         </is>
       </c>
       <c r="D58" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1778,10 +1778,10 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>46068.1875</v>
+        <v>46069.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>52.0279</v>
+        <v>55.01863</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="D59" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>46068.20833333334</v>
+        <v>46069.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>53.70872</v>
+        <v>56.98</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="D60" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1820,10 +1820,10 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>46068.22916666666</v>
+        <v>46069.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>56.98</v>
+        <v>57.31</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1831,7 +1831,7 @@
         </is>
       </c>
       <c r="D61" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1841,10 +1841,10 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>46068.25</v>
+        <v>46069.25</v>
       </c>
       <c r="B62" t="n">
-        <v>56.03</v>
+        <v>64.89</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="D62" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1862,10 +1862,10 @@
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>46068.27083333334</v>
+        <v>46069.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>53.68323</v>
+        <v>65</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1873,20 +1873,20 @@
         </is>
       </c>
       <c r="D63" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>46068.29166666666</v>
+        <v>46069.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>36.0601</v>
+        <v>56.98</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1894,20 +1894,20 @@
         </is>
       </c>
       <c r="D64" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>46068.3125</v>
+        <v>46069.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>36.0601</v>
+        <v>47.11845</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1915,7 +1915,7 @@
         </is>
       </c>
       <c r="D65" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>46068.33333333334</v>
+        <v>46069.33333333334</v>
       </c>
       <c r="B66" t="n">
         <v>36.0601</v>
@@ -1936,7 +1936,7 @@
         </is>
       </c>
       <c r="D66" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>46068.35416666666</v>
+        <v>46069.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>36.0601</v>
+        <v>20.85946</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="D67" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -1967,10 +1967,10 @@
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>46068.375</v>
+        <v>46069.375</v>
       </c>
       <c r="B68" t="n">
-        <v>36.0601</v>
+        <v>22.07</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="D68" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -1988,10 +1988,10 @@
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>46068.39583333334</v>
+        <v>46069.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>36.0601</v>
+        <v>22.07</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -1999,7 +1999,7 @@
         </is>
       </c>
       <c r="D69" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2009,10 +2009,10 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>46068.41666666666</v>
+        <v>46069.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>36.0601</v>
+        <v>22.07</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2020,7 +2020,7 @@
         </is>
       </c>
       <c r="D70" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2030,10 +2030,10 @@
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>46068.4375</v>
+        <v>46069.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>36.0601</v>
+        <v>30.83785</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="D71" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2051,10 +2051,10 @@
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>46068.45833333334</v>
+        <v>46069.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>22.07</v>
+        <v>12.76166</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="D72" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2072,10 +2072,10 @@
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>46068.47916666666</v>
+        <v>46069.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>22.07</v>
+        <v>12.54898</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2083,7 +2083,7 @@
         </is>
       </c>
       <c r="D73" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2093,10 +2093,10 @@
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>46068.5</v>
+        <v>46069.5</v>
       </c>
       <c r="B74" t="n">
-        <v>1.23444</v>
+        <v>0.66442</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2104,7 +2104,7 @@
         </is>
       </c>
       <c r="D74" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>46068.52083333334</v>
+        <v>46069.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>0.03385</v>
+        <v>0.67361</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2125,7 +2125,7 @@
         </is>
       </c>
       <c r="D75" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>46068.54166666666</v>
+        <v>46069.54166666666</v>
       </c>
       <c r="B76" t="n">
         <v>0.51</v>
@@ -2146,7 +2146,7 @@
         </is>
       </c>
       <c r="D76" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2156,10 +2156,10 @@
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>46068.5625</v>
+        <v>46069.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>0.36345</v>
+        <v>0.7</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="D77" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2177,10 +2177,10 @@
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>46068.58333333334</v>
+        <v>46069.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>0.50984</v>
+        <v>11.7925</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2188,7 +2188,7 @@
         </is>
       </c>
       <c r="D78" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2198,10 +2198,10 @@
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>46068.60416666666</v>
+        <v>46069.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>-6.99601</v>
+        <v>22.07</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2209,7 +2209,7 @@
         </is>
       </c>
       <c r="D79" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2219,10 +2219,10 @@
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>46068.625</v>
+        <v>46069.625</v>
       </c>
       <c r="B80" t="n">
-        <v>-1.80118</v>
+        <v>8.290380000000001</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="D80" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2240,10 +2240,10 @@
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>46068.64583333334</v>
+        <v>46069.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>0.0103</v>
+        <v>11.60945</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2251,7 +2251,7 @@
         </is>
       </c>
       <c r="D81" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2261,10 +2261,10 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>46068.66666666666</v>
+        <v>46069.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>9.023770000000001</v>
+        <v>42.50838</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2272,20 +2272,20 @@
         </is>
       </c>
       <c r="D82" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>46068.6875</v>
+        <v>46069.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>8.768990000000001</v>
+        <v>49.23912</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2293,20 +2293,20 @@
         </is>
       </c>
       <c r="D83" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>46068.70833333334</v>
+        <v>46069.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>8.92048</v>
+        <v>53.12629</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2314,20 +2314,20 @@
         </is>
       </c>
       <c r="D84" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>46068.72916666666</v>
+        <v>46069.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>31.10246</v>
+        <v>66.99075999999999</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2335,20 +2335,20 @@
         </is>
       </c>
       <c r="D85" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>46068.75</v>
+        <v>46069.75</v>
       </c>
       <c r="B86" t="n">
-        <v>36.62555</v>
+        <v>73.19</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2356,20 +2356,20 @@
         </is>
       </c>
       <c r="D86" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>46068.77083333334</v>
+        <v>46069.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>57.6508</v>
+        <v>75.36904</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2377,7 +2377,7 @@
         </is>
       </c>
       <c r="D87" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2387,10 +2387,10 @@
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>46068.79166666666</v>
+        <v>46069.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>64.89</v>
+        <v>90.12555999999999</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2398,7 +2398,7 @@
         </is>
       </c>
       <c r="D88" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2408,10 +2408,10 @@
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>46068.8125</v>
+        <v>46069.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>68.62712999999999</v>
+        <v>92.73465</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2419,7 +2419,7 @@
         </is>
       </c>
       <c r="D89" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2429,10 +2429,10 @@
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>46068.83333333334</v>
+        <v>46069.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>68.85534</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2440,7 +2440,7 @@
         </is>
       </c>
       <c r="D90" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2450,10 +2450,10 @@
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>46068.85416666666</v>
+        <v>46069.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>64.89</v>
+        <v>78</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2461,7 +2461,7 @@
         </is>
       </c>
       <c r="D91" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2471,10 +2471,10 @@
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>46068.875</v>
+        <v>46069.875</v>
       </c>
       <c r="B92" t="n">
-        <v>64.89</v>
+        <v>72.90904999999999</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="D92" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2492,10 +2492,10 @@
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>46068.89583333334</v>
+        <v>46069.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>60.64516</v>
+        <v>65</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2503,7 +2503,7 @@
         </is>
       </c>
       <c r="D93" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2513,10 +2513,10 @@
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>46068.91666666666</v>
+        <v>46069.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>56.98</v>
+        <v>61.73451</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2524,7 +2524,7 @@
         </is>
       </c>
       <c r="D94" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2534,10 +2534,10 @@
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>46068.9375</v>
+        <v>46069.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>47.60427</v>
+        <v>56.98</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2545,7 +2545,7 @@
         </is>
       </c>
       <c r="D95" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2555,10 +2555,10 @@
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>46068.95833333334</v>
+        <v>46069.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>42.12537</v>
+        <v>56.98</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2566,7 +2566,7 @@
         </is>
       </c>
       <c r="D96" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2576,10 +2576,10 @@
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>46068.97916666666</v>
+        <v>46069.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>36.0601</v>
+        <v>56.98</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
         </is>
       </c>
       <c r="D97" s="3" t="n">
-        <v>46068</v>
+        <v>46069</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 194)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,79 +478,99 @@
         <v>46076</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46076.22916666666</v>
+        <v>46076.20833333334</v>
       </c>
       <c r="C2" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>20.79</v>
+        <v>18.9</v>
       </c>
       <c r="E2" t="n">
-        <v>852.0254534999999</v>
+        <v>774.0742035</v>
       </c>
       <c r="F2" t="n">
-        <v>40.9824652958153</v>
+        <v>40.95630706349206</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46076.35416666666</v>
+        <v>46076.375</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>46076.66666666666</v>
       </c>
       <c r="C3" t="n">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>28.35</v>
+        <v>26.46</v>
       </c>
       <c r="E3" t="n">
-        <v>778.122267</v>
+        <v>695.4520169999998</v>
       </c>
       <c r="F3" t="n">
-        <v>27.44699354497354</v>
+        <v>26.28314501133787</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46076.875</v>
+        <v>46076.83333333334</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46077.14583333334</v>
+        <v>46077</v>
       </c>
       <c r="C4" t="n">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>24.57</v>
+        <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>964.9788037499998</v>
+        <v>701.3367465000001</v>
       </c>
       <c r="F4" t="n">
-        <v>39.27467658730158</v>
+        <v>46.38470545634922</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46077.3125</v>
+        <v>46077.33333333334</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>46077.66666666666</v>
       </c>
       <c r="C5" t="n">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>32.13</v>
+        <v>30.24</v>
       </c>
       <c r="E5" t="n">
-        <v>790.8133057499998</v>
+        <v>594.1234065</v>
       </c>
       <c r="F5" t="n">
-        <v>24.61292579365079</v>
+        <v>19.64693804563492</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>46077.83333333334</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>46078</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>15.12</v>
+      </c>
+      <c r="E6" t="n">
+        <v>660.41255475</v>
+      </c>
+      <c r="F6" t="n">
+        <v>43.67807901785714</v>
       </c>
     </row>
   </sheetData>
@@ -826,7 +846,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -973,7 +993,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1380,7 @@
         <v>46076.75</v>
       </c>
       <c r="B38" t="n">
-        <v>57.31</v>
+        <v>70.92874</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1401,7 @@
         <v>46076.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>69.89302000000001</v>
+        <v>88.27029</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,11 +1422,11 @@
         <v>46076.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>99.89228</v>
+        <v>85.13891</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1423,11 +1443,11 @@
         <v>46076.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>106.75338</v>
+        <v>85.66633</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
@@ -1444,11 +1464,11 @@
         <v>46076.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>108.01</v>
+        <v>99.35961</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
@@ -1456,7 +1476,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1465,11 +1485,11 @@
         <v>46076.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>95.5257</v>
+        <v>93.23457000000001</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1477,7 +1497,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1490,7 +1510,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1507,11 +1527,11 @@
         <v>46076.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>72.71819000000001</v>
+        <v>78</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
@@ -1528,11 +1548,11 @@
         <v>46076.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>75.76251000000001</v>
+        <v>68.61024</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
@@ -1549,11 +1569,11 @@
         <v>46076.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>71.18069</v>
+        <v>103.84773</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
@@ -1570,11 +1590,11 @@
         <v>46076.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>78</v>
+        <v>103.79417</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
@@ -1591,11 +1611,11 @@
         <v>46076.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>70.57126</v>
+        <v>94.47342</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D49" s="3" t="n">
@@ -1612,7 +1632,7 @@
         <v>46077</v>
       </c>
       <c r="B50" t="n">
-        <v>74.3154</v>
+        <v>97.72414999999999</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1624,7 +1644,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1633,7 +1653,7 @@
         <v>46077.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>78</v>
+        <v>92.20686000000001</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1645,7 +1665,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1654,7 +1674,7 @@
         <v>46077.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>78</v>
+        <v>93.19385</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1666,7 +1686,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1695,7 @@
         <v>46077.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>78</v>
+        <v>93.9629</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1687,7 +1707,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1716,7 @@
         <v>46077.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>78</v>
+        <v>92.51766000000001</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1708,7 +1728,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1717,7 +1737,7 @@
         <v>46077.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>78</v>
+        <v>102.77994</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1729,7 +1749,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1758,7 @@
         <v>46077.125</v>
       </c>
       <c r="B56" t="n">
-        <v>79.1738</v>
+        <v>103.67301</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1750,7 +1770,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1779,7 @@
         <v>46077.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>80.82232999999999</v>
+        <v>105</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1800,7 @@
         <v>46077.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>84.79000000000001</v>
+        <v>105.79</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1821,7 @@
         <v>46077.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>79.95021</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1842,7 @@
         <v>46077.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>79.95004</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1863,7 @@
         <v>46077.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>102.97224</v>
+        <v>108.01</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1884,7 @@
         <v>46077.25</v>
       </c>
       <c r="B62" t="n">
-        <v>105.79</v>
+        <v>108.01</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1906,7 +1926,7 @@
         <v>46077.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>102.71112</v>
+        <v>93.30685</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1927,7 +1947,7 @@
         <v>46077.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>74.27677</v>
+        <v>76.29461999999999</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1939,7 +1959,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1948,7 +1968,7 @@
         <v>46077.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>73.19</v>
+        <v>62.22123</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1969,7 +1989,7 @@
         <v>46077.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>57.06007</v>
+        <v>56.98</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2011,7 +2031,7 @@
         <v>46077.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>37.89</v>
+        <v>22.07</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2053,7 +2073,7 @@
         <v>46077.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>37.89</v>
+        <v>34.01</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2094,7 @@
         <v>46077.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>37.89</v>
+        <v>28.92581</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2115,7 @@
         <v>46077.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>37.89</v>
+        <v>34.01</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2136,7 @@
         <v>46077.5</v>
       </c>
       <c r="B74" t="n">
-        <v>37.89</v>
+        <v>34.01</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2157,7 @@
         <v>46077.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>37.89</v>
+        <v>34.01</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2178,7 @@
         <v>46077.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>56.98</v>
+        <v>37.89</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2199,7 @@
         <v>46077.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>37.89023</v>
+        <v>37.89</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2220,7 @@
         <v>46077.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>56.72325</v>
+        <v>37.89</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2241,7 @@
         <v>46077.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>56.98002</v>
+        <v>37.8903</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2262,7 @@
         <v>46077.625</v>
       </c>
       <c r="B80" t="n">
-        <v>37.8902</v>
+        <v>37.89</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2283,7 @@
         <v>46077.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>56.98003</v>
+        <v>37.89</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2304,7 @@
         <v>46077.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>62.00023</v>
+        <v>56.98003</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2325,7 @@
         <v>46077.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>56.80642</v>
+        <v>37.89019</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2346,7 @@
         <v>46077.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>64.89</v>
+        <v>66.19919</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2367,7 @@
         <v>46077.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>73.19</v>
+        <v>76.28172000000001</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2388,7 @@
         <v>46077.75</v>
       </c>
       <c r="B86" t="n">
-        <v>98.56792</v>
+        <v>95.73061</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2409,7 @@
         <v>46077.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>112.63281</v>
+        <v>108.89</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2430,7 @@
         <v>46077.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>115.77759</v>
+        <v>108.89</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2452,7 +2472,7 @@
         <v>46077.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>108.01</v>
+        <v>108.89</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2464,7 +2484,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2485,7 +2505,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2494,7 +2514,7 @@
         <v>46077.875</v>
       </c>
       <c r="B92" t="n">
-        <v>90.02785</v>
+        <v>98.93407999999999</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2506,7 +2526,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2515,7 +2535,7 @@
         <v>46077.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>78</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2527,7 +2547,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2536,7 +2556,7 @@
         <v>46077.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>64.89</v>
+        <v>70.57161000000001</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2548,7 +2568,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2577,7 @@
         <v>46077.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>64.89</v>
+        <v>71.47271000000001</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2569,7 +2589,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2578,7 +2598,7 @@
         <v>46077.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>64.89</v>
+        <v>72.79781</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2590,7 +2610,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2599,7 +2619,7 @@
         <v>46077.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>57.08</v>
+        <v>64.89</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -2611,7 +2631,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update latest output (run 196)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -527,10 +527,10 @@
         <v>15.12</v>
       </c>
       <c r="E4" t="n">
-        <v>511.41516075</v>
+        <v>660.1421482500001</v>
       </c>
       <c r="F4" t="n">
-        <v>33.82375401785714</v>
+        <v>43.66019499007938</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +547,10 @@
         <v>26.46</v>
       </c>
       <c r="E5" t="n">
-        <v>576.28228125</v>
+        <v>564.6798300000002</v>
       </c>
       <c r="F5" t="n">
-        <v>21.77937570861678</v>
+        <v>21.34088548752835</v>
       </c>
     </row>
     <row r="6">
@@ -567,10 +567,10 @@
         <v>15.12</v>
       </c>
       <c r="E6" t="n">
-        <v>405.99810225</v>
+        <v>408.44997375</v>
       </c>
       <c r="F6" t="n">
-        <v>26.85172633928572</v>
+        <v>27.01388715277778</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1380,7 @@
         <v>46077.75</v>
       </c>
       <c r="B38" t="n">
-        <v>107.82657</v>
+        <v>100.01</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1401,7 +1401,7 @@
         <v>46077.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>116.16282</v>
+        <v>108.89</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1422,11 +1422,11 @@
         <v>46077.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>121.0797</v>
+        <v>109.12055</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1443,11 +1443,11 @@
         <v>46077.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>109.46156</v>
+        <v>112.06343</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
@@ -1464,11 +1464,11 @@
         <v>46077.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>137.0233</v>
+        <v>109.91454</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
@@ -1485,11 +1485,11 @@
         <v>46077.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>104.95471</v>
+        <v>105</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1506,11 +1506,11 @@
         <v>46077.875</v>
       </c>
       <c r="B44" t="n">
-        <v>84.79000000000001</v>
+        <v>98.92904</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1527,11 +1527,11 @@
         <v>46077.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>75.55737999999999</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
@@ -1548,11 +1548,11 @@
         <v>46077.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>64.89</v>
+        <v>70.57004999999999</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
@@ -1569,11 +1569,11 @@
         <v>46077.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>60.03049</v>
+        <v>99.56278</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
@@ -1590,11 +1590,11 @@
         <v>46077.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>60.24732</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
@@ -1611,11 +1611,11 @@
         <v>46077.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>57.31</v>
+        <v>85.65000000000001</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D49" s="3" t="n">
@@ -1632,7 +1632,7 @@
         <v>46078</v>
       </c>
       <c r="B50" t="n">
-        <v>57.31</v>
+        <v>79.57692</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1653,7 +1653,7 @@
         <v>46078.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>64.39318</v>
+        <v>73.20008</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1674,7 +1674,7 @@
         <v>46078.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>57.31</v>
+        <v>73.20009</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1695,7 +1695,7 @@
         <v>46078.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>57.31</v>
+        <v>73.20009</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1716,7 +1716,7 @@
         <v>46078.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>57.31</v>
+        <v>73.20009</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1737,7 +1737,7 @@
         <v>46078.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>57.31</v>
+        <v>78</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1758,7 +1758,7 @@
         <v>46078.125</v>
       </c>
       <c r="B56" t="n">
-        <v>64.89</v>
+        <v>78</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1779,7 +1779,7 @@
         <v>46078.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>64.89</v>
+        <v>78</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1800,7 +1800,7 @@
         <v>46078.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>66.28234</v>
+        <v>78</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1821,7 +1821,7 @@
         <v>46078.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>57.06</v>
+        <v>66.62696</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1842,7 +1842,7 @@
         <v>46078.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>57.31</v>
+        <v>79.39904</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1863,7 +1863,7 @@
         <v>46078.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>73.2</v>
+        <v>79.95014</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1884,7 +1884,7 @@
         <v>46078.25</v>
       </c>
       <c r="B62" t="n">
-        <v>76.77948000000001</v>
+        <v>96.03658</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1905,7 +1905,7 @@
         <v>46078.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>84.79000000000001</v>
+        <v>105.79</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1926,7 +1926,7 @@
         <v>46078.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>73.20001000000001</v>
+        <v>94.22657</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1947,7 +1947,7 @@
         <v>46078.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>56.98</v>
+        <v>57.06009</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1968,7 +1968,7 @@
         <v>46078.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>56.98</v>
+        <v>55.92455</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1989,7 +1989,7 @@
         <v>46078.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>57.06</v>
+        <v>46.17584</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2010,7 +2010,7 @@
         <v>46078.375</v>
       </c>
       <c r="B68" t="n">
-        <v>39.7732</v>
+        <v>37.89016</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2031,7 +2031,7 @@
         <v>46078.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>37.88999</v>
+        <v>38.73791</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2052,7 +2052,7 @@
         <v>46078.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>37.89</v>
+        <v>37.89023</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2073,7 +2073,7 @@
         <v>46078.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>37.89</v>
+        <v>37.89022</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2094,7 +2094,7 @@
         <v>46078.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>37.89</v>
+        <v>37.89021</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2115,7 +2115,7 @@
         <v>46078.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>37.89</v>
+        <v>40.24846</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2136,7 +2136,7 @@
         <v>46078.5</v>
       </c>
       <c r="B74" t="n">
-        <v>37.89</v>
+        <v>37.89021</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2157,7 +2157,7 @@
         <v>46078.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>37.89019</v>
+        <v>37.89038</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2178,7 +2178,7 @@
         <v>46078.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>39.25537</v>
+        <v>37.89018</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2199,7 +2199,7 @@
         <v>46078.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>37.89</v>
+        <v>37.89017</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2220,7 +2220,7 @@
         <v>46078.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>37.89</v>
+        <v>37.89019</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2241,7 +2241,7 @@
         <v>46078.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>57.06</v>
+        <v>64.89</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
         <v>46078.625</v>
       </c>
       <c r="B80" t="n">
-        <v>57.06014</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2283,7 +2283,7 @@
         <v>46078.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>57.06</v>
+        <v>80.50707</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2304,7 +2304,7 @@
         <v>46078.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>57.06</v>
+        <v>91.21869</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2325,7 +2325,7 @@
         <v>46078.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>57.06</v>
+        <v>78</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2346,7 +2346,7 @@
         <v>46078.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>65</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2367,7 +2367,7 @@
         <v>46078.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>64.89</v>
+        <v>78</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2388,7 +2388,7 @@
         <v>46078.75</v>
       </c>
       <c r="B86" t="n">
-        <v>68.05078</v>
+        <v>69.44401000000001</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2409,7 +2409,7 @@
         <v>46078.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>60.74603</v>
+        <v>70.36225</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2430,7 +2430,7 @@
         <v>46078.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>68.92322</v>
+        <v>71.02005</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2451,7 +2451,7 @@
         <v>46078.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>70.36225</v>
+        <v>70.35384000000001</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2472,7 +2472,7 @@
         <v>46078.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>69.14116</v>
+        <v>69.03394</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2493,7 +2493,7 @@
         <v>46078.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>64.89</v>
+        <v>57.31</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2514,7 +2514,7 @@
         <v>46078.875</v>
       </c>
       <c r="B92" t="n">
-        <v>56.98</v>
+        <v>57.06</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2577,7 +2577,7 @@
         <v>46078.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>47.08583</v>
+        <v>56.98</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2619,7 +2619,7 @@
         <v>46078.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>45.55132</v>
+        <v>45.77911</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 198)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,59 +518,39 @@
         <v>46078.83333333334</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46079</v>
+        <v>46079.14583333334</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="D4" t="n">
-        <v>15.12</v>
+        <v>28.35</v>
       </c>
       <c r="E4" t="n">
-        <v>516.7210034999999</v>
+        <v>826.4322495</v>
       </c>
       <c r="F4" t="n">
-        <v>34.17466954365079</v>
+        <v>29.15104936507937</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46079.04166666666</v>
+        <v>46079.3125</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>46079.20833333334</v>
+        <v>46079.66666666666</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>8.5</v>
       </c>
       <c r="D5" t="n">
-        <v>15.12</v>
+        <v>32.13</v>
       </c>
       <c r="E5" t="n">
-        <v>346.33328925</v>
+        <v>255.74873025</v>
       </c>
       <c r="F5" t="n">
-        <v>22.9056408234127</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>46079.33333333334</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>46079.66666666666</v>
-      </c>
-      <c r="C6" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" t="n">
-        <v>30.24</v>
-      </c>
-      <c r="E6" t="n">
-        <v>470.72400375</v>
-      </c>
-      <c r="F6" t="n">
-        <v>15.56626996527778</v>
+        <v>7.959811087768442</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1360,7 @@
         <v>46078.75</v>
       </c>
       <c r="B38" t="n">
-        <v>62.83374</v>
+        <v>69.26627999999999</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1401,7 +1381,7 @@
         <v>46078.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>51.97591</v>
+        <v>70.36225</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1422,11 +1402,11 @@
         <v>46078.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>85.29806000000001</v>
+        <v>71.02005</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1443,11 +1423,11 @@
         <v>46078.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>75.4332</v>
+        <v>70.36225</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
@@ -1464,11 +1444,11 @@
         <v>46078.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>83.43141</v>
+        <v>69.03394</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
@@ -1485,11 +1465,11 @@
         <v>46078.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>71.02006</v>
+        <v>57.31</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1506,11 +1486,11 @@
         <v>46078.875</v>
       </c>
       <c r="B44" t="n">
-        <v>66.82984</v>
+        <v>57.06</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1527,11 +1507,11 @@
         <v>46078.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>64.93592</v>
+        <v>37.89</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
@@ -1548,11 +1528,11 @@
         <v>46078.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>64.74285</v>
+        <v>56.98</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
@@ -1569,11 +1549,11 @@
         <v>46078.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>64.89</v>
+        <v>82.42008</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
@@ -1594,7 +1574,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
@@ -1611,11 +1591,11 @@
         <v>46078.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>57.06009</v>
+        <v>57.35</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D49" s="3" t="n">
@@ -1632,7 +1612,7 @@
         <v>46079</v>
       </c>
       <c r="B50" t="n">
-        <v>51.98784</v>
+        <v>57.06008</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1644,7 +1624,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1645,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1654,7 @@
         <v>46079.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>51.28719</v>
+        <v>56.98</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1695,7 +1675,7 @@
         <v>46079.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>50.50522</v>
+        <v>51.34198</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1716,7 +1696,7 @@
         <v>46079.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>37.89014</v>
+        <v>49.63623</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1737,7 +1717,7 @@
         <v>46079.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>37.89013</v>
+        <v>48.68524</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1758,7 +1738,7 @@
         <v>46079.125</v>
       </c>
       <c r="B56" t="n">
-        <v>37.89014</v>
+        <v>51.7551</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1779,7 +1759,7 @@
         <v>46079.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>37.89013</v>
+        <v>56.98</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1791,7 +1771,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1800,7 +1780,7 @@
         <v>46079.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>48.76016</v>
+        <v>53.45754</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1812,7 +1792,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1801,7 @@
         <v>46079.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>53.10052</v>
+        <v>56.98</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1833,7 +1813,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1842,7 +1822,7 @@
         <v>46079.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>56.98</v>
+        <v>57.06006</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1884,7 +1864,7 @@
         <v>46079.25</v>
       </c>
       <c r="B62" t="n">
-        <v>65</v>
+        <v>71.39019</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1905,7 +1885,7 @@
         <v>46079.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>72.93277</v>
+        <v>76.22794</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1926,7 +1906,7 @@
         <v>46079.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>61.42566</v>
+        <v>64.99988</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1959,7 +1939,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1969,7 @@
         <v>46079.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>37.88952</v>
+        <v>35.88</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2010,7 +1990,7 @@
         <v>46079.375</v>
       </c>
       <c r="B68" t="n">
-        <v>5.26465</v>
+        <v>13.12638</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2031,7 +2011,7 @@
         <v>46079.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>2.6387</v>
+        <v>10.4403</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2052,7 +2032,7 @@
         <v>46079.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>34.3302</v>
+        <v>5.91519</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2073,7 +2053,7 @@
         <v>46079.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>37.00011</v>
+        <v>0.70613</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2094,7 +2074,7 @@
         <v>46079.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>0.70153</v>
+        <v>0.0112</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2115,7 +2095,7 @@
         <v>46079.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>34.55964</v>
+        <v>0.5101</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2136,7 +2116,7 @@
         <v>46079.5</v>
       </c>
       <c r="B74" t="n">
-        <v>34.01</v>
+        <v>0.66949</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2157,7 +2137,7 @@
         <v>46079.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>37.89</v>
+        <v>0.67367</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2178,7 +2158,7 @@
         <v>46079.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>37.89</v>
+        <v>2.45449</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2199,7 +2179,7 @@
         <v>46079.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>29.54243</v>
+        <v>0.01078</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2220,7 +2200,7 @@
         <v>46079.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>29.15887</v>
+        <v>0.51</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2241,7 +2221,7 @@
         <v>46079.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>44.30557</v>
+        <v>37.89</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2262,7 +2242,7 @@
         <v>46079.625</v>
       </c>
       <c r="B80" t="n">
-        <v>43.84263</v>
+        <v>43.8586</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2283,7 +2263,7 @@
         <v>46079.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>37.89</v>
+        <v>35.88</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2304,7 +2284,7 @@
         <v>46079.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>37.89</v>
+        <v>35.88</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2346,7 +2326,7 @@
         <v>46079.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>39.57874</v>
+        <v>47.85084</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2367,7 +2347,7 @@
         <v>46079.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>39.86199</v>
+        <v>47.7311</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2388,7 +2368,7 @@
         <v>46079.75</v>
       </c>
       <c r="B86" t="n">
-        <v>56.31362</v>
+        <v>47.6007</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2409,7 +2389,7 @@
         <v>46079.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>59.73453</v>
+        <v>62.41151</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2430,7 +2410,7 @@
         <v>46079.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>69.9247</v>
+        <v>66.70088</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2451,7 +2431,7 @@
         <v>46079.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>81.4787</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2472,7 +2452,7 @@
         <v>46079.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>76.67444999999999</v>
+        <v>78</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2493,7 +2473,7 @@
         <v>46079.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>67.09446</v>
+        <v>73.2</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2514,7 +2494,7 @@
         <v>46079.875</v>
       </c>
       <c r="B92" t="n">
-        <v>73.2</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2535,7 +2515,7 @@
         <v>46079.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>65.01000000000001</v>
+        <v>66.10442</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2556,7 +2536,7 @@
         <v>46079.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>57.51108</v>
+        <v>64.92106</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2577,7 +2557,7 @@
         <v>46079.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>57.06</v>
+        <v>57.14733</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2598,7 +2578,7 @@
         <v>46079.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>56.98</v>
+        <v>57.06</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2619,7 +2599,7 @@
         <v>46079.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>56.98</v>
+        <v>57.06</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 202)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,79 +478,39 @@
         <v>46080</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>46080.20833333334</v>
+        <v>46080.66666666666</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
-        <v>18.9</v>
+        <v>60.48</v>
       </c>
       <c r="E2" t="n">
-        <v>549.8350455</v>
+        <v>1109.702724</v>
       </c>
       <c r="F2" t="n">
-        <v>29.09180134920635</v>
+        <v>18.34825932539682</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46080.3125</v>
+        <v>46081.29166666666</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46080.66666666666</v>
+        <v>46081.79166666666</v>
       </c>
       <c r="C3" t="n">
-        <v>8.5</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>32.13</v>
+        <v>45.36</v>
       </c>
       <c r="E3" t="n">
-        <v>232.95746175</v>
+        <v>300.791088</v>
       </c>
       <c r="F3" t="n">
-        <v>7.25046566293184</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>46080.89583333334</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>46081.0625</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>15.12</v>
-      </c>
-      <c r="E4" t="n">
-        <v>459.8416192499999</v>
-      </c>
-      <c r="F4" t="n">
-        <v>30.41280550595237</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>46081.3125</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>46081.75</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>39.69</v>
-      </c>
-      <c r="E5" t="n">
-        <v>254.03809275</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6.400556632653061</v>
+        <v>6.631196825396826</v>
       </c>
     </row>
   </sheetData>
@@ -826,7 +786,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -847,7 +807,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -868,7 +828,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -889,7 +849,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -910,7 +870,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1320,7 @@
         <v>46080.75</v>
       </c>
       <c r="B38" t="n">
-        <v>51.49362</v>
+        <v>50.46801</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,7 +1341,7 @@
         <v>46080.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>57.36</v>
+        <v>64.89</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1402,11 +1362,11 @@
         <v>46080.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>73.18418</v>
+        <v>75.34523</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1423,11 +1383,11 @@
         <v>46080.8125</v>
       </c>
       <c r="B41" t="n">
-        <v>73.19</v>
+        <v>72.90706</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
@@ -1444,11 +1404,11 @@
         <v>46080.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>78</v>
+        <v>74.22528</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
@@ -1465,11 +1425,11 @@
         <v>46080.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>73.19</v>
+        <v>78</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1486,11 +1446,11 @@
         <v>46080.875</v>
       </c>
       <c r="B44" t="n">
-        <v>63.64763</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1507,11 +1467,11 @@
         <v>46080.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>62.90238</v>
+        <v>65</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
@@ -1519,7 +1479,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1528,11 +1488,11 @@
         <v>46080.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>64.35039999999999</v>
+        <v>64.89</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
@@ -1540,7 +1500,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1549,11 +1509,11 @@
         <v>46080.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>60.7497</v>
+        <v>65</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
@@ -1561,7 +1521,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1570,11 +1530,11 @@
         <v>46080.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>57.06</v>
+        <v>64.10590000000001</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
@@ -1582,7 +1542,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1551,7 @@
         <v>46080.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>56.98</v>
+        <v>65</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1603,7 +1563,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1572,7 @@
         <v>46081</v>
       </c>
       <c r="B50" t="n">
-        <v>56.98</v>
+        <v>57.06</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1624,7 +1584,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1633,7 +1593,7 @@
         <v>46081.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>57.06</v>
+        <v>65</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1645,7 +1605,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1654,7 +1614,7 @@
         <v>46081.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>55.54995</v>
+        <v>57.06</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1666,7 +1626,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1635,7 @@
         <v>46081.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>56.98</v>
+        <v>57.06</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1696,7 +1656,7 @@
         <v>46081.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>37.9</v>
+        <v>56.98</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1717,7 +1677,7 @@
         <v>46081.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>37.89</v>
+        <v>56.15292</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1738,7 +1698,7 @@
         <v>46081.125</v>
       </c>
       <c r="B56" t="n">
-        <v>37.89</v>
+        <v>55.6532</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1759,7 +1719,7 @@
         <v>46081.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>37.89</v>
+        <v>54.99855</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1740,7 @@
         <v>46081.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>37.89</v>
+        <v>55.55142</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1801,7 +1761,7 @@
         <v>46081.1875</v>
       </c>
       <c r="B59" t="n">
-        <v>37.89</v>
+        <v>55.8507</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1822,7 +1782,7 @@
         <v>46081.20833333334</v>
       </c>
       <c r="B60" t="n">
-        <v>37.89</v>
+        <v>56.18178</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1843,7 +1803,7 @@
         <v>46081.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>57.06</v>
+        <v>57.31</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1824,7 @@
         <v>46081.25</v>
       </c>
       <c r="B62" t="n">
-        <v>60.68036</v>
+        <v>57.36</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1885,7 +1845,7 @@
         <v>46081.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>65.01000000000001</v>
+        <v>57.36</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1918,7 +1878,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1948,7 +1908,7 @@
         <v>46081.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>0.7789700000000001</v>
+        <v>1.17886</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1969,7 +1929,7 @@
         <v>46081.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>1.55269</v>
+        <v>2.8337</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1990,7 +1950,7 @@
         <v>46081.375</v>
       </c>
       <c r="B68" t="n">
-        <v>8.42309</v>
+        <v>1.53977</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2011,7 +1971,7 @@
         <v>46081.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>8.191240000000001</v>
+        <v>1.12995</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2032,7 +1992,7 @@
         <v>46081.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>1.51758</v>
+        <v>6.75606</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2013,7 @@
         <v>46081.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>1.528</v>
+        <v>1.50663</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2034,7 @@
         <v>46081.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>1.51752</v>
+        <v>0.7</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2055,7 @@
         <v>46081.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>1.53509</v>
+        <v>1.46401</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2076,7 @@
         <v>46081.5</v>
       </c>
       <c r="B74" t="n">
-        <v>1.49894</v>
+        <v>1.09962</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2097,7 @@
         <v>46081.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>7.95056</v>
+        <v>1.45297</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2118,7 @@
         <v>46081.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>7.95755</v>
+        <v>0.7</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2179,7 +2139,7 @@
         <v>46081.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>7.92085</v>
+        <v>0.7</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2200,7 +2160,7 @@
         <v>46081.58333333334</v>
       </c>
       <c r="B78" t="n">
-        <v>7.9397</v>
+        <v>0.7</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2221,7 +2181,7 @@
         <v>46081.60416666666</v>
       </c>
       <c r="B79" t="n">
-        <v>22.07</v>
+        <v>8.012169999999999</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2242,7 +2202,7 @@
         <v>46081.625</v>
       </c>
       <c r="B80" t="n">
-        <v>35.88</v>
+        <v>8.223660000000001</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2263,7 +2223,7 @@
         <v>46081.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>37.89</v>
+        <v>11.89595</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2284,7 +2244,7 @@
         <v>46081.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>0.51</v>
+        <v>-3.76</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2265,7 @@
         <v>46081.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>-3.75989</v>
+        <v>-4.14527</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2286,7 @@
         <v>46081.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>35.88</v>
+        <v>27.67105</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2368,7 +2328,7 @@
         <v>46081.75</v>
       </c>
       <c r="B86" t="n">
-        <v>50.84706</v>
+        <v>50.73455</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2380,7 +2340,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2389,7 +2349,7 @@
         <v>46081.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>59.14727</v>
+        <v>57.36</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2401,7 +2361,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2410,7 +2370,7 @@
         <v>46081.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>64.23829000000001</v>
+        <v>58.88215</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2431,7 +2391,7 @@
         <v>46081.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>61.25901</v>
+        <v>63.60493</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2412,7 @@
         <v>46081.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>63.88958</v>
+        <v>60.73634</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2433,7 @@
         <v>46081.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>57.36</v>
+        <v>58.92311</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2454,7 @@
         <v>46081.875</v>
       </c>
       <c r="B92" t="n">
-        <v>57.06006</v>
+        <v>57.36</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2515,7 +2475,7 @@
         <v>46081.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>57.06</v>
+        <v>57.36</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2536,7 +2496,7 @@
         <v>46081.91666666666</v>
       </c>
       <c r="B94" t="n">
-        <v>57.06</v>
+        <v>57.32</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2557,7 +2517,7 @@
         <v>46081.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>57.06</v>
+        <v>60.72274</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2599,7 +2559,7 @@
         <v>46081.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>56.98</v>
+        <v>57.06</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update latest output (run 206)
</commit_message>
<xml_diff>
--- a/data/latest/optimisation_result.xlsx
+++ b/data/latest/optimisation_result.xlsx
@@ -498,59 +498,59 @@
         <v>46082.29166666666</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>46082.75</v>
+        <v>46082.70833333334</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>41.58</v>
+        <v>37.8</v>
       </c>
       <c r="E3" t="n">
-        <v>445.45896525</v>
+        <v>345.5872875</v>
       </c>
       <c r="F3" t="n">
-        <v>10.71329882756133</v>
+        <v>9.142520833333334</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46082.97916666666</v>
+        <v>46082.9375</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>46083.27083333334</v>
+        <v>46083.25</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="D4" t="n">
-        <v>26.46</v>
+        <v>28.35</v>
       </c>
       <c r="E4" t="n">
-        <v>618.9538192499999</v>
+        <v>805.5930577500001</v>
       </c>
       <c r="F4" t="n">
-        <v>23.39205666099773</v>
+        <v>28.41598087301588</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46083.3125</v>
+        <v>46083.41666666666</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>46083.54166666666</v>
+        <v>46083.66666666666</v>
       </c>
       <c r="C5" t="n">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>20.79</v>
+        <v>22.68</v>
       </c>
       <c r="E5" t="n">
-        <v>630.0183630000001</v>
+        <v>717.2177415</v>
       </c>
       <c r="F5" t="n">
-        <v>30.30391356421357</v>
+        <v>31.62335720899471</v>
       </c>
     </row>
   </sheetData>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
         <v>46082.72916666666</v>
       </c>
       <c r="B37" t="n">
-        <v>48.96586</v>
+        <v>56.98</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
         <v>46082.75</v>
       </c>
       <c r="B38" t="n">
-        <v>56.98</v>
+        <v>57.31</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1381,11 +1381,11 @@
         <v>46082.77083333334</v>
       </c>
       <c r="B39" t="n">
-        <v>57.31</v>
+        <v>57.36</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D39" s="3" t="n">
@@ -1402,11 +1402,11 @@
         <v>46082.79166666666</v>
       </c>
       <c r="B40" t="n">
-        <v>58.01839</v>
+        <v>57.31</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D40" s="3" t="n">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D41" s="3" t="n">
@@ -1444,11 +1444,11 @@
         <v>46082.83333333334</v>
       </c>
       <c r="B42" t="n">
-        <v>57.59646</v>
+        <v>57.06013</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D42" s="3" t="n">
@@ -1465,11 +1465,11 @@
         <v>46082.85416666666</v>
       </c>
       <c r="B43" t="n">
-        <v>57.31</v>
+        <v>57.06</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D43" s="3" t="n">
@@ -1486,11 +1486,11 @@
         <v>46082.875</v>
       </c>
       <c r="B44" t="n">
-        <v>57.06014</v>
+        <v>52.30914</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D44" s="3" t="n">
@@ -1507,11 +1507,11 @@
         <v>46082.89583333334</v>
       </c>
       <c r="B45" t="n">
-        <v>57.06</v>
+        <v>51.50676</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D45" s="3" t="n">
@@ -1528,11 +1528,11 @@
         <v>46082.91666666666</v>
       </c>
       <c r="B46" t="n">
-        <v>56.98</v>
+        <v>50.03655</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D46" s="3" t="n">
@@ -1549,11 +1549,11 @@
         <v>46082.9375</v>
       </c>
       <c r="B47" t="n">
-        <v>51.02473</v>
+        <v>52.17509</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D47" s="3" t="n">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1570,11 +1570,11 @@
         <v>46082.95833333334</v>
       </c>
       <c r="B48" t="n">
-        <v>52.1907</v>
+        <v>50.53328</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>historical</t>
         </is>
       </c>
       <c r="D48" s="3" t="n">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
         <v>46082.97916666666</v>
       </c>
       <c r="B49" t="n">
-        <v>51.11919</v>
+        <v>52.13164</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         <v>46083</v>
       </c>
       <c r="B50" t="n">
-        <v>43.0326</v>
+        <v>51.50568</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         <v>46083.02083333334</v>
       </c>
       <c r="B51" t="n">
-        <v>37.89</v>
+        <v>56.98</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         <v>46083.04166666666</v>
       </c>
       <c r="B52" t="n">
-        <v>37.89</v>
+        <v>53.70908</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
         <v>46083.0625</v>
       </c>
       <c r="B53" t="n">
-        <v>37.89</v>
+        <v>56.98</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1696,7 +1696,7 @@
         <v>46083.08333333334</v>
       </c>
       <c r="B54" t="n">
-        <v>37.89</v>
+        <v>55.22264</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         <v>46083.10416666666</v>
       </c>
       <c r="B55" t="n">
-        <v>37.89</v>
+        <v>55.27768</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1738,7 +1738,7 @@
         <v>46083.125</v>
       </c>
       <c r="B56" t="n">
-        <v>37.89</v>
+        <v>55.30405</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1759,7 +1759,7 @@
         <v>46083.14583333334</v>
       </c>
       <c r="B57" t="n">
-        <v>37.89</v>
+        <v>55.64532</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1780,7 +1780,7 @@
         <v>46083.16666666666</v>
       </c>
       <c r="B58" t="n">
-        <v>41.37121</v>
+        <v>55.62514</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1843,7 +1843,7 @@
         <v>46083.22916666666</v>
       </c>
       <c r="B61" t="n">
-        <v>57.06</v>
+        <v>61.11969</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1864,7 +1864,7 @@
         <v>46083.25</v>
       </c>
       <c r="B62" t="n">
-        <v>62.97143</v>
+        <v>65</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1885,7 +1885,7 @@
         <v>46083.27083333334</v>
       </c>
       <c r="B63" t="n">
-        <v>65</v>
+        <v>82.91262</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>46083.29166666666</v>
       </c>
       <c r="B64" t="n">
-        <v>65</v>
+        <v>72.01016</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         <v>46083.3125</v>
       </c>
       <c r="B65" t="n">
-        <v>57.06</v>
+        <v>65</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
         <v>46083.33333333334</v>
       </c>
       <c r="B66" t="n">
-        <v>57.06</v>
+        <v>65</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
         <v>46083.35416666666</v>
       </c>
       <c r="B67" t="n">
-        <v>57.06</v>
+        <v>65</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
         <v>46083.375</v>
       </c>
       <c r="B68" t="n">
-        <v>57.06</v>
+        <v>62.19162</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -2011,7 +2011,7 @@
         <v>46083.39583333334</v>
       </c>
       <c r="B69" t="n">
-        <v>65.01000000000001</v>
+        <v>65.01009999999999</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>ON</t>
+          <t>OFF</t>
         </is>
       </c>
     </row>
@@ -2032,7 +2032,7 @@
         <v>46083.41666666666</v>
       </c>
       <c r="B70" t="n">
-        <v>57.06016</v>
+        <v>64.33967</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
         <v>46083.4375</v>
       </c>
       <c r="B71" t="n">
-        <v>57.06</v>
+        <v>63.1496</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2074,7 +2074,7 @@
         <v>46083.45833333334</v>
       </c>
       <c r="B72" t="n">
-        <v>63.80252</v>
+        <v>76.99009</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2095,7 +2095,7 @@
         <v>46083.47916666666</v>
       </c>
       <c r="B73" t="n">
-        <v>60.88</v>
+        <v>65.01014000000001</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2116,7 +2116,7 @@
         <v>46083.5</v>
       </c>
       <c r="B74" t="n">
-        <v>57.06</v>
+        <v>57.06015</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         <v>46083.52083333334</v>
       </c>
       <c r="B75" t="n">
-        <v>57.06</v>
+        <v>57.06044</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2158,7 +2158,7 @@
         <v>46083.54166666666</v>
       </c>
       <c r="B76" t="n">
-        <v>65.01012</v>
+        <v>61.40941</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2179,7 +2179,7 @@
         <v>46083.5625</v>
       </c>
       <c r="B77" t="n">
-        <v>65.01011</v>
+        <v>62.45104</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2242,7 +2242,7 @@
         <v>46083.625</v>
       </c>
       <c r="B80" t="n">
-        <v>57.06</v>
+        <v>57.0602</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
         <v>46083.64583333334</v>
       </c>
       <c r="B81" t="n">
-        <v>56.98</v>
+        <v>57.1172</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>OFF</t>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -2284,7 +2284,7 @@
         <v>46083.66666666666</v>
       </c>
       <c r="B82" t="n">
-        <v>61.20485</v>
+        <v>64.89</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         <v>46083.6875</v>
       </c>
       <c r="B83" t="n">
-        <v>64.89</v>
+        <v>66.67514</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
         <v>46083.70833333334</v>
       </c>
       <c r="B84" t="n">
-        <v>67.0836</v>
+        <v>78</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>46083.72916666666</v>
       </c>
       <c r="B85" t="n">
-        <v>84.79000000000001</v>
+        <v>81.02665</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2368,7 +2368,7 @@
         <v>46083.75</v>
       </c>
       <c r="B86" t="n">
-        <v>75.56201</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2389,7 +2389,7 @@
         <v>46083.77083333334</v>
       </c>
       <c r="B87" t="n">
-        <v>88.384</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2410,7 +2410,7 @@
         <v>46083.79166666666</v>
       </c>
       <c r="B88" t="n">
-        <v>87.88893</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2431,7 +2431,7 @@
         <v>46083.8125</v>
       </c>
       <c r="B89" t="n">
-        <v>84.79000000000001</v>
+        <v>82.35193</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         <v>46083.83333333334</v>
       </c>
       <c r="B90" t="n">
-        <v>83.77110999999999</v>
+        <v>83.64431</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2473,7 +2473,7 @@
         <v>46083.85416666666</v>
       </c>
       <c r="B91" t="n">
-        <v>80.39408</v>
+        <v>79.98466000000001</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2494,7 +2494,7 @@
         <v>46083.875</v>
       </c>
       <c r="B92" t="n">
-        <v>79.18258</v>
+        <v>79.28679</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
         <v>46083.89583333334</v>
       </c>
       <c r="B93" t="n">
-        <v>70.63603999999999</v>
+        <v>78</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         <v>46083.9375</v>
       </c>
       <c r="B95" t="n">
-        <v>65.17373000000001</v>
+        <v>58.97834</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2578,7 +2578,7 @@
         <v>46083.95833333334</v>
       </c>
       <c r="B96" t="n">
-        <v>61.14933</v>
+        <v>59.25448</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
         <v>46083.97916666666</v>
       </c>
       <c r="B97" t="n">
-        <v>62.51832</v>
+        <v>57.31</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>

</xml_diff>